<commit_message>
update uk to 2023q4
</commit_message>
<xml_diff>
--- a/data-raw/uk/epu.xlsx
+++ b/data-raw/uk/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="31">
   <si>
     <t>year</t>
   </si>
@@ -96,6 +96,9 @@
     <t>2023</t>
   </si>
   <si>
+    <t>2024</t>
+  </si>
+  <si>
     <t>Source: 'Measuring Economic Policy Uncertainty' by Scott Baker, Nicholas Bloom and Steven J. Davis at www.PolicyUncertainty.com.  These data can be used freely with attribution to the authors, the paper, and the website.</t>
   </si>
   <si>
@@ -123,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -131,14 +134,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C314"/>
+  <dimension ref="A1:C317"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -156,20 +157,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0">
         <v>114.23303041919498</v>
       </c>
     </row>
@@ -177,10 +178,10 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="0">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0">
         <v>71.152468112217733</v>
       </c>
     </row>
@@ -188,10 +189,10 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="0">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0">
         <v>148.08653465656573</v>
       </c>
     </row>
@@ -199,10 +200,10 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="0">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0">
         <v>146.97678918911495</v>
       </c>
     </row>
@@ -210,10 +211,10 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="0">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0">
         <v>111.51501101796822</v>
       </c>
     </row>
@@ -221,10 +222,10 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="0">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0">
         <v>85.492917317480106</v>
       </c>
     </row>
@@ -232,10 +233,10 @@
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B8" s="0">
+        <v>7</v>
+      </c>
+      <c r="C8" s="0">
         <v>180.79302078297567</v>
       </c>
     </row>
@@ -243,10 +244,10 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9" s="0">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0">
         <v>140.59883854349383</v>
       </c>
     </row>
@@ -254,10 +255,10 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="B10" s="0">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0">
         <v>193.86284404128827</v>
       </c>
     </row>
@@ -265,10 +266,10 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B11" s="0">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0">
         <v>256.06809124079552</v>
       </c>
     </row>
@@ -276,10 +277,10 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B12" s="0">
+        <v>11</v>
+      </c>
+      <c r="C12" s="0">
         <v>172.85871532726372</v>
       </c>
     </row>
@@ -287,10 +288,10 @@
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B13" s="0">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0">
         <v>123.54462447386712</v>
       </c>
     </row>
@@ -298,10 +299,10 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B14" s="0">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0">
         <v>99.624838290417301</v>
       </c>
     </row>
@@ -309,10 +310,10 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B15" s="0">
+        <v>2</v>
+      </c>
+      <c r="C15" s="0">
         <v>89.301390805313901</v>
       </c>
     </row>
@@ -320,10 +321,10 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="1">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="B16" s="0">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0">
         <v>84.704431375507454</v>
       </c>
     </row>
@@ -331,10 +332,10 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B17" s="0">
+        <v>4</v>
+      </c>
+      <c r="C17" s="0">
         <v>63.930248201578557</v>
       </c>
     </row>
@@ -342,10 +343,10 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="1">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B18" s="0">
+        <v>5</v>
+      </c>
+      <c r="C18" s="0">
         <v>71.887983294516644</v>
       </c>
     </row>
@@ -353,10 +354,10 @@
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="B19" s="0">
+        <v>6</v>
+      </c>
+      <c r="C19" s="0">
         <v>52.256729242724006</v>
       </c>
     </row>
@@ -364,10 +365,10 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="1">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="B20" s="0">
+        <v>7</v>
+      </c>
+      <c r="C20" s="0">
         <v>81.232297333847839</v>
       </c>
     </row>
@@ -375,10 +376,10 @@
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="1">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="B21" s="0">
+        <v>8</v>
+      </c>
+      <c r="C21" s="0">
         <v>72.576704428693134</v>
       </c>
     </row>
@@ -386,10 +387,10 @@
       <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="B22" s="0">
+        <v>9</v>
+      </c>
+      <c r="C22" s="0">
         <v>67.127564501344565</v>
       </c>
     </row>
@@ -397,10 +398,10 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="1">
-        <v>10</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="B23" s="0">
+        <v>10</v>
+      </c>
+      <c r="C23" s="0">
         <v>123.12413166974538</v>
       </c>
     </row>
@@ -408,10 +409,10 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="1">
-        <v>11</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="B24" s="0">
+        <v>11</v>
+      </c>
+      <c r="C24" s="0">
         <v>26.84680026099262</v>
       </c>
     </row>
@@ -419,10 +420,10 @@
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="1">
-        <v>12</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="B25" s="0">
+        <v>12</v>
+      </c>
+      <c r="C25" s="0">
         <v>48.689985458213094</v>
       </c>
     </row>
@@ -430,10 +431,10 @@
       <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1">
+      <c r="B26" s="0">
+        <v>1</v>
+      </c>
+      <c r="C26" s="0">
         <v>53.748451022419943</v>
       </c>
     </row>
@@ -441,10 +442,10 @@
       <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="1">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1">
+      <c r="B27" s="0">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0">
         <v>58.396510954430312</v>
       </c>
     </row>
@@ -452,10 +453,10 @@
       <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="1">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="B28" s="0">
+        <v>3</v>
+      </c>
+      <c r="C28" s="0">
         <v>61.960392681100373</v>
       </c>
     </row>
@@ -463,10 +464,10 @@
       <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="1">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1">
+      <c r="B29" s="0">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0">
         <v>114.01042927352911</v>
       </c>
     </row>
@@ -474,10 +475,10 @@
       <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="1">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="B30" s="0">
+        <v>5</v>
+      </c>
+      <c r="C30" s="0">
         <v>46.368325435466247</v>
       </c>
     </row>
@@ -485,10 +486,10 @@
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="1">
-        <v>6</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="B31" s="0">
+        <v>6</v>
+      </c>
+      <c r="C31" s="0">
         <v>133.21640062369883</v>
       </c>
     </row>
@@ -496,10 +497,10 @@
       <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="1">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="B32" s="0">
+        <v>7</v>
+      </c>
+      <c r="C32" s="0">
         <v>73.706699857582223</v>
       </c>
     </row>
@@ -507,10 +508,10 @@
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="1">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="B33" s="0">
+        <v>8</v>
+      </c>
+      <c r="C33" s="0">
         <v>42.748375788974677</v>
       </c>
     </row>
@@ -518,10 +519,10 @@
       <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="1">
-        <v>9</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="B34" s="0">
+        <v>9</v>
+      </c>
+      <c r="C34" s="0">
         <v>55.577872298404039</v>
       </c>
     </row>
@@ -529,10 +530,10 @@
       <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="1">
-        <v>10</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="B35" s="0">
+        <v>10</v>
+      </c>
+      <c r="C35" s="0">
         <v>55.821764612416644</v>
       </c>
     </row>
@@ -540,10 +541,10 @@
       <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="1">
-        <v>11</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="B36" s="0">
+        <v>11</v>
+      </c>
+      <c r="C36" s="0">
         <v>68.991031741151005</v>
       </c>
     </row>
@@ -551,10 +552,10 @@
       <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="1">
-        <v>12</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="B37" s="0">
+        <v>12</v>
+      </c>
+      <c r="C37" s="0">
         <v>66.450174706116044</v>
       </c>
     </row>
@@ -562,10 +563,10 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1">
+      <c r="B38" s="0">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0">
         <v>38.407833958642684</v>
       </c>
     </row>
@@ -573,10 +574,10 @@
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="1">
-        <v>2</v>
-      </c>
-      <c r="C39" s="1">
+      <c r="B39" s="0">
+        <v>2</v>
+      </c>
+      <c r="C39" s="0">
         <v>56.693271350649312</v>
       </c>
     </row>
@@ -584,10 +585,10 @@
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="1">
-        <v>3</v>
-      </c>
-      <c r="C40" s="1">
+      <c r="B40" s="0">
+        <v>3</v>
+      </c>
+      <c r="C40" s="0">
         <v>91.642864752455026</v>
       </c>
     </row>
@@ -595,10 +596,10 @@
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="1">
-        <v>4</v>
-      </c>
-      <c r="C41" s="1">
+      <c r="B41" s="0">
+        <v>4</v>
+      </c>
+      <c r="C41" s="0">
         <v>100.98927389864957</v>
       </c>
     </row>
@@ -606,10 +607,10 @@
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="1">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1">
+      <c r="B42" s="0">
+        <v>5</v>
+      </c>
+      <c r="C42" s="0">
         <v>98.256230864099578</v>
       </c>
     </row>
@@ -617,10 +618,10 @@
       <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="1">
-        <v>6</v>
-      </c>
-      <c r="C43" s="1">
+      <c r="B43" s="0">
+        <v>6</v>
+      </c>
+      <c r="C43" s="0">
         <v>74.842735742282386</v>
       </c>
     </row>
@@ -628,10 +629,10 @@
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1">
-        <v>7</v>
-      </c>
-      <c r="C44" s="1">
+      <c r="B44" s="0">
+        <v>7</v>
+      </c>
+      <c r="C44" s="0">
         <v>66.38372519061484</v>
       </c>
     </row>
@@ -639,10 +640,10 @@
       <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="1">
-        <v>8</v>
-      </c>
-      <c r="C45" s="1">
+      <c r="B45" s="0">
+        <v>8</v>
+      </c>
+      <c r="C45" s="0">
         <v>105.13269947080015</v>
       </c>
     </row>
@@ -650,10 +651,10 @@
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="1">
-        <v>9</v>
-      </c>
-      <c r="C46" s="1">
+      <c r="B46" s="0">
+        <v>9</v>
+      </c>
+      <c r="C46" s="0">
         <v>205.25697487631768</v>
       </c>
     </row>
@@ -661,10 +662,10 @@
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="1">
-        <v>10</v>
-      </c>
-      <c r="C47" s="1">
+      <c r="B47" s="0">
+        <v>10</v>
+      </c>
+      <c r="C47" s="0">
         <v>158.72159980318426</v>
       </c>
     </row>
@@ -672,10 +673,10 @@
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="1">
-        <v>11</v>
-      </c>
-      <c r="C48" s="1">
+      <c r="B48" s="0">
+        <v>11</v>
+      </c>
+      <c r="C48" s="0">
         <v>146.11531254475</v>
       </c>
     </row>
@@ -683,10 +684,10 @@
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="1">
-        <v>12</v>
-      </c>
-      <c r="C49" s="1">
+      <c r="B49" s="0">
+        <v>12</v>
+      </c>
+      <c r="C49" s="0">
         <v>108.11412471348061</v>
       </c>
     </row>
@@ -694,10 +695,10 @@
       <c r="A50" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1">
+      <c r="B50" s="0">
+        <v>1</v>
+      </c>
+      <c r="C50" s="0">
         <v>85.506579174754521</v>
       </c>
     </row>
@@ -705,10 +706,10 @@
       <c r="A51" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="1">
-        <v>2</v>
-      </c>
-      <c r="C51" s="1">
+      <c r="B51" s="0">
+        <v>2</v>
+      </c>
+      <c r="C51" s="0">
         <v>70.793482785977702</v>
       </c>
     </row>
@@ -716,10 +717,10 @@
       <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="1">
-        <v>3</v>
-      </c>
-      <c r="C52" s="1">
+      <c r="B52" s="0">
+        <v>3</v>
+      </c>
+      <c r="C52" s="0">
         <v>76.328319642242249</v>
       </c>
     </row>
@@ -727,10 +728,10 @@
       <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="1">
-        <v>4</v>
-      </c>
-      <c r="C53" s="1">
+      <c r="B53" s="0">
+        <v>4</v>
+      </c>
+      <c r="C53" s="0">
         <v>78.088182950900872</v>
       </c>
     </row>
@@ -738,10 +739,10 @@
       <c r="A54" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="1">
-        <v>5</v>
-      </c>
-      <c r="C54" s="1">
+      <c r="B54" s="0">
+        <v>5</v>
+      </c>
+      <c r="C54" s="0">
         <v>67.406353692455028</v>
       </c>
     </row>
@@ -749,10 +750,10 @@
       <c r="A55" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="1">
-        <v>6</v>
-      </c>
-      <c r="C55" s="1">
+      <c r="B55" s="0">
+        <v>6</v>
+      </c>
+      <c r="C55" s="0">
         <v>86.879203610639379</v>
       </c>
     </row>
@@ -760,10 +761,10 @@
       <c r="A56" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="1">
-        <v>7</v>
-      </c>
-      <c r="C56" s="1">
+      <c r="B56" s="0">
+        <v>7</v>
+      </c>
+      <c r="C56" s="0">
         <v>88.472571429943144</v>
       </c>
     </row>
@@ -771,10 +772,10 @@
       <c r="A57" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="1">
-        <v>8</v>
-      </c>
-      <c r="C57" s="1">
+      <c r="B57" s="0">
+        <v>8</v>
+      </c>
+      <c r="C57" s="0">
         <v>93.723994884644043</v>
       </c>
     </row>
@@ -782,10 +783,10 @@
       <c r="A58" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="1">
-        <v>9</v>
-      </c>
-      <c r="C58" s="1">
+      <c r="B58" s="0">
+        <v>9</v>
+      </c>
+      <c r="C58" s="0">
         <v>127.27273057482194</v>
       </c>
     </row>
@@ -793,10 +794,10 @@
       <c r="A59" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="1">
-        <v>10</v>
-      </c>
-      <c r="C59" s="1">
+      <c r="B59" s="0">
+        <v>10</v>
+      </c>
+      <c r="C59" s="0">
         <v>108.4297542573948</v>
       </c>
     </row>
@@ -804,10 +805,10 @@
       <c r="A60" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="1">
-        <v>11</v>
-      </c>
-      <c r="C60" s="1">
+      <c r="B60" s="0">
+        <v>11</v>
+      </c>
+      <c r="C60" s="0">
         <v>115.09958348207847</v>
       </c>
     </row>
@@ -815,10 +816,10 @@
       <c r="A61" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="1">
-        <v>12</v>
-      </c>
-      <c r="C61" s="1">
+      <c r="B61" s="0">
+        <v>12</v>
+      </c>
+      <c r="C61" s="0">
         <v>118.64259248874143</v>
       </c>
     </row>
@@ -826,10 +827,10 @@
       <c r="A62" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="1">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1">
+      <c r="B62" s="0">
+        <v>1</v>
+      </c>
+      <c r="C62" s="0">
         <v>146.05941292203249</v>
       </c>
     </row>
@@ -837,10 +838,10 @@
       <c r="A63" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="1">
-        <v>2</v>
-      </c>
-      <c r="C63" s="1">
+      <c r="B63" s="0">
+        <v>2</v>
+      </c>
+      <c r="C63" s="0">
         <v>178.73887349178023</v>
       </c>
     </row>
@@ -848,10 +849,10 @@
       <c r="A64" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="1">
-        <v>3</v>
-      </c>
-      <c r="C64" s="1">
+      <c r="B64" s="0">
+        <v>3</v>
+      </c>
+      <c r="C64" s="0">
         <v>174.97273471435085</v>
       </c>
     </row>
@@ -859,10 +860,10 @@
       <c r="A65" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="1">
-        <v>4</v>
-      </c>
-      <c r="C65" s="1">
+      <c r="B65" s="0">
+        <v>4</v>
+      </c>
+      <c r="C65" s="0">
         <v>153.50644782837878</v>
       </c>
     </row>
@@ -870,10 +871,10 @@
       <c r="A66" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="1">
-        <v>5</v>
-      </c>
-      <c r="C66" s="1">
+      <c r="B66" s="0">
+        <v>5</v>
+      </c>
+      <c r="C66" s="0">
         <v>93.713759198405427</v>
       </c>
     </row>
@@ -881,10 +882,10 @@
       <c r="A67" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="1">
-        <v>6</v>
-      </c>
-      <c r="C67" s="1">
+      <c r="B67" s="0">
+        <v>6</v>
+      </c>
+      <c r="C67" s="0">
         <v>125.00647484433625</v>
       </c>
     </row>
@@ -892,10 +893,10 @@
       <c r="A68" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="1">
-        <v>7</v>
-      </c>
-      <c r="C68" s="1">
+      <c r="B68" s="0">
+        <v>7</v>
+      </c>
+      <c r="C68" s="0">
         <v>80.936638413478462</v>
       </c>
     </row>
@@ -903,10 +904,10 @@
       <c r="A69" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="1">
-        <v>8</v>
-      </c>
-      <c r="C69" s="1">
+      <c r="B69" s="0">
+        <v>8</v>
+      </c>
+      <c r="C69" s="0">
         <v>83.362627004704052</v>
       </c>
     </row>
@@ -914,10 +915,10 @@
       <c r="A70" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="1">
-        <v>9</v>
-      </c>
-      <c r="C70" s="1">
+      <c r="B70" s="0">
+        <v>9</v>
+      </c>
+      <c r="C70" s="0">
         <v>65.412854559766302</v>
       </c>
     </row>
@@ -925,10 +926,10 @@
       <c r="A71" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="1">
-        <v>10</v>
-      </c>
-      <c r="C71" s="1">
+      <c r="B71" s="0">
+        <v>10</v>
+      </c>
+      <c r="C71" s="0">
         <v>62.298289449657176</v>
       </c>
     </row>
@@ -936,10 +937,10 @@
       <c r="A72" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="1">
-        <v>11</v>
-      </c>
-      <c r="C72" s="1">
+      <c r="B72" s="0">
+        <v>11</v>
+      </c>
+      <c r="C72" s="0">
         <v>78.4478801122807</v>
       </c>
     </row>
@@ -947,10 +948,10 @@
       <c r="A73" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="1">
-        <v>12</v>
-      </c>
-      <c r="C73" s="1">
+      <c r="B73" s="0">
+        <v>12</v>
+      </c>
+      <c r="C73" s="0">
         <v>46.291193655705612</v>
       </c>
     </row>
@@ -958,10 +959,10 @@
       <c r="A74" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="1">
-        <v>1</v>
-      </c>
-      <c r="C74" s="1">
+      <c r="B74" s="0">
+        <v>1</v>
+      </c>
+      <c r="C74" s="0">
         <v>24.0359419445406</v>
       </c>
     </row>
@@ -969,10 +970,10 @@
       <c r="A75" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="1">
-        <v>2</v>
-      </c>
-      <c r="C75" s="1">
+      <c r="B75" s="0">
+        <v>2</v>
+      </c>
+      <c r="C75" s="0">
         <v>57.130154355236499</v>
       </c>
     </row>
@@ -980,10 +981,10 @@
       <c r="A76" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="1">
-        <v>3</v>
-      </c>
-      <c r="C76" s="1">
+      <c r="B76" s="0">
+        <v>3</v>
+      </c>
+      <c r="C76" s="0">
         <v>61.884703940211296</v>
       </c>
     </row>
@@ -991,10 +992,10 @@
       <c r="A77" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="1">
-        <v>4</v>
-      </c>
-      <c r="C77" s="1">
+      <c r="B77" s="0">
+        <v>4</v>
+      </c>
+      <c r="C77" s="0">
         <v>38.552354422083354</v>
       </c>
     </row>
@@ -1002,10 +1003,10 @@
       <c r="A78" t="s">
         <v>7</v>
       </c>
-      <c r="B78" s="1">
-        <v>5</v>
-      </c>
-      <c r="C78" s="1">
+      <c r="B78" s="0">
+        <v>5</v>
+      </c>
+      <c r="C78" s="0">
         <v>42.88216533306619</v>
       </c>
     </row>
@@ -1013,10 +1014,10 @@
       <c r="A79" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="1">
-        <v>6</v>
-      </c>
-      <c r="C79" s="1">
+      <c r="B79" s="0">
+        <v>6</v>
+      </c>
+      <c r="C79" s="0">
         <v>49.439137156664231</v>
       </c>
     </row>
@@ -1024,10 +1025,10 @@
       <c r="A80" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="1">
-        <v>7</v>
-      </c>
-      <c r="C80" s="1">
+      <c r="B80" s="0">
+        <v>7</v>
+      </c>
+      <c r="C80" s="0">
         <v>52.617274390594723</v>
       </c>
     </row>
@@ -1035,10 +1036,10 @@
       <c r="A81" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="1">
-        <v>8</v>
-      </c>
-      <c r="C81" s="1">
+      <c r="B81" s="0">
+        <v>8</v>
+      </c>
+      <c r="C81" s="0">
         <v>39.393721041190858</v>
       </c>
     </row>
@@ -1046,10 +1047,10 @@
       <c r="A82" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="1">
-        <v>9</v>
-      </c>
-      <c r="C82" s="1">
+      <c r="B82" s="0">
+        <v>9</v>
+      </c>
+      <c r="C82" s="0">
         <v>49.166223902677764</v>
       </c>
     </row>
@@ -1057,10 +1058,10 @@
       <c r="A83" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="1">
-        <v>10</v>
-      </c>
-      <c r="C83" s="1">
+      <c r="B83" s="0">
+        <v>10</v>
+      </c>
+      <c r="C83" s="0">
         <v>67.129160866436038</v>
       </c>
     </row>
@@ -1068,10 +1069,10 @@
       <c r="A84" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="1">
-        <v>11</v>
-      </c>
-      <c r="C84" s="1">
+      <c r="B84" s="0">
+        <v>11</v>
+      </c>
+      <c r="C84" s="0">
         <v>68.726025959774617</v>
       </c>
     </row>
@@ -1079,10 +1080,10 @@
       <c r="A85" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="1">
-        <v>12</v>
-      </c>
-      <c r="C85" s="1">
+      <c r="B85" s="0">
+        <v>12</v>
+      </c>
+      <c r="C85" s="0">
         <v>44.909516282941226</v>
       </c>
     </row>
@@ -1090,10 +1091,10 @@
       <c r="A86" t="s">
         <v>8</v>
       </c>
-      <c r="B86" s="1">
-        <v>1</v>
-      </c>
-      <c r="C86" s="1">
+      <c r="B86" s="0">
+        <v>1</v>
+      </c>
+      <c r="C86" s="0">
         <v>43.989646993249359</v>
       </c>
     </row>
@@ -1101,10 +1102,10 @@
       <c r="A87" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="1">
-        <v>2</v>
-      </c>
-      <c r="C87" s="1">
+      <c r="B87" s="0">
+        <v>2</v>
+      </c>
+      <c r="C87" s="0">
         <v>39.64534947881436</v>
       </c>
     </row>
@@ -1112,10 +1113,10 @@
       <c r="A88" t="s">
         <v>8</v>
       </c>
-      <c r="B88" s="1">
-        <v>3</v>
-      </c>
-      <c r="C88" s="1">
+      <c r="B88" s="0">
+        <v>3</v>
+      </c>
+      <c r="C88" s="0">
         <v>34.07870982308976</v>
       </c>
     </row>
@@ -1123,10 +1124,10 @@
       <c r="A89" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="1">
-        <v>4</v>
-      </c>
-      <c r="C89" s="1">
+      <c r="B89" s="0">
+        <v>4</v>
+      </c>
+      <c r="C89" s="0">
         <v>69.057126421663469</v>
       </c>
     </row>
@@ -1134,10 +1135,10 @@
       <c r="A90" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="1">
-        <v>5</v>
-      </c>
-      <c r="C90" s="1">
+      <c r="B90" s="0">
+        <v>5</v>
+      </c>
+      <c r="C90" s="0">
         <v>71.771089573397958</v>
       </c>
     </row>
@@ -1145,10 +1146,10 @@
       <c r="A91" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="1">
-        <v>6</v>
-      </c>
-      <c r="C91" s="1">
+      <c r="B91" s="0">
+        <v>6</v>
+      </c>
+      <c r="C91" s="0">
         <v>59.403874719354278</v>
       </c>
     </row>
@@ -1156,10 +1157,10 @@
       <c r="A92" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="1">
-        <v>7</v>
-      </c>
-      <c r="C92" s="1">
+      <c r="B92" s="0">
+        <v>7</v>
+      </c>
+      <c r="C92" s="0">
         <v>47.414013411934278</v>
       </c>
     </row>
@@ -1167,10 +1168,10 @@
       <c r="A93" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="1">
-        <v>8</v>
-      </c>
-      <c r="C93" s="1">
+      <c r="B93" s="0">
+        <v>8</v>
+      </c>
+      <c r="C93" s="0">
         <v>48.54170562625211</v>
       </c>
     </row>
@@ -1178,10 +1179,10 @@
       <c r="A94" t="s">
         <v>8</v>
       </c>
-      <c r="B94" s="1">
-        <v>9</v>
-      </c>
-      <c r="C94" s="1">
+      <c r="B94" s="0">
+        <v>9</v>
+      </c>
+      <c r="C94" s="0">
         <v>70.332476662916861</v>
       </c>
     </row>
@@ -1189,10 +1190,10 @@
       <c r="A95" t="s">
         <v>8</v>
       </c>
-      <c r="B95" s="1">
-        <v>10</v>
-      </c>
-      <c r="C95" s="1">
+      <c r="B95" s="0">
+        <v>10</v>
+      </c>
+      <c r="C95" s="0">
         <v>40.613034313794714</v>
       </c>
     </row>
@@ -1200,10 +1201,10 @@
       <c r="A96" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="1">
-        <v>11</v>
-      </c>
-      <c r="C96" s="1">
+      <c r="B96" s="0">
+        <v>11</v>
+      </c>
+      <c r="C96" s="0">
         <v>47.559237062280005</v>
       </c>
     </row>
@@ -1211,10 +1212,10 @@
       <c r="A97" t="s">
         <v>8</v>
       </c>
-      <c r="B97" s="1">
-        <v>12</v>
-      </c>
-      <c r="C97" s="1">
+      <c r="B97" s="0">
+        <v>12</v>
+      </c>
+      <c r="C97" s="0">
         <v>33.10658195369718</v>
       </c>
     </row>
@@ -1222,10 +1223,10 @@
       <c r="A98" t="s">
         <v>9</v>
       </c>
-      <c r="B98" s="1">
-        <v>1</v>
-      </c>
-      <c r="C98" s="1">
+      <c r="B98" s="0">
+        <v>1</v>
+      </c>
+      <c r="C98" s="0">
         <v>44.040050065155981</v>
       </c>
     </row>
@@ -1233,10 +1234,10 @@
       <c r="A99" t="s">
         <v>9</v>
       </c>
-      <c r="B99" s="1">
-        <v>2</v>
-      </c>
-      <c r="C99" s="1">
+      <c r="B99" s="0">
+        <v>2</v>
+      </c>
+      <c r="C99" s="0">
         <v>37.132061545598454</v>
       </c>
     </row>
@@ -1244,10 +1245,10 @@
       <c r="A100" t="s">
         <v>9</v>
       </c>
-      <c r="B100" s="1">
-        <v>3</v>
-      </c>
-      <c r="C100" s="1">
+      <c r="B100" s="0">
+        <v>3</v>
+      </c>
+      <c r="C100" s="0">
         <v>42.456446706105879</v>
       </c>
     </row>
@@ -1255,10 +1256,10 @@
       <c r="A101" t="s">
         <v>9</v>
       </c>
-      <c r="B101" s="1">
-        <v>4</v>
-      </c>
-      <c r="C101" s="1">
+      <c r="B101" s="0">
+        <v>4</v>
+      </c>
+      <c r="C101" s="0">
         <v>37.086608110653827</v>
       </c>
     </row>
@@ -1266,10 +1267,10 @@
       <c r="A102" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="1">
-        <v>5</v>
-      </c>
-      <c r="C102" s="1">
+      <c r="B102" s="0">
+        <v>5</v>
+      </c>
+      <c r="C102" s="0">
         <v>74.022673592114302</v>
       </c>
     </row>
@@ -1277,10 +1278,10 @@
       <c r="A103" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="1">
-        <v>6</v>
-      </c>
-      <c r="C103" s="1">
+      <c r="B103" s="0">
+        <v>6</v>
+      </c>
+      <c r="C103" s="0">
         <v>59.820568976535263</v>
       </c>
     </row>
@@ -1288,10 +1289,10 @@
       <c r="A104" t="s">
         <v>9</v>
       </c>
-      <c r="B104" s="1">
-        <v>7</v>
-      </c>
-      <c r="C104" s="1">
+      <c r="B104" s="0">
+        <v>7</v>
+      </c>
+      <c r="C104" s="0">
         <v>47.543782394855668</v>
       </c>
     </row>
@@ -1299,10 +1300,10 @@
       <c r="A105" t="s">
         <v>9</v>
       </c>
-      <c r="B105" s="1">
-        <v>8</v>
-      </c>
-      <c r="C105" s="1">
+      <c r="B105" s="0">
+        <v>8</v>
+      </c>
+      <c r="C105" s="0">
         <v>67.213228709248042</v>
       </c>
     </row>
@@ -1310,10 +1311,10 @@
       <c r="A106" t="s">
         <v>9</v>
       </c>
-      <c r="B106" s="1">
-        <v>9</v>
-      </c>
-      <c r="C106" s="1">
+      <c r="B106" s="0">
+        <v>9</v>
+      </c>
+      <c r="C106" s="0">
         <v>56.234482774648797</v>
       </c>
     </row>
@@ -1321,10 +1322,10 @@
       <c r="A107" t="s">
         <v>9</v>
       </c>
-      <c r="B107" s="1">
-        <v>10</v>
-      </c>
-      <c r="C107" s="1">
+      <c r="B107" s="0">
+        <v>10</v>
+      </c>
+      <c r="C107" s="0">
         <v>65.255080007947058</v>
       </c>
     </row>
@@ -1332,10 +1333,10 @@
       <c r="A108" t="s">
         <v>9</v>
       </c>
-      <c r="B108" s="1">
-        <v>11</v>
-      </c>
-      <c r="C108" s="1">
+      <c r="B108" s="0">
+        <v>11</v>
+      </c>
+      <c r="C108" s="0">
         <v>59.49058917096486</v>
       </c>
     </row>
@@ -1343,10 +1344,10 @@
       <c r="A109" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="1">
-        <v>12</v>
-      </c>
-      <c r="C109" s="1">
+      <c r="B109" s="0">
+        <v>12</v>
+      </c>
+      <c r="C109" s="0">
         <v>64.488699636232127</v>
       </c>
     </row>
@@ -1354,10 +1355,10 @@
       <c r="A110" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="1">
-        <v>1</v>
-      </c>
-      <c r="C110" s="1">
+      <c r="B110" s="0">
+        <v>1</v>
+      </c>
+      <c r="C110" s="0">
         <v>49.232184122049397</v>
       </c>
     </row>
@@ -1365,10 +1366,10 @@
       <c r="A111" t="s">
         <v>10</v>
       </c>
-      <c r="B111" s="1">
-        <v>2</v>
-      </c>
-      <c r="C111" s="1">
+      <c r="B111" s="0">
+        <v>2</v>
+      </c>
+      <c r="C111" s="0">
         <v>53.071933804627889</v>
       </c>
     </row>
@@ -1376,10 +1377,10 @@
       <c r="A112" t="s">
         <v>10</v>
       </c>
-      <c r="B112" s="1">
-        <v>3</v>
-      </c>
-      <c r="C112" s="1">
+      <c r="B112" s="0">
+        <v>3</v>
+      </c>
+      <c r="C112" s="0">
         <v>77.055227733903877</v>
       </c>
     </row>
@@ -1387,10 +1388,10 @@
       <c r="A113" t="s">
         <v>10</v>
       </c>
-      <c r="B113" s="1">
-        <v>4</v>
-      </c>
-      <c r="C113" s="1">
+      <c r="B113" s="0">
+        <v>4</v>
+      </c>
+      <c r="C113" s="0">
         <v>60.964843473864342</v>
       </c>
     </row>
@@ -1398,10 +1399,10 @@
       <c r="A114" t="s">
         <v>10</v>
       </c>
-      <c r="B114" s="1">
-        <v>5</v>
-      </c>
-      <c r="C114" s="1">
+      <c r="B114" s="0">
+        <v>5</v>
+      </c>
+      <c r="C114" s="0">
         <v>66.573947273860682</v>
       </c>
     </row>
@@ -1409,10 +1410,10 @@
       <c r="A115" t="s">
         <v>10</v>
       </c>
-      <c r="B115" s="1">
-        <v>6</v>
-      </c>
-      <c r="C115" s="1">
+      <c r="B115" s="0">
+        <v>6</v>
+      </c>
+      <c r="C115" s="0">
         <v>53.468607020779125</v>
       </c>
     </row>
@@ -1420,10 +1421,10 @@
       <c r="A116" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="1">
-        <v>7</v>
-      </c>
-      <c r="C116" s="1">
+      <c r="B116" s="0">
+        <v>7</v>
+      </c>
+      <c r="C116" s="0">
         <v>48.757679221451504</v>
       </c>
     </row>
@@ -1431,10 +1432,10 @@
       <c r="A117" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="1">
-        <v>8</v>
-      </c>
-      <c r="C117" s="1">
+      <c r="B117" s="0">
+        <v>8</v>
+      </c>
+      <c r="C117" s="0">
         <v>77.388682544021719</v>
       </c>
     </row>
@@ -1442,10 +1443,10 @@
       <c r="A118" t="s">
         <v>10</v>
       </c>
-      <c r="B118" s="1">
-        <v>9</v>
-      </c>
-      <c r="C118" s="1">
+      <c r="B118" s="0">
+        <v>9</v>
+      </c>
+      <c r="C118" s="0">
         <v>132.26575539424326</v>
       </c>
     </row>
@@ -1453,10 +1454,10 @@
       <c r="A119" t="s">
         <v>10</v>
       </c>
-      <c r="B119" s="1">
-        <v>10</v>
-      </c>
-      <c r="C119" s="1">
+      <c r="B119" s="0">
+        <v>10</v>
+      </c>
+      <c r="C119" s="0">
         <v>91.692920345072537</v>
       </c>
     </row>
@@ -1464,10 +1465,10 @@
       <c r="A120" t="s">
         <v>10</v>
       </c>
-      <c r="B120" s="1">
-        <v>11</v>
-      </c>
-      <c r="C120" s="1">
+      <c r="B120" s="0">
+        <v>11</v>
+      </c>
+      <c r="C120" s="0">
         <v>131.62321770144564</v>
       </c>
     </row>
@@ -1475,10 +1476,10 @@
       <c r="A121" t="s">
         <v>10</v>
       </c>
-      <c r="B121" s="1">
-        <v>12</v>
-      </c>
-      <c r="C121" s="1">
+      <c r="B121" s="0">
+        <v>12</v>
+      </c>
+      <c r="C121" s="0">
         <v>150.8732135162181</v>
       </c>
     </row>
@@ -1486,10 +1487,10 @@
       <c r="A122" t="s">
         <v>11</v>
       </c>
-      <c r="B122" s="1">
-        <v>1</v>
-      </c>
-      <c r="C122" s="1">
+      <c r="B122" s="0">
+        <v>1</v>
+      </c>
+      <c r="C122" s="0">
         <v>138.57289473235426</v>
       </c>
     </row>
@@ -1497,10 +1498,10 @@
       <c r="A123" t="s">
         <v>11</v>
       </c>
-      <c r="B123" s="1">
-        <v>2</v>
-      </c>
-      <c r="C123" s="1">
+      <c r="B123" s="0">
+        <v>2</v>
+      </c>
+      <c r="C123" s="0">
         <v>145.78488588875288</v>
       </c>
     </row>
@@ -1508,10 +1509,10 @@
       <c r="A124" t="s">
         <v>11</v>
       </c>
-      <c r="B124" s="1">
-        <v>3</v>
-      </c>
-      <c r="C124" s="1">
+      <c r="B124" s="0">
+        <v>3</v>
+      </c>
+      <c r="C124" s="0">
         <v>168.74941890266629</v>
       </c>
     </row>
@@ -1519,10 +1520,10 @@
       <c r="A125" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="1">
-        <v>4</v>
-      </c>
-      <c r="C125" s="1">
+      <c r="B125" s="0">
+        <v>4</v>
+      </c>
+      <c r="C125" s="0">
         <v>129.51088529834928</v>
       </c>
     </row>
@@ -1530,10 +1531,10 @@
       <c r="A126" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="1">
-        <v>5</v>
-      </c>
-      <c r="C126" s="1">
+      <c r="B126" s="0">
+        <v>5</v>
+      </c>
+      <c r="C126" s="0">
         <v>112.51807597636849</v>
       </c>
     </row>
@@ -1541,10 +1542,10 @@
       <c r="A127" t="s">
         <v>11</v>
       </c>
-      <c r="B127" s="1">
-        <v>6</v>
-      </c>
-      <c r="C127" s="1">
+      <c r="B127" s="0">
+        <v>6</v>
+      </c>
+      <c r="C127" s="0">
         <v>107.00998790223383</v>
       </c>
     </row>
@@ -1552,10 +1553,10 @@
       <c r="A128" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="1">
-        <v>7</v>
-      </c>
-      <c r="C128" s="1">
+      <c r="B128" s="0">
+        <v>7</v>
+      </c>
+      <c r="C128" s="0">
         <v>113.38642811958277</v>
       </c>
     </row>
@@ -1563,10 +1564,10 @@
       <c r="A129" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="1">
-        <v>8</v>
-      </c>
-      <c r="C129" s="1">
+      <c r="B129" s="0">
+        <v>8</v>
+      </c>
+      <c r="C129" s="0">
         <v>143.64464702090251</v>
       </c>
     </row>
@@ -1574,10 +1575,10 @@
       <c r="A130" t="s">
         <v>11</v>
       </c>
-      <c r="B130" s="1">
-        <v>9</v>
-      </c>
-      <c r="C130" s="1">
+      <c r="B130" s="0">
+        <v>9</v>
+      </c>
+      <c r="C130" s="0">
         <v>191.05963498096241</v>
       </c>
     </row>
@@ -1585,10 +1586,10 @@
       <c r="A131" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="1">
-        <v>10</v>
-      </c>
-      <c r="C131" s="1">
+      <c r="B131" s="0">
+        <v>10</v>
+      </c>
+      <c r="C131" s="0">
         <v>242.23438012932465</v>
       </c>
     </row>
@@ -1596,10 +1597,10 @@
       <c r="A132" t="s">
         <v>11</v>
       </c>
-      <c r="B132" s="1">
-        <v>11</v>
-      </c>
-      <c r="C132" s="1">
+      <c r="B132" s="0">
+        <v>11</v>
+      </c>
+      <c r="C132" s="0">
         <v>169.54905468701816</v>
       </c>
     </row>
@@ -1607,10 +1608,10 @@
       <c r="A133" t="s">
         <v>11</v>
       </c>
-      <c r="B133" s="1">
-        <v>12</v>
-      </c>
-      <c r="C133" s="1">
+      <c r="B133" s="0">
+        <v>12</v>
+      </c>
+      <c r="C133" s="0">
         <v>123.49229337979028</v>
       </c>
     </row>
@@ -1618,10 +1619,10 @@
       <c r="A134" t="s">
         <v>12</v>
       </c>
-      <c r="B134" s="1">
-        <v>1</v>
-      </c>
-      <c r="C134" s="1">
+      <c r="B134" s="0">
+        <v>1</v>
+      </c>
+      <c r="C134" s="0">
         <v>129.44590205794026</v>
       </c>
     </row>
@@ -1629,10 +1630,10 @@
       <c r="A135" t="s">
         <v>12</v>
       </c>
-      <c r="B135" s="1">
-        <v>2</v>
-      </c>
-      <c r="C135" s="1">
+      <c r="B135" s="0">
+        <v>2</v>
+      </c>
+      <c r="C135" s="0">
         <v>129.95284607940246</v>
       </c>
     </row>
@@ -1640,10 +1641,10 @@
       <c r="A136" t="s">
         <v>12</v>
       </c>
-      <c r="B136" s="1">
-        <v>3</v>
-      </c>
-      <c r="C136" s="1">
+      <c r="B136" s="0">
+        <v>3</v>
+      </c>
+      <c r="C136" s="0">
         <v>111.89680762313428</v>
       </c>
     </row>
@@ -1651,10 +1652,10 @@
       <c r="A137" t="s">
         <v>12</v>
       </c>
-      <c r="B137" s="1">
-        <v>4</v>
-      </c>
-      <c r="C137" s="1">
+      <c r="B137" s="0">
+        <v>4</v>
+      </c>
+      <c r="C137" s="0">
         <v>111.68908181978891</v>
       </c>
     </row>
@@ -1662,10 +1663,10 @@
       <c r="A138" t="s">
         <v>12</v>
       </c>
-      <c r="B138" s="1">
-        <v>5</v>
-      </c>
-      <c r="C138" s="1">
+      <c r="B138" s="0">
+        <v>5</v>
+      </c>
+      <c r="C138" s="0">
         <v>116.61089085999414</v>
       </c>
     </row>
@@ -1673,10 +1674,10 @@
       <c r="A139" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="1">
-        <v>6</v>
-      </c>
-      <c r="C139" s="1">
+      <c r="B139" s="0">
+        <v>6</v>
+      </c>
+      <c r="C139" s="0">
         <v>154.18635733037533</v>
       </c>
     </row>
@@ -1684,10 +1685,10 @@
       <c r="A140" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="1">
-        <v>7</v>
-      </c>
-      <c r="C140" s="1">
+      <c r="B140" s="0">
+        <v>7</v>
+      </c>
+      <c r="C140" s="0">
         <v>128.96145456031053</v>
       </c>
     </row>
@@ -1695,10 +1696,10 @@
       <c r="A141" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="1">
-        <v>8</v>
-      </c>
-      <c r="C141" s="1">
+      <c r="B141" s="0">
+        <v>8</v>
+      </c>
+      <c r="C141" s="0">
         <v>117.74832179758042</v>
       </c>
     </row>
@@ -1706,10 +1707,10 @@
       <c r="A142" t="s">
         <v>12</v>
       </c>
-      <c r="B142" s="1">
-        <v>9</v>
-      </c>
-      <c r="C142" s="1">
+      <c r="B142" s="0">
+        <v>9</v>
+      </c>
+      <c r="C142" s="0">
         <v>100.0763504077331</v>
       </c>
     </row>
@@ -1717,10 +1718,10 @@
       <c r="A143" t="s">
         <v>12</v>
       </c>
-      <c r="B143" s="1">
-        <v>10</v>
-      </c>
-      <c r="C143" s="1">
+      <c r="B143" s="0">
+        <v>10</v>
+      </c>
+      <c r="C143" s="0">
         <v>107.54240446531122</v>
       </c>
     </row>
@@ -1728,10 +1729,10 @@
       <c r="A144" t="s">
         <v>12</v>
       </c>
-      <c r="B144" s="1">
-        <v>11</v>
-      </c>
-      <c r="C144" s="1">
+      <c r="B144" s="0">
+        <v>11</v>
+      </c>
+      <c r="C144" s="0">
         <v>107.57200130311233</v>
       </c>
     </row>
@@ -1739,10 +1740,10 @@
       <c r="A145" t="s">
         <v>12</v>
       </c>
-      <c r="B145" s="1">
-        <v>12</v>
-      </c>
-      <c r="C145" s="1">
+      <c r="B145" s="0">
+        <v>12</v>
+      </c>
+      <c r="C145" s="0">
         <v>135.97782174570824</v>
       </c>
     </row>
@@ -1750,10 +1751,10 @@
       <c r="A146" t="s">
         <v>13</v>
       </c>
-      <c r="B146" s="1">
-        <v>1</v>
-      </c>
-      <c r="C146" s="1">
+      <c r="B146" s="0">
+        <v>1</v>
+      </c>
+      <c r="C146" s="0">
         <v>148.26556162676309</v>
       </c>
     </row>
@@ -1761,10 +1762,10 @@
       <c r="A147" t="s">
         <v>13</v>
       </c>
-      <c r="B147" s="1">
-        <v>2</v>
-      </c>
-      <c r="C147" s="1">
+      <c r="B147" s="0">
+        <v>2</v>
+      </c>
+      <c r="C147" s="0">
         <v>143.34239608678251</v>
       </c>
     </row>
@@ -1772,10 +1773,10 @@
       <c r="A148" t="s">
         <v>13</v>
       </c>
-      <c r="B148" s="1">
-        <v>3</v>
-      </c>
-      <c r="C148" s="1">
+      <c r="B148" s="0">
+        <v>3</v>
+      </c>
+      <c r="C148" s="0">
         <v>160.08868904162972</v>
       </c>
     </row>
@@ -1783,10 +1784,10 @@
       <c r="A149" t="s">
         <v>13</v>
       </c>
-      <c r="B149" s="1">
-        <v>4</v>
-      </c>
-      <c r="C149" s="1">
+      <c r="B149" s="0">
+        <v>4</v>
+      </c>
+      <c r="C149" s="0">
         <v>161.00445943010854</v>
       </c>
     </row>
@@ -1794,10 +1795,10 @@
       <c r="A150" t="s">
         <v>13</v>
       </c>
-      <c r="B150" s="1">
-        <v>5</v>
-      </c>
-      <c r="C150" s="1">
+      <c r="B150" s="0">
+        <v>5</v>
+      </c>
+      <c r="C150" s="0">
         <v>243.53857801491344</v>
       </c>
     </row>
@@ -1805,10 +1806,10 @@
       <c r="A151" t="s">
         <v>13</v>
       </c>
-      <c r="B151" s="1">
-        <v>6</v>
-      </c>
-      <c r="C151" s="1">
+      <c r="B151" s="0">
+        <v>6</v>
+      </c>
+      <c r="C151" s="0">
         <v>184.0182788836257</v>
       </c>
     </row>
@@ -1816,10 +1817,10 @@
       <c r="A152" t="s">
         <v>13</v>
       </c>
-      <c r="B152" s="1">
-        <v>7</v>
-      </c>
-      <c r="C152" s="1">
+      <c r="B152" s="0">
+        <v>7</v>
+      </c>
+      <c r="C152" s="0">
         <v>142.86163286041818</v>
       </c>
     </row>
@@ -1827,10 +1828,10 @@
       <c r="A153" t="s">
         <v>13</v>
       </c>
-      <c r="B153" s="1">
-        <v>8</v>
-      </c>
-      <c r="C153" s="1">
+      <c r="B153" s="0">
+        <v>8</v>
+      </c>
+      <c r="C153" s="0">
         <v>165.98422462934116</v>
       </c>
     </row>
@@ -1838,10 +1839,10 @@
       <c r="A154" t="s">
         <v>13</v>
       </c>
-      <c r="B154" s="1">
-        <v>9</v>
-      </c>
-      <c r="C154" s="1">
+      <c r="B154" s="0">
+        <v>9</v>
+      </c>
+      <c r="C154" s="0">
         <v>127.90262125152725</v>
       </c>
     </row>
@@ -1849,10 +1850,10 @@
       <c r="A155" t="s">
         <v>13</v>
       </c>
-      <c r="B155" s="1">
-        <v>10</v>
-      </c>
-      <c r="C155" s="1">
+      <c r="B155" s="0">
+        <v>10</v>
+      </c>
+      <c r="C155" s="0">
         <v>177.80286471621724</v>
       </c>
     </row>
@@ -1860,10 +1861,10 @@
       <c r="A156" t="s">
         <v>13</v>
       </c>
-      <c r="B156" s="1">
-        <v>11</v>
-      </c>
-      <c r="C156" s="1">
+      <c r="B156" s="0">
+        <v>11</v>
+      </c>
+      <c r="C156" s="0">
         <v>153.24843338306422</v>
       </c>
     </row>
@@ -1871,10 +1872,10 @@
       <c r="A157" t="s">
         <v>13</v>
       </c>
-      <c r="B157" s="1">
-        <v>12</v>
-      </c>
-      <c r="C157" s="1">
+      <c r="B157" s="0">
+        <v>12</v>
+      </c>
+      <c r="C157" s="0">
         <v>122.77899240938301</v>
       </c>
     </row>
@@ -1882,10 +1883,10 @@
       <c r="A158" t="s">
         <v>14</v>
       </c>
-      <c r="B158" s="1">
-        <v>1</v>
-      </c>
-      <c r="C158" s="1">
+      <c r="B158" s="0">
+        <v>1</v>
+      </c>
+      <c r="C158" s="0">
         <v>123.680147938887</v>
       </c>
     </row>
@@ -1893,10 +1894,10 @@
       <c r="A159" t="s">
         <v>14</v>
       </c>
-      <c r="B159" s="1">
-        <v>2</v>
-      </c>
-      <c r="C159" s="1">
+      <c r="B159" s="0">
+        <v>2</v>
+      </c>
+      <c r="C159" s="0">
         <v>119.12127850168046</v>
       </c>
     </row>
@@ -1904,10 +1905,10 @@
       <c r="A160" t="s">
         <v>14</v>
       </c>
-      <c r="B160" s="1">
-        <v>3</v>
-      </c>
-      <c r="C160" s="1">
+      <c r="B160" s="0">
+        <v>3</v>
+      </c>
+      <c r="C160" s="0">
         <v>131.42253843387149</v>
       </c>
     </row>
@@ -1915,10 +1916,10 @@
       <c r="A161" t="s">
         <v>14</v>
       </c>
-      <c r="B161" s="1">
-        <v>4</v>
-      </c>
-      <c r="C161" s="1">
+      <c r="B161" s="0">
+        <v>4</v>
+      </c>
+      <c r="C161" s="0">
         <v>97.93698999814309</v>
       </c>
     </row>
@@ -1926,10 +1927,10 @@
       <c r="A162" t="s">
         <v>14</v>
       </c>
-      <c r="B162" s="1">
-        <v>5</v>
-      </c>
-      <c r="C162" s="1">
+      <c r="B162" s="0">
+        <v>5</v>
+      </c>
+      <c r="C162" s="0">
         <v>94.244068778262516</v>
       </c>
     </row>
@@ -1937,10 +1938,10 @@
       <c r="A163" t="s">
         <v>14</v>
       </c>
-      <c r="B163" s="1">
-        <v>6</v>
-      </c>
-      <c r="C163" s="1">
+      <c r="B163" s="0">
+        <v>6</v>
+      </c>
+      <c r="C163" s="0">
         <v>122.6976663955935</v>
       </c>
     </row>
@@ -1948,10 +1949,10 @@
       <c r="A164" t="s">
         <v>14</v>
       </c>
-      <c r="B164" s="1">
-        <v>7</v>
-      </c>
-      <c r="C164" s="1">
+      <c r="B164" s="0">
+        <v>7</v>
+      </c>
+      <c r="C164" s="0">
         <v>149.02829406668391</v>
       </c>
     </row>
@@ -1959,10 +1960,10 @@
       <c r="A165" t="s">
         <v>14</v>
       </c>
-      <c r="B165" s="1">
-        <v>8</v>
-      </c>
-      <c r="C165" s="1">
+      <c r="B165" s="0">
+        <v>8</v>
+      </c>
+      <c r="C165" s="0">
         <v>177.75312265089235</v>
       </c>
     </row>
@@ -1970,10 +1971,10 @@
       <c r="A166" t="s">
         <v>14</v>
       </c>
-      <c r="B166" s="1">
-        <v>9</v>
-      </c>
-      <c r="C166" s="1">
+      <c r="B166" s="0">
+        <v>9</v>
+      </c>
+      <c r="C166" s="0">
         <v>153.32764352624784</v>
       </c>
     </row>
@@ -1981,10 +1982,10 @@
       <c r="A167" t="s">
         <v>14</v>
       </c>
-      <c r="B167" s="1">
-        <v>10</v>
-      </c>
-      <c r="C167" s="1">
+      <c r="B167" s="0">
+        <v>10</v>
+      </c>
+      <c r="C167" s="0">
         <v>149.69090675465347</v>
       </c>
     </row>
@@ -1992,10 +1993,10 @@
       <c r="A168" t="s">
         <v>14</v>
       </c>
-      <c r="B168" s="1">
-        <v>11</v>
-      </c>
-      <c r="C168" s="1">
+      <c r="B168" s="0">
+        <v>11</v>
+      </c>
+      <c r="C168" s="0">
         <v>209.89849346585174</v>
       </c>
     </row>
@@ -2003,10 +2004,10 @@
       <c r="A169" t="s">
         <v>14</v>
       </c>
-      <c r="B169" s="1">
-        <v>12</v>
-      </c>
-      <c r="C169" s="1">
+      <c r="B169" s="0">
+        <v>12</v>
+      </c>
+      <c r="C169" s="0">
         <v>140.62797929349495</v>
       </c>
     </row>
@@ -2014,10 +2015,10 @@
       <c r="A170" t="s">
         <v>15</v>
       </c>
-      <c r="B170" s="1">
-        <v>1</v>
-      </c>
-      <c r="C170" s="1">
+      <c r="B170" s="0">
+        <v>1</v>
+      </c>
+      <c r="C170" s="0">
         <v>137.26155402113505</v>
       </c>
     </row>
@@ -2025,10 +2026,10 @@
       <c r="A171" t="s">
         <v>15</v>
       </c>
-      <c r="B171" s="1">
-        <v>2</v>
-      </c>
-      <c r="C171" s="1">
+      <c r="B171" s="0">
+        <v>2</v>
+      </c>
+      <c r="C171" s="0">
         <v>132.0202282564008</v>
       </c>
     </row>
@@ -2036,10 +2037,10 @@
       <c r="A172" t="s">
         <v>15</v>
       </c>
-      <c r="B172" s="1">
-        <v>3</v>
-      </c>
-      <c r="C172" s="1">
+      <c r="B172" s="0">
+        <v>3</v>
+      </c>
+      <c r="C172" s="0">
         <v>103.72963719791315</v>
       </c>
     </row>
@@ -2047,10 +2048,10 @@
       <c r="A173" t="s">
         <v>15</v>
       </c>
-      <c r="B173" s="1">
-        <v>4</v>
-      </c>
-      <c r="C173" s="1">
+      <c r="B173" s="0">
+        <v>4</v>
+      </c>
+      <c r="C173" s="0">
         <v>109.31269219071331</v>
       </c>
     </row>
@@ -2058,10 +2059,10 @@
       <c r="A174" t="s">
         <v>15</v>
       </c>
-      <c r="B174" s="1">
-        <v>5</v>
-      </c>
-      <c r="C174" s="1">
+      <c r="B174" s="0">
+        <v>5</v>
+      </c>
+      <c r="C174" s="0">
         <v>151.78517880787442</v>
       </c>
     </row>
@@ -2069,10 +2070,10 @@
       <c r="A175" t="s">
         <v>15</v>
       </c>
-      <c r="B175" s="1">
-        <v>6</v>
-      </c>
-      <c r="C175" s="1">
+      <c r="B175" s="0">
+        <v>6</v>
+      </c>
+      <c r="C175" s="0">
         <v>169.64907552579561</v>
       </c>
     </row>
@@ -2080,10 +2081,10 @@
       <c r="A176" t="s">
         <v>15</v>
       </c>
-      <c r="B176" s="1">
-        <v>7</v>
-      </c>
-      <c r="C176" s="1">
+      <c r="B176" s="0">
+        <v>7</v>
+      </c>
+      <c r="C176" s="0">
         <v>129.98323050053759</v>
       </c>
     </row>
@@ -2091,10 +2092,10 @@
       <c r="A177" t="s">
         <v>15</v>
       </c>
-      <c r="B177" s="1">
-        <v>8</v>
-      </c>
-      <c r="C177" s="1">
+      <c r="B177" s="0">
+        <v>8</v>
+      </c>
+      <c r="C177" s="0">
         <v>98.178687632659731</v>
       </c>
     </row>
@@ -2102,10 +2103,10 @@
       <c r="A178" t="s">
         <v>15</v>
       </c>
-      <c r="B178" s="1">
-        <v>9</v>
-      </c>
-      <c r="C178" s="1">
+      <c r="B178" s="0">
+        <v>9</v>
+      </c>
+      <c r="C178" s="0">
         <v>124.43543264760135</v>
       </c>
     </row>
@@ -2113,10 +2114,10 @@
       <c r="A179" t="s">
         <v>15</v>
       </c>
-      <c r="B179" s="1">
-        <v>10</v>
-      </c>
-      <c r="C179" s="1">
+      <c r="B179" s="0">
+        <v>10</v>
+      </c>
+      <c r="C179" s="0">
         <v>153.99229062161274</v>
       </c>
     </row>
@@ -2124,10 +2125,10 @@
       <c r="A180" t="s">
         <v>15</v>
       </c>
-      <c r="B180" s="1">
-        <v>11</v>
-      </c>
-      <c r="C180" s="1">
+      <c r="B180" s="0">
+        <v>11</v>
+      </c>
+      <c r="C180" s="0">
         <v>162.1009636904767</v>
       </c>
     </row>
@@ -2135,10 +2136,10 @@
       <c r="A181" t="s">
         <v>15</v>
       </c>
-      <c r="B181" s="1">
-        <v>12</v>
-      </c>
-      <c r="C181" s="1">
+      <c r="B181" s="0">
+        <v>12</v>
+      </c>
+      <c r="C181" s="0">
         <v>140.64389927578668</v>
       </c>
     </row>
@@ -2146,10 +2147,10 @@
       <c r="A182" t="s">
         <v>16</v>
       </c>
-      <c r="B182" s="1">
-        <v>1</v>
-      </c>
-      <c r="C182" s="1">
+      <c r="B182" s="0">
+        <v>1</v>
+      </c>
+      <c r="C182" s="0">
         <v>187.77022088412104</v>
       </c>
     </row>
@@ -2157,10 +2158,10 @@
       <c r="A183" t="s">
         <v>16</v>
       </c>
-      <c r="B183" s="1">
-        <v>2</v>
-      </c>
-      <c r="C183" s="1">
+      <c r="B183" s="0">
+        <v>2</v>
+      </c>
+      <c r="C183" s="0">
         <v>97.381306471276645</v>
       </c>
     </row>
@@ -2168,10 +2169,10 @@
       <c r="A184" t="s">
         <v>16</v>
       </c>
-      <c r="B184" s="1">
-        <v>3</v>
-      </c>
-      <c r="C184" s="1">
+      <c r="B184" s="0">
+        <v>3</v>
+      </c>
+      <c r="C184" s="0">
         <v>108.96334469441564</v>
       </c>
     </row>
@@ -2179,10 +2180,10 @@
       <c r="A185" t="s">
         <v>16</v>
       </c>
-      <c r="B185" s="1">
-        <v>4</v>
-      </c>
-      <c r="C185" s="1">
+      <c r="B185" s="0">
+        <v>4</v>
+      </c>
+      <c r="C185" s="0">
         <v>101.40814734641286</v>
       </c>
     </row>
@@ -2190,10 +2191,10 @@
       <c r="A186" t="s">
         <v>16</v>
       </c>
-      <c r="B186" s="1">
-        <v>5</v>
-      </c>
-      <c r="C186" s="1">
+      <c r="B186" s="0">
+        <v>5</v>
+      </c>
+      <c r="C186" s="0">
         <v>72.982437440336582</v>
       </c>
     </row>
@@ -2201,10 +2202,10 @@
       <c r="A187" t="s">
         <v>16</v>
       </c>
-      <c r="B187" s="1">
-        <v>6</v>
-      </c>
-      <c r="C187" s="1">
+      <c r="B187" s="0">
+        <v>6</v>
+      </c>
+      <c r="C187" s="0">
         <v>90.508135573528975</v>
       </c>
     </row>
@@ -2212,10 +2213,10 @@
       <c r="A188" t="s">
         <v>16</v>
       </c>
-      <c r="B188" s="1">
-        <v>7</v>
-      </c>
-      <c r="C188" s="1">
+      <c r="B188" s="0">
+        <v>7</v>
+      </c>
+      <c r="C188" s="0">
         <v>68.187994849365296</v>
       </c>
     </row>
@@ -2223,10 +2224,10 @@
       <c r="A189" t="s">
         <v>16</v>
       </c>
-      <c r="B189" s="1">
-        <v>8</v>
-      </c>
-      <c r="C189" s="1">
+      <c r="B189" s="0">
+        <v>8</v>
+      </c>
+      <c r="C189" s="0">
         <v>91.647729301347653</v>
       </c>
     </row>
@@ -2234,10 +2235,10 @@
       <c r="A190" t="s">
         <v>16</v>
       </c>
-      <c r="B190" s="1">
-        <v>9</v>
-      </c>
-      <c r="C190" s="1">
+      <c r="B190" s="0">
+        <v>9</v>
+      </c>
+      <c r="C190" s="0">
         <v>94.262173923082898</v>
       </c>
     </row>
@@ -2245,10 +2246,10 @@
       <c r="A191" t="s">
         <v>16</v>
       </c>
-      <c r="B191" s="1">
-        <v>10</v>
-      </c>
-      <c r="C191" s="1">
+      <c r="B191" s="0">
+        <v>10</v>
+      </c>
+      <c r="C191" s="0">
         <v>110.99637349305908</v>
       </c>
     </row>
@@ -2256,10 +2257,10 @@
       <c r="A192" t="s">
         <v>16</v>
       </c>
-      <c r="B192" s="1">
-        <v>11</v>
-      </c>
-      <c r="C192" s="1">
+      <c r="B192" s="0">
+        <v>11</v>
+      </c>
+      <c r="C192" s="0">
         <v>82.074792420418262</v>
       </c>
     </row>
@@ -2267,10 +2268,10 @@
       <c r="A193" t="s">
         <v>16</v>
       </c>
-      <c r="B193" s="1">
-        <v>12</v>
-      </c>
-      <c r="C193" s="1">
+      <c r="B193" s="0">
+        <v>12</v>
+      </c>
+      <c r="C193" s="0">
         <v>89.423936228742434</v>
       </c>
     </row>
@@ -2278,10 +2279,10 @@
       <c r="A194" t="s">
         <v>17</v>
       </c>
-      <c r="B194" s="1">
-        <v>1</v>
-      </c>
-      <c r="C194" s="1">
+      <c r="B194" s="0">
+        <v>1</v>
+      </c>
+      <c r="C194" s="0">
         <v>103.99873345811896</v>
       </c>
     </row>
@@ -2289,10 +2290,10 @@
       <c r="A195" t="s">
         <v>17</v>
       </c>
-      <c r="B195" s="1">
-        <v>2</v>
-      </c>
-      <c r="C195" s="1">
+      <c r="B195" s="0">
+        <v>2</v>
+      </c>
+      <c r="C195" s="0">
         <v>117.69553222863824</v>
       </c>
     </row>
@@ -2300,10 +2301,10 @@
       <c r="A196" t="s">
         <v>17</v>
       </c>
-      <c r="B196" s="1">
-        <v>3</v>
-      </c>
-      <c r="C196" s="1">
+      <c r="B196" s="0">
+        <v>3</v>
+      </c>
+      <c r="C196" s="0">
         <v>111.0478958953252</v>
       </c>
     </row>
@@ -2311,10 +2312,10 @@
       <c r="A197" t="s">
         <v>17</v>
       </c>
-      <c r="B197" s="1">
-        <v>4</v>
-      </c>
-      <c r="C197" s="1">
+      <c r="B197" s="0">
+        <v>4</v>
+      </c>
+      <c r="C197" s="0">
         <v>71.1262323283146</v>
       </c>
     </row>
@@ -2322,10 +2323,10 @@
       <c r="A198" t="s">
         <v>17</v>
       </c>
-      <c r="B198" s="1">
-        <v>5</v>
-      </c>
-      <c r="C198" s="1">
+      <c r="B198" s="0">
+        <v>5</v>
+      </c>
+      <c r="C198" s="0">
         <v>90.164919466224845</v>
       </c>
     </row>
@@ -2333,10 +2334,10 @@
       <c r="A199" t="s">
         <v>17</v>
       </c>
-      <c r="B199" s="1">
-        <v>6</v>
-      </c>
-      <c r="C199" s="1">
+      <c r="B199" s="0">
+        <v>6</v>
+      </c>
+      <c r="C199" s="0">
         <v>68.777371135066772</v>
       </c>
     </row>
@@ -2344,10 +2345,10 @@
       <c r="A200" t="s">
         <v>17</v>
       </c>
-      <c r="B200" s="1">
-        <v>7</v>
-      </c>
-      <c r="C200" s="1">
+      <c r="B200" s="0">
+        <v>7</v>
+      </c>
+      <c r="C200" s="0">
         <v>62.335446437524098</v>
       </c>
     </row>
@@ -2355,10 +2356,10 @@
       <c r="A201" t="s">
         <v>17</v>
       </c>
-      <c r="B201" s="1">
-        <v>8</v>
-      </c>
-      <c r="C201" s="1">
+      <c r="B201" s="0">
+        <v>8</v>
+      </c>
+      <c r="C201" s="0">
         <v>132.4733321477305</v>
       </c>
     </row>
@@ -2366,10 +2367,10 @@
       <c r="A202" t="s">
         <v>17</v>
       </c>
-      <c r="B202" s="1">
-        <v>9</v>
-      </c>
-      <c r="C202" s="1">
+      <c r="B202" s="0">
+        <v>9</v>
+      </c>
+      <c r="C202" s="0">
         <v>176.28371206161788</v>
       </c>
     </row>
@@ -2377,10 +2378,10 @@
       <c r="A203" t="s">
         <v>17</v>
       </c>
-      <c r="B203" s="1">
-        <v>10</v>
-      </c>
-      <c r="C203" s="1">
+      <c r="B203" s="0">
+        <v>10</v>
+      </c>
+      <c r="C203" s="0">
         <v>95.969213403346714</v>
       </c>
     </row>
@@ -2388,10 +2389,10 @@
       <c r="A204" t="s">
         <v>17</v>
       </c>
-      <c r="B204" s="1">
-        <v>11</v>
-      </c>
-      <c r="C204" s="1">
+      <c r="B204" s="0">
+        <v>11</v>
+      </c>
+      <c r="C204" s="0">
         <v>86.566503465758885</v>
       </c>
     </row>
@@ -2399,10 +2400,10 @@
       <c r="A205" t="s">
         <v>17</v>
       </c>
-      <c r="B205" s="1">
-        <v>12</v>
-      </c>
-      <c r="C205" s="1">
+      <c r="B205" s="0">
+        <v>12</v>
+      </c>
+      <c r="C205" s="0">
         <v>121.59108669531599</v>
       </c>
     </row>
@@ -2410,10 +2411,10 @@
       <c r="A206" t="s">
         <v>18</v>
       </c>
-      <c r="B206" s="1">
-        <v>1</v>
-      </c>
-      <c r="C206" s="1">
+      <c r="B206" s="0">
+        <v>1</v>
+      </c>
+      <c r="C206" s="0">
         <v>135.73043577158847</v>
       </c>
     </row>
@@ -2421,10 +2422,10 @@
       <c r="A207" t="s">
         <v>18</v>
       </c>
-      <c r="B207" s="1">
-        <v>2</v>
-      </c>
-      <c r="C207" s="1">
+      <c r="B207" s="0">
+        <v>2</v>
+      </c>
+      <c r="C207" s="0">
         <v>119.08361999195742</v>
       </c>
     </row>
@@ -2432,10 +2433,10 @@
       <c r="A208" t="s">
         <v>18</v>
       </c>
-      <c r="B208" s="1">
-        <v>3</v>
-      </c>
-      <c r="C208" s="1">
+      <c r="B208" s="0">
+        <v>3</v>
+      </c>
+      <c r="C208" s="0">
         <v>131.49864754410734</v>
       </c>
     </row>
@@ -2443,10 +2444,10 @@
       <c r="A209" t="s">
         <v>18</v>
       </c>
-      <c r="B209" s="1">
-        <v>4</v>
-      </c>
-      <c r="C209" s="1">
+      <c r="B209" s="0">
+        <v>4</v>
+      </c>
+      <c r="C209" s="0">
         <v>170.47333251119781</v>
       </c>
     </row>
@@ -2454,10 +2455,10 @@
       <c r="A210" t="s">
         <v>18</v>
       </c>
-      <c r="B210" s="1">
-        <v>5</v>
-      </c>
-      <c r="C210" s="1">
+      <c r="B210" s="0">
+        <v>5</v>
+      </c>
+      <c r="C210" s="0">
         <v>140.91246000958591</v>
       </c>
     </row>
@@ -2465,10 +2466,10 @@
       <c r="A211" t="s">
         <v>18</v>
       </c>
-      <c r="B211" s="1">
-        <v>6</v>
-      </c>
-      <c r="C211" s="1">
+      <c r="B211" s="0">
+        <v>6</v>
+      </c>
+      <c r="C211" s="0">
         <v>148.8165613417035</v>
       </c>
     </row>
@@ -2476,10 +2477,10 @@
       <c r="A212" t="s">
         <v>18</v>
       </c>
-      <c r="B212" s="1">
-        <v>7</v>
-      </c>
-      <c r="C212" s="1">
+      <c r="B212" s="0">
+        <v>7</v>
+      </c>
+      <c r="C212" s="0">
         <v>136.10010571637537</v>
       </c>
     </row>
@@ -2487,10 +2488,10 @@
       <c r="A213" t="s">
         <v>18</v>
       </c>
-      <c r="B213" s="1">
-        <v>8</v>
-      </c>
-      <c r="C213" s="1">
+      <c r="B213" s="0">
+        <v>8</v>
+      </c>
+      <c r="C213" s="0">
         <v>86.143682706913722</v>
       </c>
     </row>
@@ -2498,10 +2499,10 @@
       <c r="A214" t="s">
         <v>18</v>
       </c>
-      <c r="B214" s="1">
-        <v>9</v>
-      </c>
-      <c r="C214" s="1">
+      <c r="B214" s="0">
+        <v>9</v>
+      </c>
+      <c r="C214" s="0">
         <v>135.07500553450706</v>
       </c>
     </row>
@@ -2509,10 +2510,10 @@
       <c r="A215" t="s">
         <v>18</v>
       </c>
-      <c r="B215" s="1">
-        <v>10</v>
-      </c>
-      <c r="C215" s="1">
+      <c r="B215" s="0">
+        <v>10</v>
+      </c>
+      <c r="C215" s="0">
         <v>89.914531399970812</v>
       </c>
     </row>
@@ -2520,10 +2521,10 @@
       <c r="A216" t="s">
         <v>18</v>
       </c>
-      <c r="B216" s="1">
-        <v>11</v>
-      </c>
-      <c r="C216" s="1">
+      <c r="B216" s="0">
+        <v>11</v>
+      </c>
+      <c r="C216" s="0">
         <v>120.86214520248797</v>
       </c>
     </row>
@@ -2531,10 +2532,10 @@
       <c r="A217" t="s">
         <v>18</v>
       </c>
-      <c r="B217" s="1">
-        <v>12</v>
-      </c>
-      <c r="C217" s="1">
+      <c r="B217" s="0">
+        <v>12</v>
+      </c>
+      <c r="C217" s="0">
         <v>82.872786626003631</v>
       </c>
     </row>
@@ -2542,10 +2543,10 @@
       <c r="A218" t="s">
         <v>19</v>
       </c>
-      <c r="B218" s="1">
-        <v>1</v>
-      </c>
-      <c r="C218" s="1">
+      <c r="B218" s="0">
+        <v>1</v>
+      </c>
+      <c r="C218" s="0">
         <v>135.63231704946662</v>
       </c>
     </row>
@@ -2553,10 +2554,10 @@
       <c r="A219" t="s">
         <v>19</v>
       </c>
-      <c r="B219" s="1">
-        <v>2</v>
-      </c>
-      <c r="C219" s="1">
+      <c r="B219" s="0">
+        <v>2</v>
+      </c>
+      <c r="C219" s="0">
         <v>190.81671473576529</v>
       </c>
     </row>
@@ -2564,10 +2565,10 @@
       <c r="A220" t="s">
         <v>19</v>
       </c>
-      <c r="B220" s="1">
-        <v>3</v>
-      </c>
-      <c r="C220" s="1">
+      <c r="B220" s="0">
+        <v>3</v>
+      </c>
+      <c r="C220" s="0">
         <v>290.92952088547389</v>
       </c>
     </row>
@@ -2575,10 +2576,10 @@
       <c r="A221" t="s">
         <v>19</v>
       </c>
-      <c r="B221" s="1">
-        <v>4</v>
-      </c>
-      <c r="C221" s="1">
+      <c r="B221" s="0">
+        <v>4</v>
+      </c>
+      <c r="C221" s="0">
         <v>197.17079811515333</v>
       </c>
     </row>
@@ -2586,10 +2587,10 @@
       <c r="A222" t="s">
         <v>19</v>
       </c>
-      <c r="B222" s="1">
-        <v>5</v>
-      </c>
-      <c r="C222" s="1">
+      <c r="B222" s="0">
+        <v>5</v>
+      </c>
+      <c r="C222" s="0">
         <v>246.75490878190044</v>
       </c>
     </row>
@@ -2597,10 +2598,10 @@
       <c r="A223" t="s">
         <v>19</v>
       </c>
-      <c r="B223" s="1">
-        <v>6</v>
-      </c>
-      <c r="C223" s="1">
+      <c r="B223" s="0">
+        <v>6</v>
+      </c>
+      <c r="C223" s="0">
         <v>503.94249242172845</v>
       </c>
     </row>
@@ -2608,10 +2609,10 @@
       <c r="A224" t="s">
         <v>19</v>
       </c>
-      <c r="B224" s="1">
-        <v>7</v>
-      </c>
-      <c r="C224" s="1">
+      <c r="B224" s="0">
+        <v>7</v>
+      </c>
+      <c r="C224" s="0">
         <v>558.22364201882272</v>
       </c>
     </row>
@@ -2619,10 +2620,10 @@
       <c r="A225" t="s">
         <v>19</v>
       </c>
-      <c r="B225" s="1">
-        <v>8</v>
-      </c>
-      <c r="C225" s="1">
+      <c r="B225" s="0">
+        <v>8</v>
+      </c>
+      <c r="C225" s="0">
         <v>311.36483202454485</v>
       </c>
     </row>
@@ -2630,10 +2631,10 @@
       <c r="A226" t="s">
         <v>19</v>
       </c>
-      <c r="B226" s="1">
-        <v>9</v>
-      </c>
-      <c r="C226" s="1">
+      <c r="B226" s="0">
+        <v>9</v>
+      </c>
+      <c r="C226" s="0">
         <v>209.63793843523842</v>
       </c>
     </row>
@@ -2641,10 +2642,10 @@
       <c r="A227" t="s">
         <v>19</v>
       </c>
-      <c r="B227" s="1">
-        <v>10</v>
-      </c>
-      <c r="C227" s="1">
+      <c r="B227" s="0">
+        <v>10</v>
+      </c>
+      <c r="C227" s="0">
         <v>270.02349186959714</v>
       </c>
     </row>
@@ -2652,10 +2653,10 @@
       <c r="A228" t="s">
         <v>19</v>
       </c>
-      <c r="B228" s="1">
-        <v>11</v>
-      </c>
-      <c r="C228" s="1">
+      <c r="B228" s="0">
+        <v>11</v>
+      </c>
+      <c r="C228" s="0">
         <v>358.82840880746664</v>
       </c>
     </row>
@@ -2663,10 +2664,10 @@
       <c r="A229" t="s">
         <v>19</v>
       </c>
-      <c r="B229" s="1">
-        <v>12</v>
-      </c>
-      <c r="C229" s="1">
+      <c r="B229" s="0">
+        <v>12</v>
+      </c>
+      <c r="C229" s="0">
         <v>196.34369416706684</v>
       </c>
     </row>
@@ -2674,10 +2675,10 @@
       <c r="A230" t="s">
         <v>20</v>
       </c>
-      <c r="B230" s="1">
-        <v>1</v>
-      </c>
-      <c r="C230" s="1">
+      <c r="B230" s="0">
+        <v>1</v>
+      </c>
+      <c r="C230" s="0">
         <v>257.84839749321475</v>
       </c>
     </row>
@@ -2685,10 +2686,10 @@
       <c r="A231" t="s">
         <v>20</v>
       </c>
-      <c r="B231" s="1">
-        <v>2</v>
-      </c>
-      <c r="C231" s="1">
+      <c r="B231" s="0">
+        <v>2</v>
+      </c>
+      <c r="C231" s="0">
         <v>194.04470490308728</v>
       </c>
     </row>
@@ -2696,10 +2697,10 @@
       <c r="A232" t="s">
         <v>20</v>
       </c>
-      <c r="B232" s="1">
-        <v>3</v>
-      </c>
-      <c r="C232" s="1">
+      <c r="B232" s="0">
+        <v>3</v>
+      </c>
+      <c r="C232" s="0">
         <v>232.45972604144899</v>
       </c>
     </row>
@@ -2707,10 +2708,10 @@
       <c r="A233" t="s">
         <v>20</v>
       </c>
-      <c r="B233" s="1">
-        <v>4</v>
-      </c>
-      <c r="C233" s="1">
+      <c r="B233" s="0">
+        <v>4</v>
+      </c>
+      <c r="C233" s="0">
         <v>169.17603591482319</v>
       </c>
     </row>
@@ -2718,10 +2719,10 @@
       <c r="A234" t="s">
         <v>20</v>
       </c>
-      <c r="B234" s="1">
-        <v>5</v>
-      </c>
-      <c r="C234" s="1">
+      <c r="B234" s="0">
+        <v>5</v>
+      </c>
+      <c r="C234" s="0">
         <v>159.40144524851632</v>
       </c>
     </row>
@@ -2729,10 +2730,10 @@
       <c r="A235" t="s">
         <v>20</v>
       </c>
-      <c r="B235" s="1">
-        <v>6</v>
-      </c>
-      <c r="C235" s="1">
+      <c r="B235" s="0">
+        <v>6</v>
+      </c>
+      <c r="C235" s="0">
         <v>318.99116026199204</v>
       </c>
     </row>
@@ -2740,10 +2741,10 @@
       <c r="A236" t="s">
         <v>20</v>
       </c>
-      <c r="B236" s="1">
-        <v>7</v>
-      </c>
-      <c r="C236" s="1">
+      <c r="B236" s="0">
+        <v>7</v>
+      </c>
+      <c r="C236" s="0">
         <v>183.65895058106582</v>
       </c>
     </row>
@@ -2751,10 +2752,10 @@
       <c r="A237" t="s">
         <v>20</v>
       </c>
-      <c r="B237" s="1">
-        <v>8</v>
-      </c>
-      <c r="C237" s="1">
+      <c r="B237" s="0">
+        <v>8</v>
+      </c>
+      <c r="C237" s="0">
         <v>151.20429781015469</v>
       </c>
     </row>
@@ -2762,10 +2763,10 @@
       <c r="A238" t="s">
         <v>20</v>
       </c>
-      <c r="B238" s="1">
-        <v>9</v>
-      </c>
-      <c r="C238" s="1">
+      <c r="B238" s="0">
+        <v>9</v>
+      </c>
+      <c r="C238" s="0">
         <v>140.77881633904866</v>
       </c>
     </row>
@@ -2773,10 +2774,10 @@
       <c r="A239" t="s">
         <v>20</v>
       </c>
-      <c r="B239" s="1">
-        <v>10</v>
-      </c>
-      <c r="C239" s="1">
+      <c r="B239" s="0">
+        <v>10</v>
+      </c>
+      <c r="C239" s="0">
         <v>184.03005097183708</v>
       </c>
     </row>
@@ -2784,10 +2785,10 @@
       <c r="A240" t="s">
         <v>20</v>
       </c>
-      <c r="B240" s="1">
-        <v>11</v>
-      </c>
-      <c r="C240" s="1">
+      <c r="B240" s="0">
+        <v>11</v>
+      </c>
+      <c r="C240" s="0">
         <v>214.97008095639316</v>
       </c>
     </row>
@@ -2795,10 +2796,10 @@
       <c r="A241" t="s">
         <v>20</v>
       </c>
-      <c r="B241" s="1">
-        <v>12</v>
-      </c>
-      <c r="C241" s="1">
+      <c r="B241" s="0">
+        <v>12</v>
+      </c>
+      <c r="C241" s="0">
         <v>160.7223038718837</v>
       </c>
     </row>
@@ -2806,10 +2807,10 @@
       <c r="A242" t="s">
         <v>21</v>
       </c>
-      <c r="B242" s="1">
-        <v>1</v>
-      </c>
-      <c r="C242" s="1">
+      <c r="B242" s="0">
+        <v>1</v>
+      </c>
+      <c r="C242" s="0">
         <v>123.1599969116685</v>
       </c>
     </row>
@@ -2817,10 +2818,10 @@
       <c r="A243" t="s">
         <v>21</v>
       </c>
-      <c r="B243" s="1">
-        <v>2</v>
-      </c>
-      <c r="C243" s="1">
+      <c r="B243" s="0">
+        <v>2</v>
+      </c>
+      <c r="C243" s="0">
         <v>109.7487332483494</v>
       </c>
     </row>
@@ -2828,10 +2829,10 @@
       <c r="A244" t="s">
         <v>21</v>
       </c>
-      <c r="B244" s="1">
-        <v>3</v>
-      </c>
-      <c r="C244" s="1">
+      <c r="B244" s="0">
+        <v>3</v>
+      </c>
+      <c r="C244" s="0">
         <v>116.60540265498089</v>
       </c>
     </row>
@@ -2839,10 +2840,10 @@
       <c r="A245" t="s">
         <v>21</v>
       </c>
-      <c r="B245" s="1">
-        <v>4</v>
-      </c>
-      <c r="C245" s="1">
+      <c r="B245" s="0">
+        <v>4</v>
+      </c>
+      <c r="C245" s="0">
         <v>102.28703012879106</v>
       </c>
     </row>
@@ -2850,10 +2851,10 @@
       <c r="A246" t="s">
         <v>21</v>
       </c>
-      <c r="B246" s="1">
-        <v>5</v>
-      </c>
-      <c r="C246" s="1">
+      <c r="B246" s="0">
+        <v>5</v>
+      </c>
+      <c r="C246" s="0">
         <v>121.5436956067737</v>
       </c>
     </row>
@@ -2861,10 +2862,10 @@
       <c r="A247" t="s">
         <v>21</v>
       </c>
-      <c r="B247" s="1">
-        <v>6</v>
-      </c>
-      <c r="C247" s="1">
+      <c r="B247" s="0">
+        <v>6</v>
+      </c>
+      <c r="C247" s="0">
         <v>105.48676842316939</v>
       </c>
     </row>
@@ -2872,10 +2873,10 @@
       <c r="A248" t="s">
         <v>21</v>
       </c>
-      <c r="B248" s="1">
-        <v>7</v>
-      </c>
-      <c r="C248" s="1">
+      <c r="B248" s="0">
+        <v>7</v>
+      </c>
+      <c r="C248" s="0">
         <v>129.6226424998398</v>
       </c>
     </row>
@@ -2883,10 +2884,10 @@
       <c r="A249" t="s">
         <v>21</v>
       </c>
-      <c r="B249" s="1">
-        <v>8</v>
-      </c>
-      <c r="C249" s="1">
+      <c r="B249" s="0">
+        <v>8</v>
+      </c>
+      <c r="C249" s="0">
         <v>121.62974835667606</v>
       </c>
     </row>
@@ -2894,10 +2895,10 @@
       <c r="A250" t="s">
         <v>21</v>
       </c>
-      <c r="B250" s="1">
-        <v>9</v>
-      </c>
-      <c r="C250" s="1">
+      <c r="B250" s="0">
+        <v>9</v>
+      </c>
+      <c r="C250" s="0">
         <v>157.31582080050615</v>
       </c>
     </row>
@@ -2905,10 +2906,10 @@
       <c r="A251" t="s">
         <v>21</v>
       </c>
-      <c r="B251" s="1">
-        <v>10</v>
-      </c>
-      <c r="C251" s="1">
+      <c r="B251" s="0">
+        <v>10</v>
+      </c>
+      <c r="C251" s="0">
         <v>183.25266625551419</v>
       </c>
     </row>
@@ -2916,10 +2917,10 @@
       <c r="A252" t="s">
         <v>21</v>
       </c>
-      <c r="B252" s="1">
-        <v>11</v>
-      </c>
-      <c r="C252" s="1">
+      <c r="B252" s="0">
+        <v>11</v>
+      </c>
+      <c r="C252" s="0">
         <v>191.96645652769618</v>
       </c>
     </row>
@@ -2927,10 +2928,10 @@
       <c r="A253" t="s">
         <v>21</v>
       </c>
-      <c r="B253" s="1">
-        <v>12</v>
-      </c>
-      <c r="C253" s="1">
+      <c r="B253" s="0">
+        <v>12</v>
+      </c>
+      <c r="C253" s="0">
         <v>239.69102981938227</v>
       </c>
     </row>
@@ -2938,10 +2939,10 @@
       <c r="A254" t="s">
         <v>22</v>
       </c>
-      <c r="B254" s="1">
-        <v>1</v>
-      </c>
-      <c r="C254" s="1">
+      <c r="B254" s="0">
+        <v>1</v>
+      </c>
+      <c r="C254" s="0">
         <v>309.97244945797701</v>
       </c>
     </row>
@@ -2949,10 +2950,10 @@
       <c r="A255" t="s">
         <v>22</v>
       </c>
-      <c r="B255" s="1">
-        <v>2</v>
-      </c>
-      <c r="C255" s="1">
+      <c r="B255" s="0">
+        <v>2</v>
+      </c>
+      <c r="C255" s="0">
         <v>196.95946459830401</v>
       </c>
     </row>
@@ -2960,10 +2961,10 @@
       <c r="A256" t="s">
         <v>22</v>
       </c>
-      <c r="B256" s="1">
-        <v>3</v>
-      </c>
-      <c r="C256" s="1">
+      <c r="B256" s="0">
+        <v>3</v>
+      </c>
+      <c r="C256" s="0">
         <v>212.78254189044787</v>
       </c>
     </row>
@@ -2971,10 +2972,10 @@
       <c r="A257" t="s">
         <v>22</v>
       </c>
-      <c r="B257" s="1">
-        <v>4</v>
-      </c>
-      <c r="C257" s="1">
+      <c r="B257" s="0">
+        <v>4</v>
+      </c>
+      <c r="C257" s="0">
         <v>135.51848003853243</v>
       </c>
     </row>
@@ -2982,10 +2983,10 @@
       <c r="A258" t="s">
         <v>22</v>
       </c>
-      <c r="B258" s="1">
-        <v>5</v>
-      </c>
-      <c r="C258" s="1">
+      <c r="B258" s="0">
+        <v>5</v>
+      </c>
+      <c r="C258" s="0">
         <v>158.68260551719968</v>
       </c>
     </row>
@@ -2993,10 +2994,10 @@
       <c r="A259" t="s">
         <v>22</v>
       </c>
-      <c r="B259" s="1">
-        <v>6</v>
-      </c>
-      <c r="C259" s="1">
+      <c r="B259" s="0">
+        <v>6</v>
+      </c>
+      <c r="C259" s="0">
         <v>149.80560130108137</v>
       </c>
     </row>
@@ -3004,10 +3005,10 @@
       <c r="A260" t="s">
         <v>22</v>
       </c>
-      <c r="B260" s="1">
-        <v>7</v>
-      </c>
-      <c r="C260" s="1">
+      <c r="B260" s="0">
+        <v>7</v>
+      </c>
+      <c r="C260" s="0">
         <v>202.04377955585122</v>
       </c>
     </row>
@@ -3015,10 +3016,10 @@
       <c r="A261" t="s">
         <v>22</v>
       </c>
-      <c r="B261" s="1">
-        <v>8</v>
-      </c>
-      <c r="C261" s="1">
+      <c r="B261" s="0">
+        <v>8</v>
+      </c>
+      <c r="C261" s="0">
         <v>238.91571234839765</v>
       </c>
     </row>
@@ -3026,10 +3027,10 @@
       <c r="A262" t="s">
         <v>22</v>
       </c>
-      <c r="B262" s="1">
-        <v>9</v>
-      </c>
-      <c r="C262" s="1">
+      <c r="B262" s="0">
+        <v>9</v>
+      </c>
+      <c r="C262" s="0">
         <v>187.41011632363401</v>
       </c>
     </row>
@@ -3037,10 +3038,10 @@
       <c r="A263" t="s">
         <v>22</v>
       </c>
-      <c r="B263" s="1">
-        <v>10</v>
-      </c>
-      <c r="C263" s="1">
+      <c r="B263" s="0">
+        <v>10</v>
+      </c>
+      <c r="C263" s="0">
         <v>233.31156413860188</v>
       </c>
     </row>
@@ -3048,10 +3049,10 @@
       <c r="A264" t="s">
         <v>22</v>
       </c>
-      <c r="B264" s="1">
-        <v>11</v>
-      </c>
-      <c r="C264" s="1">
+      <c r="B264" s="0">
+        <v>11</v>
+      </c>
+      <c r="C264" s="0">
         <v>205.59707355365967</v>
       </c>
     </row>
@@ -3059,10 +3060,10 @@
       <c r="A265" t="s">
         <v>22</v>
       </c>
-      <c r="B265" s="1">
-        <v>12</v>
-      </c>
-      <c r="C265" s="1">
+      <c r="B265" s="0">
+        <v>12</v>
+      </c>
+      <c r="C265" s="0">
         <v>271.30406158523687</v>
       </c>
     </row>
@@ -3070,10 +3071,10 @@
       <c r="A266" t="s">
         <v>23</v>
       </c>
-      <c r="B266" s="1">
-        <v>1</v>
-      </c>
-      <c r="C266" s="1">
+      <c r="B266" s="0">
+        <v>1</v>
+      </c>
+      <c r="C266" s="0">
         <v>198.15649141819117</v>
       </c>
     </row>
@@ -3081,10 +3082,10 @@
       <c r="A267" t="s">
         <v>23</v>
       </c>
-      <c r="B267" s="1">
-        <v>2</v>
-      </c>
-      <c r="C267" s="1">
+      <c r="B267" s="0">
+        <v>2</v>
+      </c>
+      <c r="C267" s="0">
         <v>139.62192204074458</v>
       </c>
     </row>
@@ -3092,10 +3093,10 @@
       <c r="A268" t="s">
         <v>23</v>
       </c>
-      <c r="B268" s="1">
-        <v>3</v>
-      </c>
-      <c r="C268" s="1">
+      <c r="B268" s="0">
+        <v>3</v>
+      </c>
+      <c r="C268" s="0">
         <v>281.20727140397986</v>
       </c>
     </row>
@@ -3103,10 +3104,10 @@
       <c r="A269" t="s">
         <v>23</v>
       </c>
-      <c r="B269" s="1">
-        <v>4</v>
-      </c>
-      <c r="C269" s="1">
+      <c r="B269" s="0">
+        <v>4</v>
+      </c>
+      <c r="C269" s="0">
         <v>185.35208283420195</v>
       </c>
     </row>
@@ -3114,10 +3115,10 @@
       <c r="A270" t="s">
         <v>23</v>
       </c>
-      <c r="B270" s="1">
-        <v>5</v>
-      </c>
-      <c r="C270" s="1">
+      <c r="B270" s="0">
+        <v>5</v>
+      </c>
+      <c r="C270" s="0">
         <v>230.75636037309954</v>
       </c>
     </row>
@@ -3125,10 +3126,10 @@
       <c r="A271" t="s">
         <v>23</v>
       </c>
-      <c r="B271" s="1">
-        <v>6</v>
-      </c>
-      <c r="C271" s="1">
+      <c r="B271" s="0">
+        <v>6</v>
+      </c>
+      <c r="C271" s="0">
         <v>167.69786380940585</v>
       </c>
     </row>
@@ -3136,10 +3137,10 @@
       <c r="A272" t="s">
         <v>23</v>
       </c>
-      <c r="B272" s="1">
-        <v>7</v>
-      </c>
-      <c r="C272" s="1">
+      <c r="B272" s="0">
+        <v>7</v>
+      </c>
+      <c r="C272" s="0">
         <v>189.96193934251556</v>
       </c>
     </row>
@@ -3147,10 +3148,10 @@
       <c r="A273" t="s">
         <v>23</v>
       </c>
-      <c r="B273" s="1">
-        <v>8</v>
-      </c>
-      <c r="C273" s="1">
+      <c r="B273" s="0">
+        <v>8</v>
+      </c>
+      <c r="C273" s="0">
         <v>176.54884283733892</v>
       </c>
     </row>
@@ -3158,10 +3159,10 @@
       <c r="A274" t="s">
         <v>23</v>
       </c>
-      <c r="B274" s="1">
-        <v>9</v>
-      </c>
-      <c r="C274" s="1">
+      <c r="B274" s="0">
+        <v>9</v>
+      </c>
+      <c r="C274" s="0">
         <v>184.51675172929453</v>
       </c>
     </row>
@@ -3169,10 +3170,10 @@
       <c r="A275" t="s">
         <v>23</v>
       </c>
-      <c r="B275" s="1">
-        <v>10</v>
-      </c>
-      <c r="C275" s="1">
+      <c r="B275" s="0">
+        <v>10</v>
+      </c>
+      <c r="C275" s="0">
         <v>189.1247735854013</v>
       </c>
     </row>
@@ -3180,10 +3181,10 @@
       <c r="A276" t="s">
         <v>23</v>
       </c>
-      <c r="B276" s="1">
-        <v>11</v>
-      </c>
-      <c r="C276" s="1">
+      <c r="B276" s="0">
+        <v>11</v>
+      </c>
+      <c r="C276" s="0">
         <v>214.46165401121681</v>
       </c>
     </row>
@@ -3191,10 +3192,10 @@
       <c r="A277" t="s">
         <v>23</v>
       </c>
-      <c r="B277" s="1">
-        <v>12</v>
-      </c>
-      <c r="C277" s="1">
+      <c r="B277" s="0">
+        <v>12</v>
+      </c>
+      <c r="C277" s="0">
         <v>207.60650804572748</v>
       </c>
     </row>
@@ -3202,10 +3203,10 @@
       <c r="A278" t="s">
         <v>24</v>
       </c>
-      <c r="B278" s="1">
-        <v>1</v>
-      </c>
-      <c r="C278" s="1">
+      <c r="B278" s="0">
+        <v>1</v>
+      </c>
+      <c r="C278" s="0">
         <v>112.63905727443453</v>
       </c>
     </row>
@@ -3213,10 +3214,10 @@
       <c r="A279" t="s">
         <v>24</v>
       </c>
-      <c r="B279" s="1">
-        <v>2</v>
-      </c>
-      <c r="C279" s="1">
+      <c r="B279" s="0">
+        <v>2</v>
+      </c>
+      <c r="C279" s="0">
         <v>138.00994636357206</v>
       </c>
     </row>
@@ -3224,10 +3225,10 @@
       <c r="A280" t="s">
         <v>24</v>
       </c>
-      <c r="B280" s="1">
-        <v>3</v>
-      </c>
-      <c r="C280" s="1">
+      <c r="B280" s="0">
+        <v>3</v>
+      </c>
+      <c r="C280" s="0">
         <v>142.40594412833096</v>
       </c>
     </row>
@@ -3235,10 +3236,10 @@
       <c r="A281" t="s">
         <v>24</v>
       </c>
-      <c r="B281" s="1">
-        <v>4</v>
-      </c>
-      <c r="C281" s="1">
+      <c r="B281" s="0">
+        <v>4</v>
+      </c>
+      <c r="C281" s="0">
         <v>95.280677239972462</v>
       </c>
     </row>
@@ -3246,10 +3247,10 @@
       <c r="A282" t="s">
         <v>24</v>
       </c>
-      <c r="B282" s="1">
-        <v>5</v>
-      </c>
-      <c r="C282" s="1">
+      <c r="B282" s="0">
+        <v>5</v>
+      </c>
+      <c r="C282" s="0">
         <v>98.11193470584746</v>
       </c>
     </row>
@@ -3257,10 +3258,10 @@
       <c r="A283" t="s">
         <v>24</v>
       </c>
-      <c r="B283" s="1">
-        <v>6</v>
-      </c>
-      <c r="C283" s="1">
+      <c r="B283" s="0">
+        <v>6</v>
+      </c>
+      <c r="C283" s="0">
         <v>90.334937611228654</v>
       </c>
     </row>
@@ -3268,10 +3269,10 @@
       <c r="A284" t="s">
         <v>24</v>
       </c>
-      <c r="B284" s="1">
-        <v>7</v>
-      </c>
-      <c r="C284" s="1">
+      <c r="B284" s="0">
+        <v>7</v>
+      </c>
+      <c r="C284" s="0">
         <v>88.283767152168153</v>
       </c>
     </row>
@@ -3279,10 +3280,10 @@
       <c r="A285" t="s">
         <v>24</v>
       </c>
-      <c r="B285" s="1">
-        <v>8</v>
-      </c>
-      <c r="C285" s="1">
+      <c r="B285" s="0">
+        <v>8</v>
+      </c>
+      <c r="C285" s="0">
         <v>79.109103716265921</v>
       </c>
     </row>
@@ -3290,10 +3291,10 @@
       <c r="A286" t="s">
         <v>24</v>
       </c>
-      <c r="B286" s="1">
-        <v>9</v>
-      </c>
-      <c r="C286" s="1">
+      <c r="B286" s="0">
+        <v>9</v>
+      </c>
+      <c r="C286" s="0">
         <v>78.700928887261341</v>
       </c>
     </row>
@@ -3301,10 +3302,10 @@
       <c r="A287" t="s">
         <v>24</v>
       </c>
-      <c r="B287" s="1">
-        <v>10</v>
-      </c>
-      <c r="C287" s="1">
+      <c r="B287" s="0">
+        <v>10</v>
+      </c>
+      <c r="C287" s="0">
         <v>103.9897920730636</v>
       </c>
     </row>
@@ -3312,10 +3313,10 @@
       <c r="A288" t="s">
         <v>24</v>
       </c>
-      <c r="B288" s="1">
-        <v>11</v>
-      </c>
-      <c r="C288" s="1">
+      <c r="B288" s="0">
+        <v>11</v>
+      </c>
+      <c r="C288" s="0">
         <v>75.317495277532174</v>
       </c>
     </row>
@@ -3323,10 +3324,10 @@
       <c r="A289" t="s">
         <v>24</v>
       </c>
-      <c r="B289" s="1">
-        <v>12</v>
-      </c>
-      <c r="C289" s="1">
+      <c r="B289" s="0">
+        <v>12</v>
+      </c>
+      <c r="C289" s="0">
         <v>174.83133982207281</v>
       </c>
     </row>
@@ -3334,10 +3335,10 @@
       <c r="A290" t="s">
         <v>25</v>
       </c>
-      <c r="B290" s="1">
-        <v>1</v>
-      </c>
-      <c r="C290" s="1">
+      <c r="B290" s="0">
+        <v>1</v>
+      </c>
+      <c r="C290" s="0">
         <v>88.199173561725758</v>
       </c>
     </row>
@@ -3345,10 +3346,10 @@
       <c r="A291" t="s">
         <v>25</v>
       </c>
-      <c r="B291" s="1">
-        <v>2</v>
-      </c>
-      <c r="C291" s="1">
+      <c r="B291" s="0">
+        <v>2</v>
+      </c>
+      <c r="C291" s="0">
         <v>80.71515390083168</v>
       </c>
     </row>
@@ -3356,10 +3357,10 @@
       <c r="A292" t="s">
         <v>25</v>
       </c>
-      <c r="B292" s="1">
-        <v>3</v>
-      </c>
-      <c r="C292" s="1">
+      <c r="B292" s="0">
+        <v>3</v>
+      </c>
+      <c r="C292" s="0">
         <v>170.0450385906353</v>
       </c>
     </row>
@@ -3367,10 +3368,10 @@
       <c r="A293" t="s">
         <v>25</v>
       </c>
-      <c r="B293" s="1">
-        <v>4</v>
-      </c>
-      <c r="C293" s="1">
+      <c r="B293" s="0">
+        <v>4</v>
+      </c>
+      <c r="C293" s="0">
         <v>123.43514711846839</v>
       </c>
     </row>
@@ -3378,10 +3379,10 @@
       <c r="A294" t="s">
         <v>25</v>
       </c>
-      <c r="B294" s="1">
-        <v>5</v>
-      </c>
-      <c r="C294" s="1">
+      <c r="B294" s="0">
+        <v>5</v>
+      </c>
+      <c r="C294" s="0">
         <v>105.19512401227369</v>
       </c>
     </row>
@@ -3389,10 +3390,10 @@
       <c r="A295" t="s">
         <v>25</v>
       </c>
-      <c r="B295" s="1">
-        <v>6</v>
-      </c>
-      <c r="C295" s="1">
+      <c r="B295" s="0">
+        <v>6</v>
+      </c>
+      <c r="C295" s="0">
         <v>118.81205960472241</v>
       </c>
     </row>
@@ -3400,10 +3401,10 @@
       <c r="A296" t="s">
         <v>25</v>
       </c>
-      <c r="B296" s="1">
-        <v>7</v>
-      </c>
-      <c r="C296" s="1">
+      <c r="B296" s="0">
+        <v>7</v>
+      </c>
+      <c r="C296" s="0">
         <v>184.27249051796957</v>
       </c>
     </row>
@@ -3411,10 +3412,10 @@
       <c r="A297" t="s">
         <v>25</v>
       </c>
-      <c r="B297" s="1">
-        <v>8</v>
-      </c>
-      <c r="C297" s="1">
+      <c r="B297" s="0">
+        <v>8</v>
+      </c>
+      <c r="C297" s="0">
         <v>124.28907856525075</v>
       </c>
     </row>
@@ -3422,10 +3423,10 @@
       <c r="A298" t="s">
         <v>25</v>
       </c>
-      <c r="B298" s="1">
-        <v>9</v>
-      </c>
-      <c r="C298" s="1">
+      <c r="B298" s="0">
+        <v>9</v>
+      </c>
+      <c r="C298" s="0">
         <v>230.05940534595089</v>
       </c>
     </row>
@@ -3433,10 +3434,10 @@
       <c r="A299" t="s">
         <v>25</v>
       </c>
-      <c r="B299" s="1">
-        <v>10</v>
-      </c>
-      <c r="C299" s="1">
+      <c r="B299" s="0">
+        <v>10</v>
+      </c>
+      <c r="C299" s="0">
         <v>399.80611032798606</v>
       </c>
     </row>
@@ -3444,10 +3445,10 @@
       <c r="A300" t="s">
         <v>25</v>
       </c>
-      <c r="B300" s="1">
-        <v>11</v>
-      </c>
-      <c r="C300" s="1">
+      <c r="B300" s="0">
+        <v>11</v>
+      </c>
+      <c r="C300" s="0">
         <v>220.10555967592006</v>
       </c>
     </row>
@@ -3455,10 +3456,10 @@
       <c r="A301" t="s">
         <v>25</v>
       </c>
-      <c r="B301" s="1">
-        <v>12</v>
-      </c>
-      <c r="C301" s="1">
+      <c r="B301" s="0">
+        <v>12</v>
+      </c>
+      <c r="C301" s="0">
         <v>167.63100925224853</v>
       </c>
     </row>
@@ -3466,10 +3467,10 @@
       <c r="A302" t="s">
         <v>26</v>
       </c>
-      <c r="B302" s="1">
-        <v>1</v>
-      </c>
-      <c r="C302" s="1">
+      <c r="B302" s="0">
+        <v>1</v>
+      </c>
+      <c r="C302" s="0">
         <v>140.0670895461748</v>
       </c>
     </row>
@@ -3477,10 +3478,10 @@
       <c r="A303" t="s">
         <v>26</v>
       </c>
-      <c r="B303" s="1">
-        <v>2</v>
-      </c>
-      <c r="C303" s="1">
+      <c r="B303" s="0">
+        <v>2</v>
+      </c>
+      <c r="C303" s="0">
         <v>121.21055490453543</v>
       </c>
     </row>
@@ -3488,10 +3489,10 @@
       <c r="A304" t="s">
         <v>26</v>
       </c>
-      <c r="B304" s="1">
-        <v>3</v>
-      </c>
-      <c r="C304" s="1">
+      <c r="B304" s="0">
+        <v>3</v>
+      </c>
+      <c r="C304" s="0">
         <v>132.89491891792139</v>
       </c>
     </row>
@@ -3499,10 +3500,10 @@
       <c r="A305" t="s">
         <v>26</v>
       </c>
-      <c r="B305" s="1">
-        <v>4</v>
-      </c>
-      <c r="C305" s="1">
+      <c r="B305" s="0">
+        <v>4</v>
+      </c>
+      <c r="C305" s="0">
         <v>132.91662881882434</v>
       </c>
     </row>
@@ -3510,10 +3511,10 @@
       <c r="A306" t="s">
         <v>26</v>
       </c>
-      <c r="B306" s="1">
-        <v>5</v>
-      </c>
-      <c r="C306" s="1">
+      <c r="B306" s="0">
+        <v>5</v>
+      </c>
+      <c r="C306" s="0">
         <v>118.00192593722068</v>
       </c>
     </row>
@@ -3521,10 +3522,10 @@
       <c r="A307" t="s">
         <v>26</v>
       </c>
-      <c r="B307" s="1">
-        <v>6</v>
-      </c>
-      <c r="C307" s="1">
+      <c r="B307" s="0">
+        <v>6</v>
+      </c>
+      <c r="C307" s="0">
         <v>118.06162320279019</v>
       </c>
     </row>
@@ -3532,10 +3533,10 @@
       <c r="A308" t="s">
         <v>26</v>
       </c>
-      <c r="B308" s="1">
-        <v>7</v>
-      </c>
-      <c r="C308" s="1">
+      <c r="B308" s="0">
+        <v>7</v>
+      </c>
+      <c r="C308" s="0">
         <v>118.84758179507466</v>
       </c>
     </row>
@@ -3543,10 +3544,10 @@
       <c r="A309" t="s">
         <v>26</v>
       </c>
-      <c r="B309" s="1">
-        <v>8</v>
-      </c>
-      <c r="C309" s="1">
+      <c r="B309" s="0">
+        <v>8</v>
+      </c>
+      <c r="C309" s="0">
         <v>116.07590528763814</v>
       </c>
     </row>
@@ -3554,10 +3555,10 @@
       <c r="A310" t="s">
         <v>26</v>
       </c>
-      <c r="B310" s="1">
-        <v>9</v>
-      </c>
-      <c r="C310" s="1">
+      <c r="B310" s="0">
+        <v>9</v>
+      </c>
+      <c r="C310" s="0">
         <v>130.47644814461012</v>
       </c>
     </row>
@@ -3565,10 +3566,10 @@
       <c r="A311" t="s">
         <v>26</v>
       </c>
-      <c r="B311" s="1">
-        <v>10</v>
-      </c>
-      <c r="C311" s="1">
+      <c r="B311" s="0">
+        <v>10</v>
+      </c>
+      <c r="C311" s="0">
         <v>107.93382339762844</v>
       </c>
     </row>
@@ -3576,10 +3577,10 @@
       <c r="A312" t="s">
         <v>26</v>
       </c>
-      <c r="B312" s="1">
-        <v>11</v>
-      </c>
-      <c r="C312" s="1">
+      <c r="B312" s="0">
+        <v>11</v>
+      </c>
+      <c r="C312" s="0">
         <v>115.96201204487213</v>
       </c>
     </row>
@@ -3587,19 +3588,52 @@
       <c r="A313" t="s">
         <v>26</v>
       </c>
-      <c r="B313" s="1">
-        <v>12</v>
-      </c>
-      <c r="C313" s="1">
-        <v>110.99078432276089</v>
+      <c r="B313" s="0">
+        <v>12</v>
+      </c>
+      <c r="C313" s="0">
+        <v>120.8711830857322</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="s">
         <v>27</v>
       </c>
-      <c r="B314" s="1"/>
-      <c r="C314" s="1"/>
+      <c r="B314" s="0">
+        <v>1</v>
+      </c>
+      <c r="C314" s="0">
+        <v>100.6534474406542</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>27</v>
+      </c>
+      <c r="B315" s="0">
+        <v>2</v>
+      </c>
+      <c r="C315" s="0">
+        <v>114.04066891783862</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>27</v>
+      </c>
+      <c r="B316" s="0">
+        <v>3</v>
+      </c>
+      <c r="C316" s="0">
+        <v>140.90579974144353</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>28</v>
+      </c>
+      <c r="B317" s="0"/>
+      <c r="C317" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
update uk to 2024q2
</commit_message>
<xml_diff>
--- a/data-raw/uk/epu.xlsx
+++ b/data-raw/uk/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="31">
   <si>
     <t>year</t>
   </si>
@@ -149,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C317"/>
+  <dimension ref="A1:C320"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -3625,15 +3625,48 @@
         <v>3</v>
       </c>
       <c r="C316" s="0">
-        <v>140.90579974144353</v>
+        <v>135.56394811247927</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="s">
+        <v>27</v>
+      </c>
+      <c r="B317" s="0">
+        <v>4</v>
+      </c>
+      <c r="C317" s="0">
+        <v>102.66584709712725</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>27</v>
+      </c>
+      <c r="B318" s="0">
+        <v>5</v>
+      </c>
+      <c r="C318" s="0">
+        <v>144.78526009718755</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>27</v>
+      </c>
+      <c r="B319" s="0">
+        <v>6</v>
+      </c>
+      <c r="C319" s="0">
+        <v>147.84086669715819</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
         <v>28</v>
       </c>
-      <c r="B317" s="0"/>
-      <c r="C317" s="0"/>
+      <c r="B320" s="0"/>
+      <c r="C320" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
update to uk version 2024q3
</commit_message>
<xml_diff>
--- a/data-raw/uk/epu.xlsx
+++ b/data-raw/uk/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="31">
   <si>
     <t>year</t>
   </si>
@@ -149,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C320"/>
+  <dimension ref="A1:C326"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -3647,7 +3647,7 @@
         <v>5</v>
       </c>
       <c r="C318" s="0">
-        <v>144.78526009718755</v>
+        <v>144.78328886819094</v>
       </c>
     </row>
     <row r="319">
@@ -3658,15 +3658,81 @@
         <v>6</v>
       </c>
       <c r="C319" s="0">
-        <v>147.84086669715819</v>
+        <v>146.59757407655673</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="s">
+        <v>27</v>
+      </c>
+      <c r="B320" s="0">
+        <v>7</v>
+      </c>
+      <c r="C320" s="0">
+        <v>183.28213802345289</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>27</v>
+      </c>
+      <c r="B321" s="0">
+        <v>8</v>
+      </c>
+      <c r="C321" s="0">
+        <v>116.87180249328715</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>27</v>
+      </c>
+      <c r="B322" s="0">
+        <v>9</v>
+      </c>
+      <c r="C322" s="0">
+        <v>184.40996223935207</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>27</v>
+      </c>
+      <c r="B323" s="0">
+        <v>10</v>
+      </c>
+      <c r="C323" s="0">
+        <v>273.85700012719877</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>27</v>
+      </c>
+      <c r="B324" s="0">
+        <v>11</v>
+      </c>
+      <c r="C324" s="0">
+        <v>327.23352118076377</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>27</v>
+      </c>
+      <c r="B325" s="0">
+        <v>12</v>
+      </c>
+      <c r="C325" s="0">
+        <v>223.55022080880141</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
         <v>28</v>
       </c>
-      <c r="B320" s="0"/>
-      <c r="C320" s="0"/>
+      <c r="B326" s="0"/>
+      <c r="C326" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
update UK to 2024q4
</commit_message>
<xml_diff>
--- a/data-raw/uk/epu.xlsx
+++ b/data-raw/uk/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="32">
   <si>
     <t>year</t>
   </si>
@@ -99,6 +99,9 @@
     <t>2024</t>
   </si>
   <si>
+    <t>2025</t>
+  </si>
+  <si>
     <t>Source: 'Measuring Economic Policy Uncertainty' by Scott Baker, Nicholas Bloom and Steven J. Davis at www.PolicyUncertainty.com.  These data can be used freely with attribution to the authors, the paper, and the website.</t>
   </si>
   <si>
@@ -126,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,12 +137,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,7 +154,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C326"/>
+  <dimension ref="A1:C329"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -157,20 +162,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>114.23303041919498</v>
       </c>
     </row>
@@ -178,10 +183,10 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
         <v>71.152468112217733</v>
       </c>
     </row>
@@ -189,10 +194,10 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="0">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0">
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
         <v>148.08653465656573</v>
       </c>
     </row>
@@ -200,10 +205,10 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="0">
-        <v>4</v>
-      </c>
-      <c r="C5" s="0">
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
         <v>146.97678918911495</v>
       </c>
     </row>
@@ -211,10 +216,10 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="0">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0">
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
         <v>111.51501101796822</v>
       </c>
     </row>
@@ -222,10 +227,10 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="0">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0">
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
         <v>85.492917317480106</v>
       </c>
     </row>
@@ -233,10 +238,10 @@
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="0">
-        <v>7</v>
-      </c>
-      <c r="C8" s="0">
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
         <v>180.79302078297567</v>
       </c>
     </row>
@@ -244,10 +249,10 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="0">
-        <v>8</v>
-      </c>
-      <c r="C9" s="0">
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
         <v>140.59883854349383</v>
       </c>
     </row>
@@ -255,10 +260,10 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="0">
-        <v>9</v>
-      </c>
-      <c r="C10" s="0">
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
         <v>193.86284404128827</v>
       </c>
     </row>
@@ -266,10 +271,10 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="0">
-        <v>10</v>
-      </c>
-      <c r="C11" s="0">
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
         <v>256.06809124079552</v>
       </c>
     </row>
@@ -277,10 +282,10 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="0">
-        <v>11</v>
-      </c>
-      <c r="C12" s="0">
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
         <v>172.85871532726372</v>
       </c>
     </row>
@@ -288,10 +293,10 @@
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="0">
-        <v>12</v>
-      </c>
-      <c r="C13" s="0">
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
         <v>123.54462447386712</v>
       </c>
     </row>
@@ -299,10 +304,10 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="0">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
         <v>99.624838290417301</v>
       </c>
     </row>
@@ -310,10 +315,10 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="0">
-        <v>2</v>
-      </c>
-      <c r="C15" s="0">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
         <v>89.301390805313901</v>
       </c>
     </row>
@@ -321,10 +326,10 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="0">
-        <v>3</v>
-      </c>
-      <c r="C16" s="0">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
         <v>84.704431375507454</v>
       </c>
     </row>
@@ -332,10 +337,10 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="0">
-        <v>4</v>
-      </c>
-      <c r="C17" s="0">
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
         <v>63.930248201578557</v>
       </c>
     </row>
@@ -343,10 +348,10 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="0">
-        <v>5</v>
-      </c>
-      <c r="C18" s="0">
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
         <v>71.887983294516644</v>
       </c>
     </row>
@@ -354,10 +359,10 @@
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="0">
-        <v>6</v>
-      </c>
-      <c r="C19" s="0">
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
         <v>52.256729242724006</v>
       </c>
     </row>
@@ -365,10 +370,10 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="0">
-        <v>7</v>
-      </c>
-      <c r="C20" s="0">
+      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
         <v>81.232297333847839</v>
       </c>
     </row>
@@ -376,10 +381,10 @@
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="0">
-        <v>8</v>
-      </c>
-      <c r="C21" s="0">
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
         <v>72.576704428693134</v>
       </c>
     </row>
@@ -387,10 +392,10 @@
       <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="0">
-        <v>9</v>
-      </c>
-      <c r="C22" s="0">
+      <c r="B22" s="1">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1">
         <v>67.127564501344565</v>
       </c>
     </row>
@@ -398,10 +403,10 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="0">
-        <v>10</v>
-      </c>
-      <c r="C23" s="0">
+      <c r="B23" s="1">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1">
         <v>123.12413166974538</v>
       </c>
     </row>
@@ -409,10 +414,10 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="0">
-        <v>11</v>
-      </c>
-      <c r="C24" s="0">
+      <c r="B24" s="1">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1">
         <v>26.84680026099262</v>
       </c>
     </row>
@@ -420,10 +425,10 @@
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="0">
-        <v>12</v>
-      </c>
-      <c r="C25" s="0">
+      <c r="B25" s="1">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1">
         <v>48.689985458213094</v>
       </c>
     </row>
@@ -431,10 +436,10 @@
       <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="0">
-        <v>1</v>
-      </c>
-      <c r="C26" s="0">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
         <v>53.748451022419943</v>
       </c>
     </row>
@@ -442,10 +447,10 @@
       <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="0">
-        <v>2</v>
-      </c>
-      <c r="C27" s="0">
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
         <v>58.396510954430312</v>
       </c>
     </row>
@@ -453,10 +458,10 @@
       <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="0">
-        <v>3</v>
-      </c>
-      <c r="C28" s="0">
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
         <v>61.960392681100373</v>
       </c>
     </row>
@@ -464,10 +469,10 @@
       <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="0">
-        <v>4</v>
-      </c>
-      <c r="C29" s="0">
+      <c r="B29" s="1">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
         <v>114.01042927352911</v>
       </c>
     </row>
@@ -475,10 +480,10 @@
       <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="0">
-        <v>5</v>
-      </c>
-      <c r="C30" s="0">
+      <c r="B30" s="1">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1">
         <v>46.368325435466247</v>
       </c>
     </row>
@@ -486,10 +491,10 @@
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="0">
-        <v>6</v>
-      </c>
-      <c r="C31" s="0">
+      <c r="B31" s="1">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1">
         <v>133.21640062369883</v>
       </c>
     </row>
@@ -497,10 +502,10 @@
       <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="0">
-        <v>7</v>
-      </c>
-      <c r="C32" s="0">
+      <c r="B32" s="1">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1">
         <v>73.706699857582223</v>
       </c>
     </row>
@@ -508,10 +513,10 @@
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="0">
-        <v>8</v>
-      </c>
-      <c r="C33" s="0">
+      <c r="B33" s="1">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
         <v>42.748375788974677</v>
       </c>
     </row>
@@ -519,10 +524,10 @@
       <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="0">
-        <v>9</v>
-      </c>
-      <c r="C34" s="0">
+      <c r="B34" s="1">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1">
         <v>55.577872298404039</v>
       </c>
     </row>
@@ -530,10 +535,10 @@
       <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="0">
-        <v>10</v>
-      </c>
-      <c r="C35" s="0">
+      <c r="B35" s="1">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1">
         <v>55.821764612416644</v>
       </c>
     </row>
@@ -541,10 +546,10 @@
       <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="0">
-        <v>11</v>
-      </c>
-      <c r="C36" s="0">
+      <c r="B36" s="1">
+        <v>11</v>
+      </c>
+      <c r="C36" s="1">
         <v>68.991031741151005</v>
       </c>
     </row>
@@ -552,10 +557,10 @@
       <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="0">
-        <v>12</v>
-      </c>
-      <c r="C37" s="0">
+      <c r="B37" s="1">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1">
         <v>66.450174706116044</v>
       </c>
     </row>
@@ -563,10 +568,10 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="0">
-        <v>1</v>
-      </c>
-      <c r="C38" s="0">
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
         <v>38.407833958642684</v>
       </c>
     </row>
@@ -574,10 +579,10 @@
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="0">
-        <v>2</v>
-      </c>
-      <c r="C39" s="0">
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1">
         <v>56.693271350649312</v>
       </c>
     </row>
@@ -585,10 +590,10 @@
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="0">
-        <v>3</v>
-      </c>
-      <c r="C40" s="0">
+      <c r="B40" s="1">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1">
         <v>91.642864752455026</v>
       </c>
     </row>
@@ -596,10 +601,10 @@
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="0">
-        <v>4</v>
-      </c>
-      <c r="C41" s="0">
+      <c r="B41" s="1">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1">
         <v>100.98927389864957</v>
       </c>
     </row>
@@ -607,10 +612,10 @@
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="0">
-        <v>5</v>
-      </c>
-      <c r="C42" s="0">
+      <c r="B42" s="1">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1">
         <v>98.256230864099578</v>
       </c>
     </row>
@@ -618,10 +623,10 @@
       <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="0">
-        <v>6</v>
-      </c>
-      <c r="C43" s="0">
+      <c r="B43" s="1">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1">
         <v>74.842735742282386</v>
       </c>
     </row>
@@ -629,10 +634,10 @@
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="0">
-        <v>7</v>
-      </c>
-      <c r="C44" s="0">
+      <c r="B44" s="1">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1">
         <v>66.38372519061484</v>
       </c>
     </row>
@@ -640,10 +645,10 @@
       <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="0">
-        <v>8</v>
-      </c>
-      <c r="C45" s="0">
+      <c r="B45" s="1">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1">
         <v>105.13269947080015</v>
       </c>
     </row>
@@ -651,10 +656,10 @@
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="0">
-        <v>9</v>
-      </c>
-      <c r="C46" s="0">
+      <c r="B46" s="1">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1">
         <v>205.25697487631768</v>
       </c>
     </row>
@@ -662,10 +667,10 @@
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="0">
-        <v>10</v>
-      </c>
-      <c r="C47" s="0">
+      <c r="B47" s="1">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1">
         <v>158.72159980318426</v>
       </c>
     </row>
@@ -673,10 +678,10 @@
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="0">
-        <v>11</v>
-      </c>
-      <c r="C48" s="0">
+      <c r="B48" s="1">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1">
         <v>146.11531254475</v>
       </c>
     </row>
@@ -684,10 +689,10 @@
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="0">
-        <v>12</v>
-      </c>
-      <c r="C49" s="0">
+      <c r="B49" s="1">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1">
         <v>108.11412471348061</v>
       </c>
     </row>
@@ -695,10 +700,10 @@
       <c r="A50" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="0">
-        <v>1</v>
-      </c>
-      <c r="C50" s="0">
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1">
         <v>85.506579174754521</v>
       </c>
     </row>
@@ -706,10 +711,10 @@
       <c r="A51" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="0">
-        <v>2</v>
-      </c>
-      <c r="C51" s="0">
+      <c r="B51" s="1">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1">
         <v>70.793482785977702</v>
       </c>
     </row>
@@ -717,10 +722,10 @@
       <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="0">
-        <v>3</v>
-      </c>
-      <c r="C52" s="0">
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1">
         <v>76.328319642242249</v>
       </c>
     </row>
@@ -728,10 +733,10 @@
       <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="0">
-        <v>4</v>
-      </c>
-      <c r="C53" s="0">
+      <c r="B53" s="1">
+        <v>4</v>
+      </c>
+      <c r="C53" s="1">
         <v>78.088182950900872</v>
       </c>
     </row>
@@ -739,10 +744,10 @@
       <c r="A54" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="0">
-        <v>5</v>
-      </c>
-      <c r="C54" s="0">
+      <c r="B54" s="1">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1">
         <v>67.406353692455028</v>
       </c>
     </row>
@@ -750,10 +755,10 @@
       <c r="A55" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="0">
-        <v>6</v>
-      </c>
-      <c r="C55" s="0">
+      <c r="B55" s="1">
+        <v>6</v>
+      </c>
+      <c r="C55" s="1">
         <v>86.879203610639379</v>
       </c>
     </row>
@@ -761,10 +766,10 @@
       <c r="A56" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="0">
-        <v>7</v>
-      </c>
-      <c r="C56" s="0">
+      <c r="B56" s="1">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1">
         <v>88.472571429943144</v>
       </c>
     </row>
@@ -772,10 +777,10 @@
       <c r="A57" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="0">
-        <v>8</v>
-      </c>
-      <c r="C57" s="0">
+      <c r="B57" s="1">
+        <v>8</v>
+      </c>
+      <c r="C57" s="1">
         <v>93.723994884644043</v>
       </c>
     </row>
@@ -783,10 +788,10 @@
       <c r="A58" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="0">
-        <v>9</v>
-      </c>
-      <c r="C58" s="0">
+      <c r="B58" s="1">
+        <v>9</v>
+      </c>
+      <c r="C58" s="1">
         <v>127.27273057482194</v>
       </c>
     </row>
@@ -794,10 +799,10 @@
       <c r="A59" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="0">
-        <v>10</v>
-      </c>
-      <c r="C59" s="0">
+      <c r="B59" s="1">
+        <v>10</v>
+      </c>
+      <c r="C59" s="1">
         <v>108.4297542573948</v>
       </c>
     </row>
@@ -805,10 +810,10 @@
       <c r="A60" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="0">
-        <v>11</v>
-      </c>
-      <c r="C60" s="0">
+      <c r="B60" s="1">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1">
         <v>115.09958348207847</v>
       </c>
     </row>
@@ -816,10 +821,10 @@
       <c r="A61" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="0">
-        <v>12</v>
-      </c>
-      <c r="C61" s="0">
+      <c r="B61" s="1">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1">
         <v>118.64259248874143</v>
       </c>
     </row>
@@ -827,10 +832,10 @@
       <c r="A62" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="0">
-        <v>1</v>
-      </c>
-      <c r="C62" s="0">
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1">
         <v>146.05941292203249</v>
       </c>
     </row>
@@ -838,10 +843,10 @@
       <c r="A63" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="0">
-        <v>2</v>
-      </c>
-      <c r="C63" s="0">
+      <c r="B63" s="1">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1">
         <v>178.73887349178023</v>
       </c>
     </row>
@@ -849,10 +854,10 @@
       <c r="A64" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="0">
-        <v>3</v>
-      </c>
-      <c r="C64" s="0">
+      <c r="B64" s="1">
+        <v>3</v>
+      </c>
+      <c r="C64" s="1">
         <v>174.97273471435085</v>
       </c>
     </row>
@@ -860,10 +865,10 @@
       <c r="A65" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="0">
-        <v>4</v>
-      </c>
-      <c r="C65" s="0">
+      <c r="B65" s="1">
+        <v>4</v>
+      </c>
+      <c r="C65" s="1">
         <v>153.50644782837878</v>
       </c>
     </row>
@@ -871,10 +876,10 @@
       <c r="A66" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="0">
-        <v>5</v>
-      </c>
-      <c r="C66" s="0">
+      <c r="B66" s="1">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1">
         <v>93.713759198405427</v>
       </c>
     </row>
@@ -882,10 +887,10 @@
       <c r="A67" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="0">
-        <v>6</v>
-      </c>
-      <c r="C67" s="0">
+      <c r="B67" s="1">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1">
         <v>125.00647484433625</v>
       </c>
     </row>
@@ -893,10 +898,10 @@
       <c r="A68" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="0">
-        <v>7</v>
-      </c>
-      <c r="C68" s="0">
+      <c r="B68" s="1">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1">
         <v>80.936638413478462</v>
       </c>
     </row>
@@ -904,10 +909,10 @@
       <c r="A69" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="0">
-        <v>8</v>
-      </c>
-      <c r="C69" s="0">
+      <c r="B69" s="1">
+        <v>8</v>
+      </c>
+      <c r="C69" s="1">
         <v>83.362627004704052</v>
       </c>
     </row>
@@ -915,10 +920,10 @@
       <c r="A70" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="0">
-        <v>9</v>
-      </c>
-      <c r="C70" s="0">
+      <c r="B70" s="1">
+        <v>9</v>
+      </c>
+      <c r="C70" s="1">
         <v>65.412854559766302</v>
       </c>
     </row>
@@ -926,10 +931,10 @@
       <c r="A71" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="0">
-        <v>10</v>
-      </c>
-      <c r="C71" s="0">
+      <c r="B71" s="1">
+        <v>10</v>
+      </c>
+      <c r="C71" s="1">
         <v>62.298289449657176</v>
       </c>
     </row>
@@ -937,10 +942,10 @@
       <c r="A72" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="0">
-        <v>11</v>
-      </c>
-      <c r="C72" s="0">
+      <c r="B72" s="1">
+        <v>11</v>
+      </c>
+      <c r="C72" s="1">
         <v>78.4478801122807</v>
       </c>
     </row>
@@ -948,10 +953,10 @@
       <c r="A73" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="0">
-        <v>12</v>
-      </c>
-      <c r="C73" s="0">
+      <c r="B73" s="1">
+        <v>12</v>
+      </c>
+      <c r="C73" s="1">
         <v>46.291193655705612</v>
       </c>
     </row>
@@ -959,10 +964,10 @@
       <c r="A74" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="0">
-        <v>1</v>
-      </c>
-      <c r="C74" s="0">
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1">
         <v>24.0359419445406</v>
       </c>
     </row>
@@ -970,10 +975,10 @@
       <c r="A75" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="0">
-        <v>2</v>
-      </c>
-      <c r="C75" s="0">
+      <c r="B75" s="1">
+        <v>2</v>
+      </c>
+      <c r="C75" s="1">
         <v>57.130154355236499</v>
       </c>
     </row>
@@ -981,10 +986,10 @@
       <c r="A76" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="0">
-        <v>3</v>
-      </c>
-      <c r="C76" s="0">
+      <c r="B76" s="1">
+        <v>3</v>
+      </c>
+      <c r="C76" s="1">
         <v>61.884703940211296</v>
       </c>
     </row>
@@ -992,10 +997,10 @@
       <c r="A77" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="0">
-        <v>4</v>
-      </c>
-      <c r="C77" s="0">
+      <c r="B77" s="1">
+        <v>4</v>
+      </c>
+      <c r="C77" s="1">
         <v>38.552354422083354</v>
       </c>
     </row>
@@ -1003,10 +1008,10 @@
       <c r="A78" t="s">
         <v>7</v>
       </c>
-      <c r="B78" s="0">
-        <v>5</v>
-      </c>
-      <c r="C78" s="0">
+      <c r="B78" s="1">
+        <v>5</v>
+      </c>
+      <c r="C78" s="1">
         <v>42.88216533306619</v>
       </c>
     </row>
@@ -1014,10 +1019,10 @@
       <c r="A79" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="0">
-        <v>6</v>
-      </c>
-      <c r="C79" s="0">
+      <c r="B79" s="1">
+        <v>6</v>
+      </c>
+      <c r="C79" s="1">
         <v>49.439137156664231</v>
       </c>
     </row>
@@ -1025,10 +1030,10 @@
       <c r="A80" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="0">
-        <v>7</v>
-      </c>
-      <c r="C80" s="0">
+      <c r="B80" s="1">
+        <v>7</v>
+      </c>
+      <c r="C80" s="1">
         <v>52.617274390594723</v>
       </c>
     </row>
@@ -1036,10 +1041,10 @@
       <c r="A81" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="0">
-        <v>8</v>
-      </c>
-      <c r="C81" s="0">
+      <c r="B81" s="1">
+        <v>8</v>
+      </c>
+      <c r="C81" s="1">
         <v>39.393721041190858</v>
       </c>
     </row>
@@ -1047,10 +1052,10 @@
       <c r="A82" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="0">
-        <v>9</v>
-      </c>
-      <c r="C82" s="0">
+      <c r="B82" s="1">
+        <v>9</v>
+      </c>
+      <c r="C82" s="1">
         <v>49.166223902677764</v>
       </c>
     </row>
@@ -1058,10 +1063,10 @@
       <c r="A83" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="0">
-        <v>10</v>
-      </c>
-      <c r="C83" s="0">
+      <c r="B83" s="1">
+        <v>10</v>
+      </c>
+      <c r="C83" s="1">
         <v>67.129160866436038</v>
       </c>
     </row>
@@ -1069,10 +1074,10 @@
       <c r="A84" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="0">
-        <v>11</v>
-      </c>
-      <c r="C84" s="0">
+      <c r="B84" s="1">
+        <v>11</v>
+      </c>
+      <c r="C84" s="1">
         <v>68.726025959774617</v>
       </c>
     </row>
@@ -1080,10 +1085,10 @@
       <c r="A85" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="0">
-        <v>12</v>
-      </c>
-      <c r="C85" s="0">
+      <c r="B85" s="1">
+        <v>12</v>
+      </c>
+      <c r="C85" s="1">
         <v>44.909516282941226</v>
       </c>
     </row>
@@ -1091,10 +1096,10 @@
       <c r="A86" t="s">
         <v>8</v>
       </c>
-      <c r="B86" s="0">
-        <v>1</v>
-      </c>
-      <c r="C86" s="0">
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1">
         <v>43.989646993249359</v>
       </c>
     </row>
@@ -1102,10 +1107,10 @@
       <c r="A87" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="0">
-        <v>2</v>
-      </c>
-      <c r="C87" s="0">
+      <c r="B87" s="1">
+        <v>2</v>
+      </c>
+      <c r="C87" s="1">
         <v>39.64534947881436</v>
       </c>
     </row>
@@ -1113,10 +1118,10 @@
       <c r="A88" t="s">
         <v>8</v>
       </c>
-      <c r="B88" s="0">
-        <v>3</v>
-      </c>
-      <c r="C88" s="0">
+      <c r="B88" s="1">
+        <v>3</v>
+      </c>
+      <c r="C88" s="1">
         <v>34.07870982308976</v>
       </c>
     </row>
@@ -1124,10 +1129,10 @@
       <c r="A89" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="0">
-        <v>4</v>
-      </c>
-      <c r="C89" s="0">
+      <c r="B89" s="1">
+        <v>4</v>
+      </c>
+      <c r="C89" s="1">
         <v>69.057126421663469</v>
       </c>
     </row>
@@ -1135,10 +1140,10 @@
       <c r="A90" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="0">
-        <v>5</v>
-      </c>
-      <c r="C90" s="0">
+      <c r="B90" s="1">
+        <v>5</v>
+      </c>
+      <c r="C90" s="1">
         <v>71.771089573397958</v>
       </c>
     </row>
@@ -1146,10 +1151,10 @@
       <c r="A91" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="0">
-        <v>6</v>
-      </c>
-      <c r="C91" s="0">
+      <c r="B91" s="1">
+        <v>6</v>
+      </c>
+      <c r="C91" s="1">
         <v>59.403874719354278</v>
       </c>
     </row>
@@ -1157,10 +1162,10 @@
       <c r="A92" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="0">
-        <v>7</v>
-      </c>
-      <c r="C92" s="0">
+      <c r="B92" s="1">
+        <v>7</v>
+      </c>
+      <c r="C92" s="1">
         <v>47.414013411934278</v>
       </c>
     </row>
@@ -1168,10 +1173,10 @@
       <c r="A93" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="0">
-        <v>8</v>
-      </c>
-      <c r="C93" s="0">
+      <c r="B93" s="1">
+        <v>8</v>
+      </c>
+      <c r="C93" s="1">
         <v>48.54170562625211</v>
       </c>
     </row>
@@ -1179,10 +1184,10 @@
       <c r="A94" t="s">
         <v>8</v>
       </c>
-      <c r="B94" s="0">
-        <v>9</v>
-      </c>
-      <c r="C94" s="0">
+      <c r="B94" s="1">
+        <v>9</v>
+      </c>
+      <c r="C94" s="1">
         <v>70.332476662916861</v>
       </c>
     </row>
@@ -1190,10 +1195,10 @@
       <c r="A95" t="s">
         <v>8</v>
       </c>
-      <c r="B95" s="0">
-        <v>10</v>
-      </c>
-      <c r="C95" s="0">
+      <c r="B95" s="1">
+        <v>10</v>
+      </c>
+      <c r="C95" s="1">
         <v>40.613034313794714</v>
       </c>
     </row>
@@ -1201,10 +1206,10 @@
       <c r="A96" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="0">
-        <v>11</v>
-      </c>
-      <c r="C96" s="0">
+      <c r="B96" s="1">
+        <v>11</v>
+      </c>
+      <c r="C96" s="1">
         <v>47.559237062280005</v>
       </c>
     </row>
@@ -1212,10 +1217,10 @@
       <c r="A97" t="s">
         <v>8</v>
       </c>
-      <c r="B97" s="0">
-        <v>12</v>
-      </c>
-      <c r="C97" s="0">
+      <c r="B97" s="1">
+        <v>12</v>
+      </c>
+      <c r="C97" s="1">
         <v>33.10658195369718</v>
       </c>
     </row>
@@ -1223,10 +1228,10 @@
       <c r="A98" t="s">
         <v>9</v>
       </c>
-      <c r="B98" s="0">
-        <v>1</v>
-      </c>
-      <c r="C98" s="0">
+      <c r="B98" s="1">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1">
         <v>44.040050065155981</v>
       </c>
     </row>
@@ -1234,10 +1239,10 @@
       <c r="A99" t="s">
         <v>9</v>
       </c>
-      <c r="B99" s="0">
-        <v>2</v>
-      </c>
-      <c r="C99" s="0">
+      <c r="B99" s="1">
+        <v>2</v>
+      </c>
+      <c r="C99" s="1">
         <v>37.132061545598454</v>
       </c>
     </row>
@@ -1245,10 +1250,10 @@
       <c r="A100" t="s">
         <v>9</v>
       </c>
-      <c r="B100" s="0">
-        <v>3</v>
-      </c>
-      <c r="C100" s="0">
+      <c r="B100" s="1">
+        <v>3</v>
+      </c>
+      <c r="C100" s="1">
         <v>42.456446706105879</v>
       </c>
     </row>
@@ -1256,10 +1261,10 @@
       <c r="A101" t="s">
         <v>9</v>
       </c>
-      <c r="B101" s="0">
-        <v>4</v>
-      </c>
-      <c r="C101" s="0">
+      <c r="B101" s="1">
+        <v>4</v>
+      </c>
+      <c r="C101" s="1">
         <v>37.086608110653827</v>
       </c>
     </row>
@@ -1267,10 +1272,10 @@
       <c r="A102" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="0">
-        <v>5</v>
-      </c>
-      <c r="C102" s="0">
+      <c r="B102" s="1">
+        <v>5</v>
+      </c>
+      <c r="C102" s="1">
         <v>74.022673592114302</v>
       </c>
     </row>
@@ -1278,10 +1283,10 @@
       <c r="A103" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="0">
-        <v>6</v>
-      </c>
-      <c r="C103" s="0">
+      <c r="B103" s="1">
+        <v>6</v>
+      </c>
+      <c r="C103" s="1">
         <v>59.820568976535263</v>
       </c>
     </row>
@@ -1289,10 +1294,10 @@
       <c r="A104" t="s">
         <v>9</v>
       </c>
-      <c r="B104" s="0">
-        <v>7</v>
-      </c>
-      <c r="C104" s="0">
+      <c r="B104" s="1">
+        <v>7</v>
+      </c>
+      <c r="C104" s="1">
         <v>47.543782394855668</v>
       </c>
     </row>
@@ -1300,10 +1305,10 @@
       <c r="A105" t="s">
         <v>9</v>
       </c>
-      <c r="B105" s="0">
-        <v>8</v>
-      </c>
-      <c r="C105" s="0">
+      <c r="B105" s="1">
+        <v>8</v>
+      </c>
+      <c r="C105" s="1">
         <v>67.213228709248042</v>
       </c>
     </row>
@@ -1311,10 +1316,10 @@
       <c r="A106" t="s">
         <v>9</v>
       </c>
-      <c r="B106" s="0">
-        <v>9</v>
-      </c>
-      <c r="C106" s="0">
+      <c r="B106" s="1">
+        <v>9</v>
+      </c>
+      <c r="C106" s="1">
         <v>56.234482774648797</v>
       </c>
     </row>
@@ -1322,10 +1327,10 @@
       <c r="A107" t="s">
         <v>9</v>
       </c>
-      <c r="B107" s="0">
-        <v>10</v>
-      </c>
-      <c r="C107" s="0">
+      <c r="B107" s="1">
+        <v>10</v>
+      </c>
+      <c r="C107" s="1">
         <v>65.255080007947058</v>
       </c>
     </row>
@@ -1333,10 +1338,10 @@
       <c r="A108" t="s">
         <v>9</v>
       </c>
-      <c r="B108" s="0">
-        <v>11</v>
-      </c>
-      <c r="C108" s="0">
+      <c r="B108" s="1">
+        <v>11</v>
+      </c>
+      <c r="C108" s="1">
         <v>59.49058917096486</v>
       </c>
     </row>
@@ -1344,10 +1349,10 @@
       <c r="A109" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="0">
-        <v>12</v>
-      </c>
-      <c r="C109" s="0">
+      <c r="B109" s="1">
+        <v>12</v>
+      </c>
+      <c r="C109" s="1">
         <v>64.488699636232127</v>
       </c>
     </row>
@@ -1355,10 +1360,10 @@
       <c r="A110" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="0">
-        <v>1</v>
-      </c>
-      <c r="C110" s="0">
+      <c r="B110" s="1">
+        <v>1</v>
+      </c>
+      <c r="C110" s="1">
         <v>49.232184122049397</v>
       </c>
     </row>
@@ -1366,10 +1371,10 @@
       <c r="A111" t="s">
         <v>10</v>
       </c>
-      <c r="B111" s="0">
-        <v>2</v>
-      </c>
-      <c r="C111" s="0">
+      <c r="B111" s="1">
+        <v>2</v>
+      </c>
+      <c r="C111" s="1">
         <v>53.071933804627889</v>
       </c>
     </row>
@@ -1377,10 +1382,10 @@
       <c r="A112" t="s">
         <v>10</v>
       </c>
-      <c r="B112" s="0">
-        <v>3</v>
-      </c>
-      <c r="C112" s="0">
+      <c r="B112" s="1">
+        <v>3</v>
+      </c>
+      <c r="C112" s="1">
         <v>77.055227733903877</v>
       </c>
     </row>
@@ -1388,10 +1393,10 @@
       <c r="A113" t="s">
         <v>10</v>
       </c>
-      <c r="B113" s="0">
-        <v>4</v>
-      </c>
-      <c r="C113" s="0">
+      <c r="B113" s="1">
+        <v>4</v>
+      </c>
+      <c r="C113" s="1">
         <v>60.964843473864342</v>
       </c>
     </row>
@@ -1399,10 +1404,10 @@
       <c r="A114" t="s">
         <v>10</v>
       </c>
-      <c r="B114" s="0">
-        <v>5</v>
-      </c>
-      <c r="C114" s="0">
+      <c r="B114" s="1">
+        <v>5</v>
+      </c>
+      <c r="C114" s="1">
         <v>66.573947273860682</v>
       </c>
     </row>
@@ -1410,10 +1415,10 @@
       <c r="A115" t="s">
         <v>10</v>
       </c>
-      <c r="B115" s="0">
-        <v>6</v>
-      </c>
-      <c r="C115" s="0">
+      <c r="B115" s="1">
+        <v>6</v>
+      </c>
+      <c r="C115" s="1">
         <v>53.468607020779125</v>
       </c>
     </row>
@@ -1421,10 +1426,10 @@
       <c r="A116" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="0">
-        <v>7</v>
-      </c>
-      <c r="C116" s="0">
+      <c r="B116" s="1">
+        <v>7</v>
+      </c>
+      <c r="C116" s="1">
         <v>48.757679221451504</v>
       </c>
     </row>
@@ -1432,10 +1437,10 @@
       <c r="A117" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="0">
-        <v>8</v>
-      </c>
-      <c r="C117" s="0">
+      <c r="B117" s="1">
+        <v>8</v>
+      </c>
+      <c r="C117" s="1">
         <v>77.388682544021719</v>
       </c>
     </row>
@@ -1443,10 +1448,10 @@
       <c r="A118" t="s">
         <v>10</v>
       </c>
-      <c r="B118" s="0">
-        <v>9</v>
-      </c>
-      <c r="C118" s="0">
+      <c r="B118" s="1">
+        <v>9</v>
+      </c>
+      <c r="C118" s="1">
         <v>132.26575539424326</v>
       </c>
     </row>
@@ -1454,10 +1459,10 @@
       <c r="A119" t="s">
         <v>10</v>
       </c>
-      <c r="B119" s="0">
-        <v>10</v>
-      </c>
-      <c r="C119" s="0">
+      <c r="B119" s="1">
+        <v>10</v>
+      </c>
+      <c r="C119" s="1">
         <v>91.692920345072537</v>
       </c>
     </row>
@@ -1465,10 +1470,10 @@
       <c r="A120" t="s">
         <v>10</v>
       </c>
-      <c r="B120" s="0">
-        <v>11</v>
-      </c>
-      <c r="C120" s="0">
+      <c r="B120" s="1">
+        <v>11</v>
+      </c>
+      <c r="C120" s="1">
         <v>131.62321770144564</v>
       </c>
     </row>
@@ -1476,10 +1481,10 @@
       <c r="A121" t="s">
         <v>10</v>
       </c>
-      <c r="B121" s="0">
-        <v>12</v>
-      </c>
-      <c r="C121" s="0">
+      <c r="B121" s="1">
+        <v>12</v>
+      </c>
+      <c r="C121" s="1">
         <v>150.8732135162181</v>
       </c>
     </row>
@@ -1487,10 +1492,10 @@
       <c r="A122" t="s">
         <v>11</v>
       </c>
-      <c r="B122" s="0">
-        <v>1</v>
-      </c>
-      <c r="C122" s="0">
+      <c r="B122" s="1">
+        <v>1</v>
+      </c>
+      <c r="C122" s="1">
         <v>138.57289473235426</v>
       </c>
     </row>
@@ -1498,10 +1503,10 @@
       <c r="A123" t="s">
         <v>11</v>
       </c>
-      <c r="B123" s="0">
-        <v>2</v>
-      </c>
-      <c r="C123" s="0">
+      <c r="B123" s="1">
+        <v>2</v>
+      </c>
+      <c r="C123" s="1">
         <v>145.78488588875288</v>
       </c>
     </row>
@@ -1509,10 +1514,10 @@
       <c r="A124" t="s">
         <v>11</v>
       </c>
-      <c r="B124" s="0">
-        <v>3</v>
-      </c>
-      <c r="C124" s="0">
+      <c r="B124" s="1">
+        <v>3</v>
+      </c>
+      <c r="C124" s="1">
         <v>168.74941890266629</v>
       </c>
     </row>
@@ -1520,10 +1525,10 @@
       <c r="A125" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="0">
-        <v>4</v>
-      </c>
-      <c r="C125" s="0">
+      <c r="B125" s="1">
+        <v>4</v>
+      </c>
+      <c r="C125" s="1">
         <v>129.51088529834928</v>
       </c>
     </row>
@@ -1531,10 +1536,10 @@
       <c r="A126" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="0">
-        <v>5</v>
-      </c>
-      <c r="C126" s="0">
+      <c r="B126" s="1">
+        <v>5</v>
+      </c>
+      <c r="C126" s="1">
         <v>112.51807597636849</v>
       </c>
     </row>
@@ -1542,10 +1547,10 @@
       <c r="A127" t="s">
         <v>11</v>
       </c>
-      <c r="B127" s="0">
-        <v>6</v>
-      </c>
-      <c r="C127" s="0">
+      <c r="B127" s="1">
+        <v>6</v>
+      </c>
+      <c r="C127" s="1">
         <v>107.00998790223383</v>
       </c>
     </row>
@@ -1553,10 +1558,10 @@
       <c r="A128" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="0">
-        <v>7</v>
-      </c>
-      <c r="C128" s="0">
+      <c r="B128" s="1">
+        <v>7</v>
+      </c>
+      <c r="C128" s="1">
         <v>113.38642811958277</v>
       </c>
     </row>
@@ -1564,10 +1569,10 @@
       <c r="A129" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="0">
-        <v>8</v>
-      </c>
-      <c r="C129" s="0">
+      <c r="B129" s="1">
+        <v>8</v>
+      </c>
+      <c r="C129" s="1">
         <v>143.64464702090251</v>
       </c>
     </row>
@@ -1575,10 +1580,10 @@
       <c r="A130" t="s">
         <v>11</v>
       </c>
-      <c r="B130" s="0">
-        <v>9</v>
-      </c>
-      <c r="C130" s="0">
+      <c r="B130" s="1">
+        <v>9</v>
+      </c>
+      <c r="C130" s="1">
         <v>191.05963498096241</v>
       </c>
     </row>
@@ -1586,10 +1591,10 @@
       <c r="A131" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="0">
-        <v>10</v>
-      </c>
-      <c r="C131" s="0">
+      <c r="B131" s="1">
+        <v>10</v>
+      </c>
+      <c r="C131" s="1">
         <v>242.23438012932465</v>
       </c>
     </row>
@@ -1597,10 +1602,10 @@
       <c r="A132" t="s">
         <v>11</v>
       </c>
-      <c r="B132" s="0">
-        <v>11</v>
-      </c>
-      <c r="C132" s="0">
+      <c r="B132" s="1">
+        <v>11</v>
+      </c>
+      <c r="C132" s="1">
         <v>169.54905468701816</v>
       </c>
     </row>
@@ -1608,10 +1613,10 @@
       <c r="A133" t="s">
         <v>11</v>
       </c>
-      <c r="B133" s="0">
-        <v>12</v>
-      </c>
-      <c r="C133" s="0">
+      <c r="B133" s="1">
+        <v>12</v>
+      </c>
+      <c r="C133" s="1">
         <v>123.49229337979028</v>
       </c>
     </row>
@@ -1619,10 +1624,10 @@
       <c r="A134" t="s">
         <v>12</v>
       </c>
-      <c r="B134" s="0">
-        <v>1</v>
-      </c>
-      <c r="C134" s="0">
+      <c r="B134" s="1">
+        <v>1</v>
+      </c>
+      <c r="C134" s="1">
         <v>129.44590205794026</v>
       </c>
     </row>
@@ -1630,10 +1635,10 @@
       <c r="A135" t="s">
         <v>12</v>
       </c>
-      <c r="B135" s="0">
-        <v>2</v>
-      </c>
-      <c r="C135" s="0">
+      <c r="B135" s="1">
+        <v>2</v>
+      </c>
+      <c r="C135" s="1">
         <v>129.95284607940246</v>
       </c>
     </row>
@@ -1641,10 +1646,10 @@
       <c r="A136" t="s">
         <v>12</v>
       </c>
-      <c r="B136" s="0">
-        <v>3</v>
-      </c>
-      <c r="C136" s="0">
+      <c r="B136" s="1">
+        <v>3</v>
+      </c>
+      <c r="C136" s="1">
         <v>111.89680762313428</v>
       </c>
     </row>
@@ -1652,10 +1657,10 @@
       <c r="A137" t="s">
         <v>12</v>
       </c>
-      <c r="B137" s="0">
-        <v>4</v>
-      </c>
-      <c r="C137" s="0">
+      <c r="B137" s="1">
+        <v>4</v>
+      </c>
+      <c r="C137" s="1">
         <v>111.68908181978891</v>
       </c>
     </row>
@@ -1663,10 +1668,10 @@
       <c r="A138" t="s">
         <v>12</v>
       </c>
-      <c r="B138" s="0">
-        <v>5</v>
-      </c>
-      <c r="C138" s="0">
+      <c r="B138" s="1">
+        <v>5</v>
+      </c>
+      <c r="C138" s="1">
         <v>116.61089085999414</v>
       </c>
     </row>
@@ -1674,10 +1679,10 @@
       <c r="A139" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="0">
-        <v>6</v>
-      </c>
-      <c r="C139" s="0">
+      <c r="B139" s="1">
+        <v>6</v>
+      </c>
+      <c r="C139" s="1">
         <v>154.18635733037533</v>
       </c>
     </row>
@@ -1685,10 +1690,10 @@
       <c r="A140" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="0">
-        <v>7</v>
-      </c>
-      <c r="C140" s="0">
+      <c r="B140" s="1">
+        <v>7</v>
+      </c>
+      <c r="C140" s="1">
         <v>128.96145456031053</v>
       </c>
     </row>
@@ -1696,10 +1701,10 @@
       <c r="A141" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="0">
-        <v>8</v>
-      </c>
-      <c r="C141" s="0">
+      <c r="B141" s="1">
+        <v>8</v>
+      </c>
+      <c r="C141" s="1">
         <v>117.74832179758042</v>
       </c>
     </row>
@@ -1707,10 +1712,10 @@
       <c r="A142" t="s">
         <v>12</v>
       </c>
-      <c r="B142" s="0">
-        <v>9</v>
-      </c>
-      <c r="C142" s="0">
+      <c r="B142" s="1">
+        <v>9</v>
+      </c>
+      <c r="C142" s="1">
         <v>100.0763504077331</v>
       </c>
     </row>
@@ -1718,10 +1723,10 @@
       <c r="A143" t="s">
         <v>12</v>
       </c>
-      <c r="B143" s="0">
-        <v>10</v>
-      </c>
-      <c r="C143" s="0">
+      <c r="B143" s="1">
+        <v>10</v>
+      </c>
+      <c r="C143" s="1">
         <v>107.54240446531122</v>
       </c>
     </row>
@@ -1729,10 +1734,10 @@
       <c r="A144" t="s">
         <v>12</v>
       </c>
-      <c r="B144" s="0">
-        <v>11</v>
-      </c>
-      <c r="C144" s="0">
+      <c r="B144" s="1">
+        <v>11</v>
+      </c>
+      <c r="C144" s="1">
         <v>107.57200130311233</v>
       </c>
     </row>
@@ -1740,10 +1745,10 @@
       <c r="A145" t="s">
         <v>12</v>
       </c>
-      <c r="B145" s="0">
-        <v>12</v>
-      </c>
-      <c r="C145" s="0">
+      <c r="B145" s="1">
+        <v>12</v>
+      </c>
+      <c r="C145" s="1">
         <v>135.97782174570824</v>
       </c>
     </row>
@@ -1751,10 +1756,10 @@
       <c r="A146" t="s">
         <v>13</v>
       </c>
-      <c r="B146" s="0">
-        <v>1</v>
-      </c>
-      <c r="C146" s="0">
+      <c r="B146" s="1">
+        <v>1</v>
+      </c>
+      <c r="C146" s="1">
         <v>148.26556162676309</v>
       </c>
     </row>
@@ -1762,10 +1767,10 @@
       <c r="A147" t="s">
         <v>13</v>
       </c>
-      <c r="B147" s="0">
-        <v>2</v>
-      </c>
-      <c r="C147" s="0">
+      <c r="B147" s="1">
+        <v>2</v>
+      </c>
+      <c r="C147" s="1">
         <v>143.34239608678251</v>
       </c>
     </row>
@@ -1773,10 +1778,10 @@
       <c r="A148" t="s">
         <v>13</v>
       </c>
-      <c r="B148" s="0">
-        <v>3</v>
-      </c>
-      <c r="C148" s="0">
+      <c r="B148" s="1">
+        <v>3</v>
+      </c>
+      <c r="C148" s="1">
         <v>160.08868904162972</v>
       </c>
     </row>
@@ -1784,10 +1789,10 @@
       <c r="A149" t="s">
         <v>13</v>
       </c>
-      <c r="B149" s="0">
-        <v>4</v>
-      </c>
-      <c r="C149" s="0">
+      <c r="B149" s="1">
+        <v>4</v>
+      </c>
+      <c r="C149" s="1">
         <v>161.00445943010854</v>
       </c>
     </row>
@@ -1795,10 +1800,10 @@
       <c r="A150" t="s">
         <v>13</v>
       </c>
-      <c r="B150" s="0">
-        <v>5</v>
-      </c>
-      <c r="C150" s="0">
+      <c r="B150" s="1">
+        <v>5</v>
+      </c>
+      <c r="C150" s="1">
         <v>243.53857801491344</v>
       </c>
     </row>
@@ -1806,10 +1811,10 @@
       <c r="A151" t="s">
         <v>13</v>
       </c>
-      <c r="B151" s="0">
-        <v>6</v>
-      </c>
-      <c r="C151" s="0">
+      <c r="B151" s="1">
+        <v>6</v>
+      </c>
+      <c r="C151" s="1">
         <v>184.0182788836257</v>
       </c>
     </row>
@@ -1817,10 +1822,10 @@
       <c r="A152" t="s">
         <v>13</v>
       </c>
-      <c r="B152" s="0">
-        <v>7</v>
-      </c>
-      <c r="C152" s="0">
+      <c r="B152" s="1">
+        <v>7</v>
+      </c>
+      <c r="C152" s="1">
         <v>142.86163286041818</v>
       </c>
     </row>
@@ -1828,10 +1833,10 @@
       <c r="A153" t="s">
         <v>13</v>
       </c>
-      <c r="B153" s="0">
-        <v>8</v>
-      </c>
-      <c r="C153" s="0">
+      <c r="B153" s="1">
+        <v>8</v>
+      </c>
+      <c r="C153" s="1">
         <v>165.98422462934116</v>
       </c>
     </row>
@@ -1839,10 +1844,10 @@
       <c r="A154" t="s">
         <v>13</v>
       </c>
-      <c r="B154" s="0">
-        <v>9</v>
-      </c>
-      <c r="C154" s="0">
+      <c r="B154" s="1">
+        <v>9</v>
+      </c>
+      <c r="C154" s="1">
         <v>127.90262125152725</v>
       </c>
     </row>
@@ -1850,10 +1855,10 @@
       <c r="A155" t="s">
         <v>13</v>
       </c>
-      <c r="B155" s="0">
-        <v>10</v>
-      </c>
-      <c r="C155" s="0">
+      <c r="B155" s="1">
+        <v>10</v>
+      </c>
+      <c r="C155" s="1">
         <v>177.80286471621724</v>
       </c>
     </row>
@@ -1861,10 +1866,10 @@
       <c r="A156" t="s">
         <v>13</v>
       </c>
-      <c r="B156" s="0">
-        <v>11</v>
-      </c>
-      <c r="C156" s="0">
+      <c r="B156" s="1">
+        <v>11</v>
+      </c>
+      <c r="C156" s="1">
         <v>153.24843338306422</v>
       </c>
     </row>
@@ -1872,10 +1877,10 @@
       <c r="A157" t="s">
         <v>13</v>
       </c>
-      <c r="B157" s="0">
-        <v>12</v>
-      </c>
-      <c r="C157" s="0">
+      <c r="B157" s="1">
+        <v>12</v>
+      </c>
+      <c r="C157" s="1">
         <v>122.77899240938301</v>
       </c>
     </row>
@@ -1883,10 +1888,10 @@
       <c r="A158" t="s">
         <v>14</v>
       </c>
-      <c r="B158" s="0">
-        <v>1</v>
-      </c>
-      <c r="C158" s="0">
+      <c r="B158" s="1">
+        <v>1</v>
+      </c>
+      <c r="C158" s="1">
         <v>123.680147938887</v>
       </c>
     </row>
@@ -1894,10 +1899,10 @@
       <c r="A159" t="s">
         <v>14</v>
       </c>
-      <c r="B159" s="0">
-        <v>2</v>
-      </c>
-      <c r="C159" s="0">
+      <c r="B159" s="1">
+        <v>2</v>
+      </c>
+      <c r="C159" s="1">
         <v>119.12127850168046</v>
       </c>
     </row>
@@ -1905,10 +1910,10 @@
       <c r="A160" t="s">
         <v>14</v>
       </c>
-      <c r="B160" s="0">
-        <v>3</v>
-      </c>
-      <c r="C160" s="0">
+      <c r="B160" s="1">
+        <v>3</v>
+      </c>
+      <c r="C160" s="1">
         <v>131.42253843387149</v>
       </c>
     </row>
@@ -1916,10 +1921,10 @@
       <c r="A161" t="s">
         <v>14</v>
       </c>
-      <c r="B161" s="0">
-        <v>4</v>
-      </c>
-      <c r="C161" s="0">
+      <c r="B161" s="1">
+        <v>4</v>
+      </c>
+      <c r="C161" s="1">
         <v>97.93698999814309</v>
       </c>
     </row>
@@ -1927,10 +1932,10 @@
       <c r="A162" t="s">
         <v>14</v>
       </c>
-      <c r="B162" s="0">
-        <v>5</v>
-      </c>
-      <c r="C162" s="0">
+      <c r="B162" s="1">
+        <v>5</v>
+      </c>
+      <c r="C162" s="1">
         <v>94.244068778262516</v>
       </c>
     </row>
@@ -1938,10 +1943,10 @@
       <c r="A163" t="s">
         <v>14</v>
       </c>
-      <c r="B163" s="0">
-        <v>6</v>
-      </c>
-      <c r="C163" s="0">
+      <c r="B163" s="1">
+        <v>6</v>
+      </c>
+      <c r="C163" s="1">
         <v>122.6976663955935</v>
       </c>
     </row>
@@ -1949,10 +1954,10 @@
       <c r="A164" t="s">
         <v>14</v>
       </c>
-      <c r="B164" s="0">
-        <v>7</v>
-      </c>
-      <c r="C164" s="0">
+      <c r="B164" s="1">
+        <v>7</v>
+      </c>
+      <c r="C164" s="1">
         <v>149.02829406668391</v>
       </c>
     </row>
@@ -1960,10 +1965,10 @@
       <c r="A165" t="s">
         <v>14</v>
       </c>
-      <c r="B165" s="0">
-        <v>8</v>
-      </c>
-      <c r="C165" s="0">
+      <c r="B165" s="1">
+        <v>8</v>
+      </c>
+      <c r="C165" s="1">
         <v>177.75312265089235</v>
       </c>
     </row>
@@ -1971,10 +1976,10 @@
       <c r="A166" t="s">
         <v>14</v>
       </c>
-      <c r="B166" s="0">
-        <v>9</v>
-      </c>
-      <c r="C166" s="0">
+      <c r="B166" s="1">
+        <v>9</v>
+      </c>
+      <c r="C166" s="1">
         <v>153.32764352624784</v>
       </c>
     </row>
@@ -1982,10 +1987,10 @@
       <c r="A167" t="s">
         <v>14</v>
       </c>
-      <c r="B167" s="0">
-        <v>10</v>
-      </c>
-      <c r="C167" s="0">
+      <c r="B167" s="1">
+        <v>10</v>
+      </c>
+      <c r="C167" s="1">
         <v>149.69090675465347</v>
       </c>
     </row>
@@ -1993,10 +1998,10 @@
       <c r="A168" t="s">
         <v>14</v>
       </c>
-      <c r="B168" s="0">
-        <v>11</v>
-      </c>
-      <c r="C168" s="0">
+      <c r="B168" s="1">
+        <v>11</v>
+      </c>
+      <c r="C168" s="1">
         <v>209.89849346585174</v>
       </c>
     </row>
@@ -2004,10 +2009,10 @@
       <c r="A169" t="s">
         <v>14</v>
       </c>
-      <c r="B169" s="0">
-        <v>12</v>
-      </c>
-      <c r="C169" s="0">
+      <c r="B169" s="1">
+        <v>12</v>
+      </c>
+      <c r="C169" s="1">
         <v>140.62797929349495</v>
       </c>
     </row>
@@ -2015,10 +2020,10 @@
       <c r="A170" t="s">
         <v>15</v>
       </c>
-      <c r="B170" s="0">
-        <v>1</v>
-      </c>
-      <c r="C170" s="0">
+      <c r="B170" s="1">
+        <v>1</v>
+      </c>
+      <c r="C170" s="1">
         <v>137.26155402113505</v>
       </c>
     </row>
@@ -2026,10 +2031,10 @@
       <c r="A171" t="s">
         <v>15</v>
       </c>
-      <c r="B171" s="0">
-        <v>2</v>
-      </c>
-      <c r="C171" s="0">
+      <c r="B171" s="1">
+        <v>2</v>
+      </c>
+      <c r="C171" s="1">
         <v>132.0202282564008</v>
       </c>
     </row>
@@ -2037,10 +2042,10 @@
       <c r="A172" t="s">
         <v>15</v>
       </c>
-      <c r="B172" s="0">
-        <v>3</v>
-      </c>
-      <c r="C172" s="0">
+      <c r="B172" s="1">
+        <v>3</v>
+      </c>
+      <c r="C172" s="1">
         <v>103.72963719791315</v>
       </c>
     </row>
@@ -2048,10 +2053,10 @@
       <c r="A173" t="s">
         <v>15</v>
       </c>
-      <c r="B173" s="0">
-        <v>4</v>
-      </c>
-      <c r="C173" s="0">
+      <c r="B173" s="1">
+        <v>4</v>
+      </c>
+      <c r="C173" s="1">
         <v>109.31269219071331</v>
       </c>
     </row>
@@ -2059,10 +2064,10 @@
       <c r="A174" t="s">
         <v>15</v>
       </c>
-      <c r="B174" s="0">
-        <v>5</v>
-      </c>
-      <c r="C174" s="0">
+      <c r="B174" s="1">
+        <v>5</v>
+      </c>
+      <c r="C174" s="1">
         <v>151.78517880787442</v>
       </c>
     </row>
@@ -2070,10 +2075,10 @@
       <c r="A175" t="s">
         <v>15</v>
       </c>
-      <c r="B175" s="0">
-        <v>6</v>
-      </c>
-      <c r="C175" s="0">
+      <c r="B175" s="1">
+        <v>6</v>
+      </c>
+      <c r="C175" s="1">
         <v>169.64907552579561</v>
       </c>
     </row>
@@ -2081,10 +2086,10 @@
       <c r="A176" t="s">
         <v>15</v>
       </c>
-      <c r="B176" s="0">
-        <v>7</v>
-      </c>
-      <c r="C176" s="0">
+      <c r="B176" s="1">
+        <v>7</v>
+      </c>
+      <c r="C176" s="1">
         <v>129.98323050053759</v>
       </c>
     </row>
@@ -2092,10 +2097,10 @@
       <c r="A177" t="s">
         <v>15</v>
       </c>
-      <c r="B177" s="0">
-        <v>8</v>
-      </c>
-      <c r="C177" s="0">
+      <c r="B177" s="1">
+        <v>8</v>
+      </c>
+      <c r="C177" s="1">
         <v>98.178687632659731</v>
       </c>
     </row>
@@ -2103,10 +2108,10 @@
       <c r="A178" t="s">
         <v>15</v>
       </c>
-      <c r="B178" s="0">
-        <v>9</v>
-      </c>
-      <c r="C178" s="0">
+      <c r="B178" s="1">
+        <v>9</v>
+      </c>
+      <c r="C178" s="1">
         <v>124.43543264760135</v>
       </c>
     </row>
@@ -2114,10 +2119,10 @@
       <c r="A179" t="s">
         <v>15</v>
       </c>
-      <c r="B179" s="0">
-        <v>10</v>
-      </c>
-      <c r="C179" s="0">
+      <c r="B179" s="1">
+        <v>10</v>
+      </c>
+      <c r="C179" s="1">
         <v>153.99229062161274</v>
       </c>
     </row>
@@ -2125,10 +2130,10 @@
       <c r="A180" t="s">
         <v>15</v>
       </c>
-      <c r="B180" s="0">
-        <v>11</v>
-      </c>
-      <c r="C180" s="0">
+      <c r="B180" s="1">
+        <v>11</v>
+      </c>
+      <c r="C180" s="1">
         <v>162.1009636904767</v>
       </c>
     </row>
@@ -2136,10 +2141,10 @@
       <c r="A181" t="s">
         <v>15</v>
       </c>
-      <c r="B181" s="0">
-        <v>12</v>
-      </c>
-      <c r="C181" s="0">
+      <c r="B181" s="1">
+        <v>12</v>
+      </c>
+      <c r="C181" s="1">
         <v>140.64389927578668</v>
       </c>
     </row>
@@ -2147,10 +2152,10 @@
       <c r="A182" t="s">
         <v>16</v>
       </c>
-      <c r="B182" s="0">
-        <v>1</v>
-      </c>
-      <c r="C182" s="0">
+      <c r="B182" s="1">
+        <v>1</v>
+      </c>
+      <c r="C182" s="1">
         <v>187.77022088412104</v>
       </c>
     </row>
@@ -2158,10 +2163,10 @@
       <c r="A183" t="s">
         <v>16</v>
       </c>
-      <c r="B183" s="0">
-        <v>2</v>
-      </c>
-      <c r="C183" s="0">
+      <c r="B183" s="1">
+        <v>2</v>
+      </c>
+      <c r="C183" s="1">
         <v>97.381306471276645</v>
       </c>
     </row>
@@ -2169,10 +2174,10 @@
       <c r="A184" t="s">
         <v>16</v>
       </c>
-      <c r="B184" s="0">
-        <v>3</v>
-      </c>
-      <c r="C184" s="0">
+      <c r="B184" s="1">
+        <v>3</v>
+      </c>
+      <c r="C184" s="1">
         <v>108.96334469441564</v>
       </c>
     </row>
@@ -2180,10 +2185,10 @@
       <c r="A185" t="s">
         <v>16</v>
       </c>
-      <c r="B185" s="0">
-        <v>4</v>
-      </c>
-      <c r="C185" s="0">
+      <c r="B185" s="1">
+        <v>4</v>
+      </c>
+      <c r="C185" s="1">
         <v>101.40814734641286</v>
       </c>
     </row>
@@ -2191,10 +2196,10 @@
       <c r="A186" t="s">
         <v>16</v>
       </c>
-      <c r="B186" s="0">
-        <v>5</v>
-      </c>
-      <c r="C186" s="0">
+      <c r="B186" s="1">
+        <v>5</v>
+      </c>
+      <c r="C186" s="1">
         <v>72.982437440336582</v>
       </c>
     </row>
@@ -2202,10 +2207,10 @@
       <c r="A187" t="s">
         <v>16</v>
       </c>
-      <c r="B187" s="0">
-        <v>6</v>
-      </c>
-      <c r="C187" s="0">
+      <c r="B187" s="1">
+        <v>6</v>
+      </c>
+      <c r="C187" s="1">
         <v>90.508135573528975</v>
       </c>
     </row>
@@ -2213,10 +2218,10 @@
       <c r="A188" t="s">
         <v>16</v>
       </c>
-      <c r="B188" s="0">
-        <v>7</v>
-      </c>
-      <c r="C188" s="0">
+      <c r="B188" s="1">
+        <v>7</v>
+      </c>
+      <c r="C188" s="1">
         <v>68.187994849365296</v>
       </c>
     </row>
@@ -2224,10 +2229,10 @@
       <c r="A189" t="s">
         <v>16</v>
       </c>
-      <c r="B189" s="0">
-        <v>8</v>
-      </c>
-      <c r="C189" s="0">
+      <c r="B189" s="1">
+        <v>8</v>
+      </c>
+      <c r="C189" s="1">
         <v>91.647729301347653</v>
       </c>
     </row>
@@ -2235,10 +2240,10 @@
       <c r="A190" t="s">
         <v>16</v>
       </c>
-      <c r="B190" s="0">
-        <v>9</v>
-      </c>
-      <c r="C190" s="0">
+      <c r="B190" s="1">
+        <v>9</v>
+      </c>
+      <c r="C190" s="1">
         <v>94.262173923082898</v>
       </c>
     </row>
@@ -2246,10 +2251,10 @@
       <c r="A191" t="s">
         <v>16</v>
       </c>
-      <c r="B191" s="0">
-        <v>10</v>
-      </c>
-      <c r="C191" s="0">
+      <c r="B191" s="1">
+        <v>10</v>
+      </c>
+      <c r="C191" s="1">
         <v>110.99637349305908</v>
       </c>
     </row>
@@ -2257,10 +2262,10 @@
       <c r="A192" t="s">
         <v>16</v>
       </c>
-      <c r="B192" s="0">
-        <v>11</v>
-      </c>
-      <c r="C192" s="0">
+      <c r="B192" s="1">
+        <v>11</v>
+      </c>
+      <c r="C192" s="1">
         <v>82.074792420418262</v>
       </c>
     </row>
@@ -2268,10 +2273,10 @@
       <c r="A193" t="s">
         <v>16</v>
       </c>
-      <c r="B193" s="0">
-        <v>12</v>
-      </c>
-      <c r="C193" s="0">
+      <c r="B193" s="1">
+        <v>12</v>
+      </c>
+      <c r="C193" s="1">
         <v>89.423936228742434</v>
       </c>
     </row>
@@ -2279,10 +2284,10 @@
       <c r="A194" t="s">
         <v>17</v>
       </c>
-      <c r="B194" s="0">
-        <v>1</v>
-      </c>
-      <c r="C194" s="0">
+      <c r="B194" s="1">
+        <v>1</v>
+      </c>
+      <c r="C194" s="1">
         <v>103.99873345811896</v>
       </c>
     </row>
@@ -2290,10 +2295,10 @@
       <c r="A195" t="s">
         <v>17</v>
       </c>
-      <c r="B195" s="0">
-        <v>2</v>
-      </c>
-      <c r="C195" s="0">
+      <c r="B195" s="1">
+        <v>2</v>
+      </c>
+      <c r="C195" s="1">
         <v>117.69553222863824</v>
       </c>
     </row>
@@ -2301,10 +2306,10 @@
       <c r="A196" t="s">
         <v>17</v>
       </c>
-      <c r="B196" s="0">
-        <v>3</v>
-      </c>
-      <c r="C196" s="0">
+      <c r="B196" s="1">
+        <v>3</v>
+      </c>
+      <c r="C196" s="1">
         <v>111.0478958953252</v>
       </c>
     </row>
@@ -2312,10 +2317,10 @@
       <c r="A197" t="s">
         <v>17</v>
       </c>
-      <c r="B197" s="0">
-        <v>4</v>
-      </c>
-      <c r="C197" s="0">
+      <c r="B197" s="1">
+        <v>4</v>
+      </c>
+      <c r="C197" s="1">
         <v>71.1262323283146</v>
       </c>
     </row>
@@ -2323,10 +2328,10 @@
       <c r="A198" t="s">
         <v>17</v>
       </c>
-      <c r="B198" s="0">
-        <v>5</v>
-      </c>
-      <c r="C198" s="0">
+      <c r="B198" s="1">
+        <v>5</v>
+      </c>
+      <c r="C198" s="1">
         <v>90.164919466224845</v>
       </c>
     </row>
@@ -2334,10 +2339,10 @@
       <c r="A199" t="s">
         <v>17</v>
       </c>
-      <c r="B199" s="0">
-        <v>6</v>
-      </c>
-      <c r="C199" s="0">
+      <c r="B199" s="1">
+        <v>6</v>
+      </c>
+      <c r="C199" s="1">
         <v>68.777371135066772</v>
       </c>
     </row>
@@ -2345,10 +2350,10 @@
       <c r="A200" t="s">
         <v>17</v>
       </c>
-      <c r="B200" s="0">
-        <v>7</v>
-      </c>
-      <c r="C200" s="0">
+      <c r="B200" s="1">
+        <v>7</v>
+      </c>
+      <c r="C200" s="1">
         <v>62.335446437524098</v>
       </c>
     </row>
@@ -2356,10 +2361,10 @@
       <c r="A201" t="s">
         <v>17</v>
       </c>
-      <c r="B201" s="0">
-        <v>8</v>
-      </c>
-      <c r="C201" s="0">
+      <c r="B201" s="1">
+        <v>8</v>
+      </c>
+      <c r="C201" s="1">
         <v>132.4733321477305</v>
       </c>
     </row>
@@ -2367,10 +2372,10 @@
       <c r="A202" t="s">
         <v>17</v>
       </c>
-      <c r="B202" s="0">
-        <v>9</v>
-      </c>
-      <c r="C202" s="0">
+      <c r="B202" s="1">
+        <v>9</v>
+      </c>
+      <c r="C202" s="1">
         <v>176.28371206161788</v>
       </c>
     </row>
@@ -2378,10 +2383,10 @@
       <c r="A203" t="s">
         <v>17</v>
       </c>
-      <c r="B203" s="0">
-        <v>10</v>
-      </c>
-      <c r="C203" s="0">
+      <c r="B203" s="1">
+        <v>10</v>
+      </c>
+      <c r="C203" s="1">
         <v>95.969213403346714</v>
       </c>
     </row>
@@ -2389,10 +2394,10 @@
       <c r="A204" t="s">
         <v>17</v>
       </c>
-      <c r="B204" s="0">
-        <v>11</v>
-      </c>
-      <c r="C204" s="0">
+      <c r="B204" s="1">
+        <v>11</v>
+      </c>
+      <c r="C204" s="1">
         <v>86.566503465758885</v>
       </c>
     </row>
@@ -2400,10 +2405,10 @@
       <c r="A205" t="s">
         <v>17</v>
       </c>
-      <c r="B205" s="0">
-        <v>12</v>
-      </c>
-      <c r="C205" s="0">
+      <c r="B205" s="1">
+        <v>12</v>
+      </c>
+      <c r="C205" s="1">
         <v>121.59108669531599</v>
       </c>
     </row>
@@ -2411,10 +2416,10 @@
       <c r="A206" t="s">
         <v>18</v>
       </c>
-      <c r="B206" s="0">
-        <v>1</v>
-      </c>
-      <c r="C206" s="0">
+      <c r="B206" s="1">
+        <v>1</v>
+      </c>
+      <c r="C206" s="1">
         <v>135.73043577158847</v>
       </c>
     </row>
@@ -2422,10 +2427,10 @@
       <c r="A207" t="s">
         <v>18</v>
       </c>
-      <c r="B207" s="0">
-        <v>2</v>
-      </c>
-      <c r="C207" s="0">
+      <c r="B207" s="1">
+        <v>2</v>
+      </c>
+      <c r="C207" s="1">
         <v>119.08361999195742</v>
       </c>
     </row>
@@ -2433,10 +2438,10 @@
       <c r="A208" t="s">
         <v>18</v>
       </c>
-      <c r="B208" s="0">
-        <v>3</v>
-      </c>
-      <c r="C208" s="0">
+      <c r="B208" s="1">
+        <v>3</v>
+      </c>
+      <c r="C208" s="1">
         <v>131.49864754410734</v>
       </c>
     </row>
@@ -2444,10 +2449,10 @@
       <c r="A209" t="s">
         <v>18</v>
       </c>
-      <c r="B209" s="0">
-        <v>4</v>
-      </c>
-      <c r="C209" s="0">
+      <c r="B209" s="1">
+        <v>4</v>
+      </c>
+      <c r="C209" s="1">
         <v>170.47333251119781</v>
       </c>
     </row>
@@ -2455,10 +2460,10 @@
       <c r="A210" t="s">
         <v>18</v>
       </c>
-      <c r="B210" s="0">
-        <v>5</v>
-      </c>
-      <c r="C210" s="0">
+      <c r="B210" s="1">
+        <v>5</v>
+      </c>
+      <c r="C210" s="1">
         <v>140.91246000958591</v>
       </c>
     </row>
@@ -2466,10 +2471,10 @@
       <c r="A211" t="s">
         <v>18</v>
       </c>
-      <c r="B211" s="0">
-        <v>6</v>
-      </c>
-      <c r="C211" s="0">
+      <c r="B211" s="1">
+        <v>6</v>
+      </c>
+      <c r="C211" s="1">
         <v>148.8165613417035</v>
       </c>
     </row>
@@ -2477,10 +2482,10 @@
       <c r="A212" t="s">
         <v>18</v>
       </c>
-      <c r="B212" s="0">
-        <v>7</v>
-      </c>
-      <c r="C212" s="0">
+      <c r="B212" s="1">
+        <v>7</v>
+      </c>
+      <c r="C212" s="1">
         <v>136.10010571637537</v>
       </c>
     </row>
@@ -2488,10 +2493,10 @@
       <c r="A213" t="s">
         <v>18</v>
       </c>
-      <c r="B213" s="0">
-        <v>8</v>
-      </c>
-      <c r="C213" s="0">
+      <c r="B213" s="1">
+        <v>8</v>
+      </c>
+      <c r="C213" s="1">
         <v>86.143682706913722</v>
       </c>
     </row>
@@ -2499,10 +2504,10 @@
       <c r="A214" t="s">
         <v>18</v>
       </c>
-      <c r="B214" s="0">
-        <v>9</v>
-      </c>
-      <c r="C214" s="0">
+      <c r="B214" s="1">
+        <v>9</v>
+      </c>
+      <c r="C214" s="1">
         <v>135.07500553450706</v>
       </c>
     </row>
@@ -2510,10 +2515,10 @@
       <c r="A215" t="s">
         <v>18</v>
       </c>
-      <c r="B215" s="0">
-        <v>10</v>
-      </c>
-      <c r="C215" s="0">
+      <c r="B215" s="1">
+        <v>10</v>
+      </c>
+      <c r="C215" s="1">
         <v>89.914531399970812</v>
       </c>
     </row>
@@ -2521,10 +2526,10 @@
       <c r="A216" t="s">
         <v>18</v>
       </c>
-      <c r="B216" s="0">
-        <v>11</v>
-      </c>
-      <c r="C216" s="0">
+      <c r="B216" s="1">
+        <v>11</v>
+      </c>
+      <c r="C216" s="1">
         <v>120.86214520248797</v>
       </c>
     </row>
@@ -2532,10 +2537,10 @@
       <c r="A217" t="s">
         <v>18</v>
       </c>
-      <c r="B217" s="0">
-        <v>12</v>
-      </c>
-      <c r="C217" s="0">
+      <c r="B217" s="1">
+        <v>12</v>
+      </c>
+      <c r="C217" s="1">
         <v>82.872786626003631</v>
       </c>
     </row>
@@ -2543,10 +2548,10 @@
       <c r="A218" t="s">
         <v>19</v>
       </c>
-      <c r="B218" s="0">
-        <v>1</v>
-      </c>
-      <c r="C218" s="0">
+      <c r="B218" s="1">
+        <v>1</v>
+      </c>
+      <c r="C218" s="1">
         <v>135.63231704946662</v>
       </c>
     </row>
@@ -2554,10 +2559,10 @@
       <c r="A219" t="s">
         <v>19</v>
       </c>
-      <c r="B219" s="0">
-        <v>2</v>
-      </c>
-      <c r="C219" s="0">
+      <c r="B219" s="1">
+        <v>2</v>
+      </c>
+      <c r="C219" s="1">
         <v>190.81671473576529</v>
       </c>
     </row>
@@ -2565,10 +2570,10 @@
       <c r="A220" t="s">
         <v>19</v>
       </c>
-      <c r="B220" s="0">
-        <v>3</v>
-      </c>
-      <c r="C220" s="0">
+      <c r="B220" s="1">
+        <v>3</v>
+      </c>
+      <c r="C220" s="1">
         <v>290.92952088547389</v>
       </c>
     </row>
@@ -2576,10 +2581,10 @@
       <c r="A221" t="s">
         <v>19</v>
       </c>
-      <c r="B221" s="0">
-        <v>4</v>
-      </c>
-      <c r="C221" s="0">
+      <c r="B221" s="1">
+        <v>4</v>
+      </c>
+      <c r="C221" s="1">
         <v>197.17079811515333</v>
       </c>
     </row>
@@ -2587,10 +2592,10 @@
       <c r="A222" t="s">
         <v>19</v>
       </c>
-      <c r="B222" s="0">
-        <v>5</v>
-      </c>
-      <c r="C222" s="0">
+      <c r="B222" s="1">
+        <v>5</v>
+      </c>
+      <c r="C222" s="1">
         <v>246.75490878190044</v>
       </c>
     </row>
@@ -2598,10 +2603,10 @@
       <c r="A223" t="s">
         <v>19</v>
       </c>
-      <c r="B223" s="0">
-        <v>6</v>
-      </c>
-      <c r="C223" s="0">
+      <c r="B223" s="1">
+        <v>6</v>
+      </c>
+      <c r="C223" s="1">
         <v>503.94249242172845</v>
       </c>
     </row>
@@ -2609,10 +2614,10 @@
       <c r="A224" t="s">
         <v>19</v>
       </c>
-      <c r="B224" s="0">
-        <v>7</v>
-      </c>
-      <c r="C224" s="0">
+      <c r="B224" s="1">
+        <v>7</v>
+      </c>
+      <c r="C224" s="1">
         <v>558.22364201882272</v>
       </c>
     </row>
@@ -2620,10 +2625,10 @@
       <c r="A225" t="s">
         <v>19</v>
       </c>
-      <c r="B225" s="0">
-        <v>8</v>
-      </c>
-      <c r="C225" s="0">
+      <c r="B225" s="1">
+        <v>8</v>
+      </c>
+      <c r="C225" s="1">
         <v>311.36483202454485</v>
       </c>
     </row>
@@ -2631,10 +2636,10 @@
       <c r="A226" t="s">
         <v>19</v>
       </c>
-      <c r="B226" s="0">
-        <v>9</v>
-      </c>
-      <c r="C226" s="0">
+      <c r="B226" s="1">
+        <v>9</v>
+      </c>
+      <c r="C226" s="1">
         <v>209.63793843523842</v>
       </c>
     </row>
@@ -2642,10 +2647,10 @@
       <c r="A227" t="s">
         <v>19</v>
       </c>
-      <c r="B227" s="0">
-        <v>10</v>
-      </c>
-      <c r="C227" s="0">
+      <c r="B227" s="1">
+        <v>10</v>
+      </c>
+      <c r="C227" s="1">
         <v>270.02349186959714</v>
       </c>
     </row>
@@ -2653,10 +2658,10 @@
       <c r="A228" t="s">
         <v>19</v>
       </c>
-      <c r="B228" s="0">
-        <v>11</v>
-      </c>
-      <c r="C228" s="0">
+      <c r="B228" s="1">
+        <v>11</v>
+      </c>
+      <c r="C228" s="1">
         <v>358.82840880746664</v>
       </c>
     </row>
@@ -2664,10 +2669,10 @@
       <c r="A229" t="s">
         <v>19</v>
       </c>
-      <c r="B229" s="0">
-        <v>12</v>
-      </c>
-      <c r="C229" s="0">
+      <c r="B229" s="1">
+        <v>12</v>
+      </c>
+      <c r="C229" s="1">
         <v>196.34369416706684</v>
       </c>
     </row>
@@ -2675,10 +2680,10 @@
       <c r="A230" t="s">
         <v>20</v>
       </c>
-      <c r="B230" s="0">
-        <v>1</v>
-      </c>
-      <c r="C230" s="0">
+      <c r="B230" s="1">
+        <v>1</v>
+      </c>
+      <c r="C230" s="1">
         <v>257.84839749321475</v>
       </c>
     </row>
@@ -2686,10 +2691,10 @@
       <c r="A231" t="s">
         <v>20</v>
       </c>
-      <c r="B231" s="0">
-        <v>2</v>
-      </c>
-      <c r="C231" s="0">
+      <c r="B231" s="1">
+        <v>2</v>
+      </c>
+      <c r="C231" s="1">
         <v>194.04470490308728</v>
       </c>
     </row>
@@ -2697,10 +2702,10 @@
       <c r="A232" t="s">
         <v>20</v>
       </c>
-      <c r="B232" s="0">
-        <v>3</v>
-      </c>
-      <c r="C232" s="0">
+      <c r="B232" s="1">
+        <v>3</v>
+      </c>
+      <c r="C232" s="1">
         <v>232.45972604144899</v>
       </c>
     </row>
@@ -2708,10 +2713,10 @@
       <c r="A233" t="s">
         <v>20</v>
       </c>
-      <c r="B233" s="0">
-        <v>4</v>
-      </c>
-      <c r="C233" s="0">
+      <c r="B233" s="1">
+        <v>4</v>
+      </c>
+      <c r="C233" s="1">
         <v>169.17603591482319</v>
       </c>
     </row>
@@ -2719,10 +2724,10 @@
       <c r="A234" t="s">
         <v>20</v>
       </c>
-      <c r="B234" s="0">
-        <v>5</v>
-      </c>
-      <c r="C234" s="0">
+      <c r="B234" s="1">
+        <v>5</v>
+      </c>
+      <c r="C234" s="1">
         <v>159.40144524851632</v>
       </c>
     </row>
@@ -2730,10 +2735,10 @@
       <c r="A235" t="s">
         <v>20</v>
       </c>
-      <c r="B235" s="0">
-        <v>6</v>
-      </c>
-      <c r="C235" s="0">
+      <c r="B235" s="1">
+        <v>6</v>
+      </c>
+      <c r="C235" s="1">
         <v>318.99116026199204</v>
       </c>
     </row>
@@ -2741,10 +2746,10 @@
       <c r="A236" t="s">
         <v>20</v>
       </c>
-      <c r="B236" s="0">
-        <v>7</v>
-      </c>
-      <c r="C236" s="0">
+      <c r="B236" s="1">
+        <v>7</v>
+      </c>
+      <c r="C236" s="1">
         <v>183.65895058106582</v>
       </c>
     </row>
@@ -2752,10 +2757,10 @@
       <c r="A237" t="s">
         <v>20</v>
       </c>
-      <c r="B237" s="0">
-        <v>8</v>
-      </c>
-      <c r="C237" s="0">
+      <c r="B237" s="1">
+        <v>8</v>
+      </c>
+      <c r="C237" s="1">
         <v>151.20429781015469</v>
       </c>
     </row>
@@ -2763,10 +2768,10 @@
       <c r="A238" t="s">
         <v>20</v>
       </c>
-      <c r="B238" s="0">
-        <v>9</v>
-      </c>
-      <c r="C238" s="0">
+      <c r="B238" s="1">
+        <v>9</v>
+      </c>
+      <c r="C238" s="1">
         <v>140.77881633904866</v>
       </c>
     </row>
@@ -2774,10 +2779,10 @@
       <c r="A239" t="s">
         <v>20</v>
       </c>
-      <c r="B239" s="0">
-        <v>10</v>
-      </c>
-      <c r="C239" s="0">
+      <c r="B239" s="1">
+        <v>10</v>
+      </c>
+      <c r="C239" s="1">
         <v>184.03005097183708</v>
       </c>
     </row>
@@ -2785,10 +2790,10 @@
       <c r="A240" t="s">
         <v>20</v>
       </c>
-      <c r="B240" s="0">
-        <v>11</v>
-      </c>
-      <c r="C240" s="0">
+      <c r="B240" s="1">
+        <v>11</v>
+      </c>
+      <c r="C240" s="1">
         <v>214.97008095639316</v>
       </c>
     </row>
@@ -2796,10 +2801,10 @@
       <c r="A241" t="s">
         <v>20</v>
       </c>
-      <c r="B241" s="0">
-        <v>12</v>
-      </c>
-      <c r="C241" s="0">
+      <c r="B241" s="1">
+        <v>12</v>
+      </c>
+      <c r="C241" s="1">
         <v>160.7223038718837</v>
       </c>
     </row>
@@ -2807,10 +2812,10 @@
       <c r="A242" t="s">
         <v>21</v>
       </c>
-      <c r="B242" s="0">
-        <v>1</v>
-      </c>
-      <c r="C242" s="0">
+      <c r="B242" s="1">
+        <v>1</v>
+      </c>
+      <c r="C242" s="1">
         <v>123.1599969116685</v>
       </c>
     </row>
@@ -2818,10 +2823,10 @@
       <c r="A243" t="s">
         <v>21</v>
       </c>
-      <c r="B243" s="0">
-        <v>2</v>
-      </c>
-      <c r="C243" s="0">
+      <c r="B243" s="1">
+        <v>2</v>
+      </c>
+      <c r="C243" s="1">
         <v>109.7487332483494</v>
       </c>
     </row>
@@ -2829,10 +2834,10 @@
       <c r="A244" t="s">
         <v>21</v>
       </c>
-      <c r="B244" s="0">
-        <v>3</v>
-      </c>
-      <c r="C244" s="0">
+      <c r="B244" s="1">
+        <v>3</v>
+      </c>
+      <c r="C244" s="1">
         <v>116.60540265498089</v>
       </c>
     </row>
@@ -2840,10 +2845,10 @@
       <c r="A245" t="s">
         <v>21</v>
       </c>
-      <c r="B245" s="0">
-        <v>4</v>
-      </c>
-      <c r="C245" s="0">
+      <c r="B245" s="1">
+        <v>4</v>
+      </c>
+      <c r="C245" s="1">
         <v>102.28703012879106</v>
       </c>
     </row>
@@ -2851,10 +2856,10 @@
       <c r="A246" t="s">
         <v>21</v>
       </c>
-      <c r="B246" s="0">
-        <v>5</v>
-      </c>
-      <c r="C246" s="0">
+      <c r="B246" s="1">
+        <v>5</v>
+      </c>
+      <c r="C246" s="1">
         <v>121.5436956067737</v>
       </c>
     </row>
@@ -2862,10 +2867,10 @@
       <c r="A247" t="s">
         <v>21</v>
       </c>
-      <c r="B247" s="0">
-        <v>6</v>
-      </c>
-      <c r="C247" s="0">
+      <c r="B247" s="1">
+        <v>6</v>
+      </c>
+      <c r="C247" s="1">
         <v>105.48676842316939</v>
       </c>
     </row>
@@ -2873,10 +2878,10 @@
       <c r="A248" t="s">
         <v>21</v>
       </c>
-      <c r="B248" s="0">
-        <v>7</v>
-      </c>
-      <c r="C248" s="0">
+      <c r="B248" s="1">
+        <v>7</v>
+      </c>
+      <c r="C248" s="1">
         <v>129.6226424998398</v>
       </c>
     </row>
@@ -2884,10 +2889,10 @@
       <c r="A249" t="s">
         <v>21</v>
       </c>
-      <c r="B249" s="0">
-        <v>8</v>
-      </c>
-      <c r="C249" s="0">
+      <c r="B249" s="1">
+        <v>8</v>
+      </c>
+      <c r="C249" s="1">
         <v>121.62974835667606</v>
       </c>
     </row>
@@ -2895,10 +2900,10 @@
       <c r="A250" t="s">
         <v>21</v>
       </c>
-      <c r="B250" s="0">
-        <v>9</v>
-      </c>
-      <c r="C250" s="0">
+      <c r="B250" s="1">
+        <v>9</v>
+      </c>
+      <c r="C250" s="1">
         <v>157.31582080050615</v>
       </c>
     </row>
@@ -2906,10 +2911,10 @@
       <c r="A251" t="s">
         <v>21</v>
       </c>
-      <c r="B251" s="0">
-        <v>10</v>
-      </c>
-      <c r="C251" s="0">
+      <c r="B251" s="1">
+        <v>10</v>
+      </c>
+      <c r="C251" s="1">
         <v>183.25266625551419</v>
       </c>
     </row>
@@ -2917,10 +2922,10 @@
       <c r="A252" t="s">
         <v>21</v>
       </c>
-      <c r="B252" s="0">
-        <v>11</v>
-      </c>
-      <c r="C252" s="0">
+      <c r="B252" s="1">
+        <v>11</v>
+      </c>
+      <c r="C252" s="1">
         <v>191.96645652769618</v>
       </c>
     </row>
@@ -2928,10 +2933,10 @@
       <c r="A253" t="s">
         <v>21</v>
       </c>
-      <c r="B253" s="0">
-        <v>12</v>
-      </c>
-      <c r="C253" s="0">
+      <c r="B253" s="1">
+        <v>12</v>
+      </c>
+      <c r="C253" s="1">
         <v>239.69102981938227</v>
       </c>
     </row>
@@ -2939,10 +2944,10 @@
       <c r="A254" t="s">
         <v>22</v>
       </c>
-      <c r="B254" s="0">
-        <v>1</v>
-      </c>
-      <c r="C254" s="0">
+      <c r="B254" s="1">
+        <v>1</v>
+      </c>
+      <c r="C254" s="1">
         <v>309.97244945797701</v>
       </c>
     </row>
@@ -2950,10 +2955,10 @@
       <c r="A255" t="s">
         <v>22</v>
       </c>
-      <c r="B255" s="0">
-        <v>2</v>
-      </c>
-      <c r="C255" s="0">
+      <c r="B255" s="1">
+        <v>2</v>
+      </c>
+      <c r="C255" s="1">
         <v>196.95946459830401</v>
       </c>
     </row>
@@ -2961,10 +2966,10 @@
       <c r="A256" t="s">
         <v>22</v>
       </c>
-      <c r="B256" s="0">
-        <v>3</v>
-      </c>
-      <c r="C256" s="0">
+      <c r="B256" s="1">
+        <v>3</v>
+      </c>
+      <c r="C256" s="1">
         <v>212.78254189044787</v>
       </c>
     </row>
@@ -2972,10 +2977,10 @@
       <c r="A257" t="s">
         <v>22</v>
       </c>
-      <c r="B257" s="0">
-        <v>4</v>
-      </c>
-      <c r="C257" s="0">
+      <c r="B257" s="1">
+        <v>4</v>
+      </c>
+      <c r="C257" s="1">
         <v>135.51848003853243</v>
       </c>
     </row>
@@ -2983,10 +2988,10 @@
       <c r="A258" t="s">
         <v>22</v>
       </c>
-      <c r="B258" s="0">
-        <v>5</v>
-      </c>
-      <c r="C258" s="0">
+      <c r="B258" s="1">
+        <v>5</v>
+      </c>
+      <c r="C258" s="1">
         <v>158.68260551719968</v>
       </c>
     </row>
@@ -2994,10 +2999,10 @@
       <c r="A259" t="s">
         <v>22</v>
       </c>
-      <c r="B259" s="0">
-        <v>6</v>
-      </c>
-      <c r="C259" s="0">
+      <c r="B259" s="1">
+        <v>6</v>
+      </c>
+      <c r="C259" s="1">
         <v>149.80560130108137</v>
       </c>
     </row>
@@ -3005,10 +3010,10 @@
       <c r="A260" t="s">
         <v>22</v>
       </c>
-      <c r="B260" s="0">
-        <v>7</v>
-      </c>
-      <c r="C260" s="0">
+      <c r="B260" s="1">
+        <v>7</v>
+      </c>
+      <c r="C260" s="1">
         <v>202.04377955585122</v>
       </c>
     </row>
@@ -3016,10 +3021,10 @@
       <c r="A261" t="s">
         <v>22</v>
       </c>
-      <c r="B261" s="0">
-        <v>8</v>
-      </c>
-      <c r="C261" s="0">
+      <c r="B261" s="1">
+        <v>8</v>
+      </c>
+      <c r="C261" s="1">
         <v>238.91571234839765</v>
       </c>
     </row>
@@ -3027,10 +3032,10 @@
       <c r="A262" t="s">
         <v>22</v>
       </c>
-      <c r="B262" s="0">
-        <v>9</v>
-      </c>
-      <c r="C262" s="0">
+      <c r="B262" s="1">
+        <v>9</v>
+      </c>
+      <c r="C262" s="1">
         <v>187.41011632363401</v>
       </c>
     </row>
@@ -3038,10 +3043,10 @@
       <c r="A263" t="s">
         <v>22</v>
       </c>
-      <c r="B263" s="0">
-        <v>10</v>
-      </c>
-      <c r="C263" s="0">
+      <c r="B263" s="1">
+        <v>10</v>
+      </c>
+      <c r="C263" s="1">
         <v>233.31156413860188</v>
       </c>
     </row>
@@ -3049,10 +3054,10 @@
       <c r="A264" t="s">
         <v>22</v>
       </c>
-      <c r="B264" s="0">
-        <v>11</v>
-      </c>
-      <c r="C264" s="0">
+      <c r="B264" s="1">
+        <v>11</v>
+      </c>
+      <c r="C264" s="1">
         <v>205.59707355365967</v>
       </c>
     </row>
@@ -3060,10 +3065,10 @@
       <c r="A265" t="s">
         <v>22</v>
       </c>
-      <c r="B265" s="0">
-        <v>12</v>
-      </c>
-      <c r="C265" s="0">
+      <c r="B265" s="1">
+        <v>12</v>
+      </c>
+      <c r="C265" s="1">
         <v>271.30406158523687</v>
       </c>
     </row>
@@ -3071,10 +3076,10 @@
       <c r="A266" t="s">
         <v>23</v>
       </c>
-      <c r="B266" s="0">
-        <v>1</v>
-      </c>
-      <c r="C266" s="0">
+      <c r="B266" s="1">
+        <v>1</v>
+      </c>
+      <c r="C266" s="1">
         <v>198.15649141819117</v>
       </c>
     </row>
@@ -3082,10 +3087,10 @@
       <c r="A267" t="s">
         <v>23</v>
       </c>
-      <c r="B267" s="0">
-        <v>2</v>
-      </c>
-      <c r="C267" s="0">
+      <c r="B267" s="1">
+        <v>2</v>
+      </c>
+      <c r="C267" s="1">
         <v>139.62192204074458</v>
       </c>
     </row>
@@ -3093,10 +3098,10 @@
       <c r="A268" t="s">
         <v>23</v>
       </c>
-      <c r="B268" s="0">
-        <v>3</v>
-      </c>
-      <c r="C268" s="0">
+      <c r="B268" s="1">
+        <v>3</v>
+      </c>
+      <c r="C268" s="1">
         <v>281.20727140397986</v>
       </c>
     </row>
@@ -3104,10 +3109,10 @@
       <c r="A269" t="s">
         <v>23</v>
       </c>
-      <c r="B269" s="0">
-        <v>4</v>
-      </c>
-      <c r="C269" s="0">
+      <c r="B269" s="1">
+        <v>4</v>
+      </c>
+      <c r="C269" s="1">
         <v>185.35208283420195</v>
       </c>
     </row>
@@ -3115,10 +3120,10 @@
       <c r="A270" t="s">
         <v>23</v>
       </c>
-      <c r="B270" s="0">
-        <v>5</v>
-      </c>
-      <c r="C270" s="0">
+      <c r="B270" s="1">
+        <v>5</v>
+      </c>
+      <c r="C270" s="1">
         <v>230.75636037309954</v>
       </c>
     </row>
@@ -3126,10 +3131,10 @@
       <c r="A271" t="s">
         <v>23</v>
       </c>
-      <c r="B271" s="0">
-        <v>6</v>
-      </c>
-      <c r="C271" s="0">
+      <c r="B271" s="1">
+        <v>6</v>
+      </c>
+      <c r="C271" s="1">
         <v>167.69786380940585</v>
       </c>
     </row>
@@ -3137,10 +3142,10 @@
       <c r="A272" t="s">
         <v>23</v>
       </c>
-      <c r="B272" s="0">
-        <v>7</v>
-      </c>
-      <c r="C272" s="0">
+      <c r="B272" s="1">
+        <v>7</v>
+      </c>
+      <c r="C272" s="1">
         <v>189.96193934251556</v>
       </c>
     </row>
@@ -3148,10 +3153,10 @@
       <c r="A273" t="s">
         <v>23</v>
       </c>
-      <c r="B273" s="0">
-        <v>8</v>
-      </c>
-      <c r="C273" s="0">
+      <c r="B273" s="1">
+        <v>8</v>
+      </c>
+      <c r="C273" s="1">
         <v>176.54884283733892</v>
       </c>
     </row>
@@ -3159,10 +3164,10 @@
       <c r="A274" t="s">
         <v>23</v>
       </c>
-      <c r="B274" s="0">
-        <v>9</v>
-      </c>
-      <c r="C274" s="0">
+      <c r="B274" s="1">
+        <v>9</v>
+      </c>
+      <c r="C274" s="1">
         <v>184.51675172929453</v>
       </c>
     </row>
@@ -3170,10 +3175,10 @@
       <c r="A275" t="s">
         <v>23</v>
       </c>
-      <c r="B275" s="0">
-        <v>10</v>
-      </c>
-      <c r="C275" s="0">
+      <c r="B275" s="1">
+        <v>10</v>
+      </c>
+      <c r="C275" s="1">
         <v>189.1247735854013</v>
       </c>
     </row>
@@ -3181,10 +3186,10 @@
       <c r="A276" t="s">
         <v>23</v>
       </c>
-      <c r="B276" s="0">
-        <v>11</v>
-      </c>
-      <c r="C276" s="0">
+      <c r="B276" s="1">
+        <v>11</v>
+      </c>
+      <c r="C276" s="1">
         <v>214.46165401121681</v>
       </c>
     </row>
@@ -3192,10 +3197,10 @@
       <c r="A277" t="s">
         <v>23</v>
       </c>
-      <c r="B277" s="0">
-        <v>12</v>
-      </c>
-      <c r="C277" s="0">
+      <c r="B277" s="1">
+        <v>12</v>
+      </c>
+      <c r="C277" s="1">
         <v>207.60650804572748</v>
       </c>
     </row>
@@ -3203,10 +3208,10 @@
       <c r="A278" t="s">
         <v>24</v>
       </c>
-      <c r="B278" s="0">
-        <v>1</v>
-      </c>
-      <c r="C278" s="0">
+      <c r="B278" s="1">
+        <v>1</v>
+      </c>
+      <c r="C278" s="1">
         <v>112.63905727443453</v>
       </c>
     </row>
@@ -3214,10 +3219,10 @@
       <c r="A279" t="s">
         <v>24</v>
       </c>
-      <c r="B279" s="0">
-        <v>2</v>
-      </c>
-      <c r="C279" s="0">
+      <c r="B279" s="1">
+        <v>2</v>
+      </c>
+      <c r="C279" s="1">
         <v>138.00994636357206</v>
       </c>
     </row>
@@ -3225,10 +3230,10 @@
       <c r="A280" t="s">
         <v>24</v>
       </c>
-      <c r="B280" s="0">
-        <v>3</v>
-      </c>
-      <c r="C280" s="0">
+      <c r="B280" s="1">
+        <v>3</v>
+      </c>
+      <c r="C280" s="1">
         <v>142.40594412833096</v>
       </c>
     </row>
@@ -3236,10 +3241,10 @@
       <c r="A281" t="s">
         <v>24</v>
       </c>
-      <c r="B281" s="0">
-        <v>4</v>
-      </c>
-      <c r="C281" s="0">
+      <c r="B281" s="1">
+        <v>4</v>
+      </c>
+      <c r="C281" s="1">
         <v>95.280677239972462</v>
       </c>
     </row>
@@ -3247,10 +3252,10 @@
       <c r="A282" t="s">
         <v>24</v>
       </c>
-      <c r="B282" s="0">
-        <v>5</v>
-      </c>
-      <c r="C282" s="0">
+      <c r="B282" s="1">
+        <v>5</v>
+      </c>
+      <c r="C282" s="1">
         <v>98.11193470584746</v>
       </c>
     </row>
@@ -3258,10 +3263,10 @@
       <c r="A283" t="s">
         <v>24</v>
       </c>
-      <c r="B283" s="0">
-        <v>6</v>
-      </c>
-      <c r="C283" s="0">
+      <c r="B283" s="1">
+        <v>6</v>
+      </c>
+      <c r="C283" s="1">
         <v>90.334937611228654</v>
       </c>
     </row>
@@ -3269,10 +3274,10 @@
       <c r="A284" t="s">
         <v>24</v>
       </c>
-      <c r="B284" s="0">
-        <v>7</v>
-      </c>
-      <c r="C284" s="0">
+      <c r="B284" s="1">
+        <v>7</v>
+      </c>
+      <c r="C284" s="1">
         <v>88.283767152168153</v>
       </c>
     </row>
@@ -3280,10 +3285,10 @@
       <c r="A285" t="s">
         <v>24</v>
       </c>
-      <c r="B285" s="0">
-        <v>8</v>
-      </c>
-      <c r="C285" s="0">
+      <c r="B285" s="1">
+        <v>8</v>
+      </c>
+      <c r="C285" s="1">
         <v>79.109103716265921</v>
       </c>
     </row>
@@ -3291,10 +3296,10 @@
       <c r="A286" t="s">
         <v>24</v>
       </c>
-      <c r="B286" s="0">
-        <v>9</v>
-      </c>
-      <c r="C286" s="0">
+      <c r="B286" s="1">
+        <v>9</v>
+      </c>
+      <c r="C286" s="1">
         <v>78.700928887261341</v>
       </c>
     </row>
@@ -3302,10 +3307,10 @@
       <c r="A287" t="s">
         <v>24</v>
       </c>
-      <c r="B287" s="0">
-        <v>10</v>
-      </c>
-      <c r="C287" s="0">
+      <c r="B287" s="1">
+        <v>10</v>
+      </c>
+      <c r="C287" s="1">
         <v>103.9897920730636</v>
       </c>
     </row>
@@ -3313,10 +3318,10 @@
       <c r="A288" t="s">
         <v>24</v>
       </c>
-      <c r="B288" s="0">
-        <v>11</v>
-      </c>
-      <c r="C288" s="0">
+      <c r="B288" s="1">
+        <v>11</v>
+      </c>
+      <c r="C288" s="1">
         <v>75.317495277532174</v>
       </c>
     </row>
@@ -3324,10 +3329,10 @@
       <c r="A289" t="s">
         <v>24</v>
       </c>
-      <c r="B289" s="0">
-        <v>12</v>
-      </c>
-      <c r="C289" s="0">
+      <c r="B289" s="1">
+        <v>12</v>
+      </c>
+      <c r="C289" s="1">
         <v>174.83133982207281</v>
       </c>
     </row>
@@ -3335,10 +3340,10 @@
       <c r="A290" t="s">
         <v>25</v>
       </c>
-      <c r="B290" s="0">
-        <v>1</v>
-      </c>
-      <c r="C290" s="0">
+      <c r="B290" s="1">
+        <v>1</v>
+      </c>
+      <c r="C290" s="1">
         <v>88.199173561725758</v>
       </c>
     </row>
@@ -3346,10 +3351,10 @@
       <c r="A291" t="s">
         <v>25</v>
       </c>
-      <c r="B291" s="0">
-        <v>2</v>
-      </c>
-      <c r="C291" s="0">
+      <c r="B291" s="1">
+        <v>2</v>
+      </c>
+      <c r="C291" s="1">
         <v>80.71515390083168</v>
       </c>
     </row>
@@ -3357,10 +3362,10 @@
       <c r="A292" t="s">
         <v>25</v>
       </c>
-      <c r="B292" s="0">
-        <v>3</v>
-      </c>
-      <c r="C292" s="0">
+      <c r="B292" s="1">
+        <v>3</v>
+      </c>
+      <c r="C292" s="1">
         <v>170.0450385906353</v>
       </c>
     </row>
@@ -3368,10 +3373,10 @@
       <c r="A293" t="s">
         <v>25</v>
       </c>
-      <c r="B293" s="0">
-        <v>4</v>
-      </c>
-      <c r="C293" s="0">
+      <c r="B293" s="1">
+        <v>4</v>
+      </c>
+      <c r="C293" s="1">
         <v>123.43514711846839</v>
       </c>
     </row>
@@ -3379,10 +3384,10 @@
       <c r="A294" t="s">
         <v>25</v>
       </c>
-      <c r="B294" s="0">
-        <v>5</v>
-      </c>
-      <c r="C294" s="0">
+      <c r="B294" s="1">
+        <v>5</v>
+      </c>
+      <c r="C294" s="1">
         <v>105.19512401227369</v>
       </c>
     </row>
@@ -3390,10 +3395,10 @@
       <c r="A295" t="s">
         <v>25</v>
       </c>
-      <c r="B295" s="0">
-        <v>6</v>
-      </c>
-      <c r="C295" s="0">
+      <c r="B295" s="1">
+        <v>6</v>
+      </c>
+      <c r="C295" s="1">
         <v>118.81205960472241</v>
       </c>
     </row>
@@ -3401,10 +3406,10 @@
       <c r="A296" t="s">
         <v>25</v>
       </c>
-      <c r="B296" s="0">
-        <v>7</v>
-      </c>
-      <c r="C296" s="0">
+      <c r="B296" s="1">
+        <v>7</v>
+      </c>
+      <c r="C296" s="1">
         <v>184.27249051796957</v>
       </c>
     </row>
@@ -3412,10 +3417,10 @@
       <c r="A297" t="s">
         <v>25</v>
       </c>
-      <c r="B297" s="0">
-        <v>8</v>
-      </c>
-      <c r="C297" s="0">
+      <c r="B297" s="1">
+        <v>8</v>
+      </c>
+      <c r="C297" s="1">
         <v>124.28907856525075</v>
       </c>
     </row>
@@ -3423,10 +3428,10 @@
       <c r="A298" t="s">
         <v>25</v>
       </c>
-      <c r="B298" s="0">
-        <v>9</v>
-      </c>
-      <c r="C298" s="0">
+      <c r="B298" s="1">
+        <v>9</v>
+      </c>
+      <c r="C298" s="1">
         <v>230.05940534595089</v>
       </c>
     </row>
@@ -3434,10 +3439,10 @@
       <c r="A299" t="s">
         <v>25</v>
       </c>
-      <c r="B299" s="0">
-        <v>10</v>
-      </c>
-      <c r="C299" s="0">
+      <c r="B299" s="1">
+        <v>10</v>
+      </c>
+      <c r="C299" s="1">
         <v>399.80611032798606</v>
       </c>
     </row>
@@ -3445,10 +3450,10 @@
       <c r="A300" t="s">
         <v>25</v>
       </c>
-      <c r="B300" s="0">
-        <v>11</v>
-      </c>
-      <c r="C300" s="0">
+      <c r="B300" s="1">
+        <v>11</v>
+      </c>
+      <c r="C300" s="1">
         <v>220.10555967592006</v>
       </c>
     </row>
@@ -3456,10 +3461,10 @@
       <c r="A301" t="s">
         <v>25</v>
       </c>
-      <c r="B301" s="0">
-        <v>12</v>
-      </c>
-      <c r="C301" s="0">
+      <c r="B301" s="1">
+        <v>12</v>
+      </c>
+      <c r="C301" s="1">
         <v>167.63100925224853</v>
       </c>
     </row>
@@ -3467,10 +3472,10 @@
       <c r="A302" t="s">
         <v>26</v>
       </c>
-      <c r="B302" s="0">
-        <v>1</v>
-      </c>
-      <c r="C302" s="0">
+      <c r="B302" s="1">
+        <v>1</v>
+      </c>
+      <c r="C302" s="1">
         <v>140.0670895461748</v>
       </c>
     </row>
@@ -3478,10 +3483,10 @@
       <c r="A303" t="s">
         <v>26</v>
       </c>
-      <c r="B303" s="0">
-        <v>2</v>
-      </c>
-      <c r="C303" s="0">
+      <c r="B303" s="1">
+        <v>2</v>
+      </c>
+      <c r="C303" s="1">
         <v>121.21055490453543</v>
       </c>
     </row>
@@ -3489,10 +3494,10 @@
       <c r="A304" t="s">
         <v>26</v>
       </c>
-      <c r="B304" s="0">
-        <v>3</v>
-      </c>
-      <c r="C304" s="0">
+      <c r="B304" s="1">
+        <v>3</v>
+      </c>
+      <c r="C304" s="1">
         <v>132.89491891792139</v>
       </c>
     </row>
@@ -3500,10 +3505,10 @@
       <c r="A305" t="s">
         <v>26</v>
       </c>
-      <c r="B305" s="0">
-        <v>4</v>
-      </c>
-      <c r="C305" s="0">
+      <c r="B305" s="1">
+        <v>4</v>
+      </c>
+      <c r="C305" s="1">
         <v>132.91662881882434</v>
       </c>
     </row>
@@ -3511,10 +3516,10 @@
       <c r="A306" t="s">
         <v>26</v>
       </c>
-      <c r="B306" s="0">
-        <v>5</v>
-      </c>
-      <c r="C306" s="0">
+      <c r="B306" s="1">
+        <v>5</v>
+      </c>
+      <c r="C306" s="1">
         <v>118.00192593722068</v>
       </c>
     </row>
@@ -3522,10 +3527,10 @@
       <c r="A307" t="s">
         <v>26</v>
       </c>
-      <c r="B307" s="0">
-        <v>6</v>
-      </c>
-      <c r="C307" s="0">
+      <c r="B307" s="1">
+        <v>6</v>
+      </c>
+      <c r="C307" s="1">
         <v>118.06162320279019</v>
       </c>
     </row>
@@ -3533,10 +3538,10 @@
       <c r="A308" t="s">
         <v>26</v>
       </c>
-      <c r="B308" s="0">
-        <v>7</v>
-      </c>
-      <c r="C308" s="0">
+      <c r="B308" s="1">
+        <v>7</v>
+      </c>
+      <c r="C308" s="1">
         <v>118.84758179507466</v>
       </c>
     </row>
@@ -3544,10 +3549,10 @@
       <c r="A309" t="s">
         <v>26</v>
       </c>
-      <c r="B309" s="0">
-        <v>8</v>
-      </c>
-      <c r="C309" s="0">
+      <c r="B309" s="1">
+        <v>8</v>
+      </c>
+      <c r="C309" s="1">
         <v>116.07590528763814</v>
       </c>
     </row>
@@ -3555,10 +3560,10 @@
       <c r="A310" t="s">
         <v>26</v>
       </c>
-      <c r="B310" s="0">
-        <v>9</v>
-      </c>
-      <c r="C310" s="0">
+      <c r="B310" s="1">
+        <v>9</v>
+      </c>
+      <c r="C310" s="1">
         <v>130.47644814461012</v>
       </c>
     </row>
@@ -3566,10 +3571,10 @@
       <c r="A311" t="s">
         <v>26</v>
       </c>
-      <c r="B311" s="0">
-        <v>10</v>
-      </c>
-      <c r="C311" s="0">
+      <c r="B311" s="1">
+        <v>10</v>
+      </c>
+      <c r="C311" s="1">
         <v>107.93382339762844</v>
       </c>
     </row>
@@ -3577,10 +3582,10 @@
       <c r="A312" t="s">
         <v>26</v>
       </c>
-      <c r="B312" s="0">
-        <v>11</v>
-      </c>
-      <c r="C312" s="0">
+      <c r="B312" s="1">
+        <v>11</v>
+      </c>
+      <c r="C312" s="1">
         <v>115.96201204487213</v>
       </c>
     </row>
@@ -3588,10 +3593,10 @@
       <c r="A313" t="s">
         <v>26</v>
       </c>
-      <c r="B313" s="0">
-        <v>12</v>
-      </c>
-      <c r="C313" s="0">
+      <c r="B313" s="1">
+        <v>12</v>
+      </c>
+      <c r="C313" s="1">
         <v>120.8711830857322</v>
       </c>
     </row>
@@ -3599,10 +3604,10 @@
       <c r="A314" t="s">
         <v>27</v>
       </c>
-      <c r="B314" s="0">
-        <v>1</v>
-      </c>
-      <c r="C314" s="0">
+      <c r="B314" s="1">
+        <v>1</v>
+      </c>
+      <c r="C314" s="1">
         <v>100.6534474406542</v>
       </c>
     </row>
@@ -3610,10 +3615,10 @@
       <c r="A315" t="s">
         <v>27</v>
       </c>
-      <c r="B315" s="0">
-        <v>2</v>
-      </c>
-      <c r="C315" s="0">
+      <c r="B315" s="1">
+        <v>2</v>
+      </c>
+      <c r="C315" s="1">
         <v>114.04066891783862</v>
       </c>
     </row>
@@ -3621,10 +3626,10 @@
       <c r="A316" t="s">
         <v>27</v>
       </c>
-      <c r="B316" s="0">
-        <v>3</v>
-      </c>
-      <c r="C316" s="0">
+      <c r="B316" s="1">
+        <v>3</v>
+      </c>
+      <c r="C316" s="1">
         <v>135.56394811247927</v>
       </c>
     </row>
@@ -3632,10 +3637,10 @@
       <c r="A317" t="s">
         <v>27</v>
       </c>
-      <c r="B317" s="0">
-        <v>4</v>
-      </c>
-      <c r="C317" s="0">
+      <c r="B317" s="1">
+        <v>4</v>
+      </c>
+      <c r="C317" s="1">
         <v>102.66584709712725</v>
       </c>
     </row>
@@ -3643,10 +3648,10 @@
       <c r="A318" t="s">
         <v>27</v>
       </c>
-      <c r="B318" s="0">
-        <v>5</v>
-      </c>
-      <c r="C318" s="0">
+      <c r="B318" s="1">
+        <v>5</v>
+      </c>
+      <c r="C318" s="1">
         <v>144.78328886819094</v>
       </c>
     </row>
@@ -3654,10 +3659,10 @@
       <c r="A319" t="s">
         <v>27</v>
       </c>
-      <c r="B319" s="0">
-        <v>6</v>
-      </c>
-      <c r="C319" s="0">
+      <c r="B319" s="1">
+        <v>6</v>
+      </c>
+      <c r="C319" s="1">
         <v>146.59757407655673</v>
       </c>
     </row>
@@ -3665,10 +3670,10 @@
       <c r="A320" t="s">
         <v>27</v>
       </c>
-      <c r="B320" s="0">
-        <v>7</v>
-      </c>
-      <c r="C320" s="0">
+      <c r="B320" s="1">
+        <v>7</v>
+      </c>
+      <c r="C320" s="1">
         <v>183.28213802345289</v>
       </c>
     </row>
@@ -3676,10 +3681,10 @@
       <c r="A321" t="s">
         <v>27</v>
       </c>
-      <c r="B321" s="0">
-        <v>8</v>
-      </c>
-      <c r="C321" s="0">
+      <c r="B321" s="1">
+        <v>8</v>
+      </c>
+      <c r="C321" s="1">
         <v>116.87180249328715</v>
       </c>
     </row>
@@ -3687,10 +3692,10 @@
       <c r="A322" t="s">
         <v>27</v>
       </c>
-      <c r="B322" s="0">
-        <v>9</v>
-      </c>
-      <c r="C322" s="0">
+      <c r="B322" s="1">
+        <v>9</v>
+      </c>
+      <c r="C322" s="1">
         <v>184.40996223935207</v>
       </c>
     </row>
@@ -3698,10 +3703,10 @@
       <c r="A323" t="s">
         <v>27</v>
       </c>
-      <c r="B323" s="0">
-        <v>10</v>
-      </c>
-      <c r="C323" s="0">
+      <c r="B323" s="1">
+        <v>10</v>
+      </c>
+      <c r="C323" s="1">
         <v>273.85700012719877</v>
       </c>
     </row>
@@ -3709,10 +3714,10 @@
       <c r="A324" t="s">
         <v>27</v>
       </c>
-      <c r="B324" s="0">
-        <v>11</v>
-      </c>
-      <c r="C324" s="0">
+      <c r="B324" s="1">
+        <v>11</v>
+      </c>
+      <c r="C324" s="1">
         <v>327.23352118076377</v>
       </c>
     </row>
@@ -3720,19 +3725,52 @@
       <c r="A325" t="s">
         <v>27</v>
       </c>
-      <c r="B325" s="0">
-        <v>12</v>
-      </c>
-      <c r="C325" s="0">
-        <v>223.55022080880141</v>
+      <c r="B325" s="1">
+        <v>12</v>
+      </c>
+      <c r="C325" s="1">
+        <v>220.88985818828877</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="s">
         <v>28</v>
       </c>
-      <c r="B326" s="0"/>
-      <c r="C326" s="0"/>
+      <c r="B326" s="1">
+        <v>1</v>
+      </c>
+      <c r="C326" s="1">
+        <v>238.0605201956827</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>28</v>
+      </c>
+      <c r="B327" s="1">
+        <v>2</v>
+      </c>
+      <c r="C327" s="1">
+        <v>218.64806853848614</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>28</v>
+      </c>
+      <c r="B328" s="1">
+        <v>3</v>
+      </c>
+      <c r="C328" s="1">
+        <v>472.94710322622365</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s">
+        <v>29</v>
+      </c>
+      <c r="B329" s="1"/>
+      <c r="C329" s="1"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>